<commit_message>
some updates to literature search
</commit_message>
<xml_diff>
--- a/Literature_search/database.xlsx
+++ b/Literature_search/database.xlsx
@@ -1,19 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin Vasilev\Dropbox\PhD\Noise\reading_sounds\Literature_search\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="987" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="987" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="WoS" sheetId="1" r:id="rId1"/>
     <sheet name="Scopus" sheetId="2" r:id="rId2"/>
     <sheet name="Google Scholar" sheetId="3" r:id="rId3"/>
-    <sheet name="In-text" sheetId="6" r:id="rId4"/>
-    <sheet name=" Step 2" sheetId="4" r:id="rId5"/>
-    <sheet name="Step 3 " sheetId="5" r:id="rId6"/>
-    <sheet name="Step 4" sheetId="8" r:id="rId7"/>
+    <sheet name="ProQuest Diss" sheetId="9" r:id="rId4"/>
+    <sheet name="Reviews" sheetId="10" r:id="rId5"/>
+    <sheet name="In-text" sheetId="6" r:id="rId6"/>
+    <sheet name=" Step 2" sheetId="4" r:id="rId7"/>
+    <sheet name="Step 3 " sheetId="5" r:id="rId8"/>
+    <sheet name="Step 4" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -22,10 +29,45 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
+    <author>Martin R. Vasilev</author>
+  </authors>
+  <commentList>
+    <comment ref="B19" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Martin R. Vasilev:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+full-text found
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
     <author>Martin,Vasilev</author>
   </authors>
   <commentList>
-    <comment ref="D276" authorId="0">
+    <comment ref="D276" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -53,13 +95,13 @@
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Martin R. Vasilev</author>
   </authors>
   <commentList>
-    <comment ref="B73" authorId="0">
+    <comment ref="B73" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -89,7 +131,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3163" uniqueCount="719">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3244" uniqueCount="752">
   <si>
     <t>Search words: background noise AND reading -&gt; returned 445 records</t>
   </si>
@@ -23729,6 +23771,606 @@
       </rPr>
       <t>(1), 72-92.</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t>Kasiri, F. (2015). The impact of non-lyrical Iranian traditional music on reading comprehension performance of Iranian EFL learners: The case of gender, attitude, and familiarity. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Procedia-Social and Behavioral Sciences</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>199</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, 157-162.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Cho, H. (2015). Is Background Music a Distraction or Facilitator?: An Investigation on the Influence of Background Music in L2 Writing.</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Multimedia-Assisted Language Learning</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>18</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(2), 37-58.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Penttinen, M., Huovinen, E., &amp; Ylitalo, A. K. (2015). Reading ahead: Adult music students’ eye movements in temporally controlled performances of a children’s song. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>International Journal of Music Education</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>33</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(1), 36-50.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Schwartzberg, E. T., &amp; Silverman, M. J. (2016). Effects of a music-based short story on short-and long-term reading comprehension of individuals with Autism Spectrum Disorder: A cluster randomized study. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>The Arts in Psychotherapy</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>48</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, 54-61.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Schäfer, T., &amp; Fachner, J. (2015). Listening to music reduces eye movements. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Attention, Perception, &amp; Psychophysics</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>77</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(2), 551-559.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Flaugnacco, E., Lopez, L., Terribili, C., Montico, M., Zoia, S., &amp; Schön, D. (2015). Music training increases phonological awareness and reading skills in developmental dyslexia: a randomized control trial. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>PloS one</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(9), e0138715.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Khaghaninejad, M. S., Motlagh, H. S., &amp; Chamacham, R. (2016). How does Mozart’s music affect the reading comprehension of Iranian EFL Learners of both genders?. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>International Journal of Humanities and Cultural Studies (IJHCS)​ ISSN 2356-5926</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, 488-499.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Fonseca-Mora, M. C., Jara-Jiménez, P., &amp; Gómez-Domínguez, M. (2015). Musical plus phonological input for young foreign language readers. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Frontiers in psychology</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, 286.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Ohlenforst, B., Souza, P. E., &amp; MacDonald, E. N. (2016). Exploring the Relationship Between Working Memory, Compressor Speed, and Background Noise Characteristics. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Ear and hearing</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>37</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(2), 137-143.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>White-Schwoch, T., Carr, K. W., Thompson, E. C., Anderson, S., Nicol, T., Bradlow, A. R., ... &amp; Kraus, N. (2015). Auditory processing in noise: a preschool biomarker for literacy. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>PLoS Biol</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>13</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(7), e1002196.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Brännström, K. J., Holm, L., Lyberg-Åhlander, V., Haake, M., Kastberg, T., &amp; Sahlén, B. (2015). Children's subjective ratings and opinions of typical and dysphonic voice after performing a language comprehension task in background noise. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Journal of Voice</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>29</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(5), 624-630.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Seabi, J., Cockcroft, K., Goldschagg, P., &amp; Greyling, M. (2015). A prospective follow-up study of the effects of chronic aircraft noise exposure on learners’ reading comprehension in South Africa. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Journal of Exposure Science and Environmental Epidemiology</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>25</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(1), 84-88.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Schlittmeier, S. J., Feil, A., Liebl, A., &amp; Hellbrück, J. (2015). The impact of road traffic noise on cognitive performance in attention-based tasks depends on noise level even within moderate-level ranges. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Noise and health</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>17</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(76), 148.</t>
+    </r>
+  </si>
+  <si>
+    <t>Dove, M. K. (2009). The relationship of rhythmic and melodic perception with background music distraction in college level students (Order No. 3358711). Available from ProQuest Dissertations and Theses A&amp;I: The Humanities and Social Sciences Collection. (304917640). Retrieved from http://search.proquest.com/docview/304917640?accountid=9679</t>
+  </si>
+  <si>
+    <t>Chou, P. (2007). The effects of background music on the reading performance of taiwanese ESL students (Order No. 3293448). Available from ProQuest Dissertations and Theses A&amp;I: The Humanities and Social Sciences Collection. (304857770). Retrieved from http://search.proquest.com/docview/304857770?accountid=9679</t>
+  </si>
+  <si>
+    <t>Barnes, M. P. (2002). Individual differences in undergraduate reading comprehension as a function of extraversion -introversion level and background music complexity (Order No. 3046285). Available from ProQuest Dissertations and Theses A&amp;I: The Sciences and Engineering Collection. (305612017). Retrieved from http://search.proquest.com/docview/305612017?accountid=9679</t>
+  </si>
+  <si>
+    <t>Dawson, D. (2003). Listening to music and increasing reading achievement scores in vocabulary and comprehension and total reading ability (Order No. 3116329). Available from ProQuest Dissertations and Theses A&amp;I: The Humanities and Social Sciences Collection. (305232542). Retrieved from http://search.proquest.com/docview/305232542?accountid=9679</t>
+  </si>
+  <si>
+    <t>Anderson, S. A. (2007). The effect of music on the reading comprehension of junior high school students (Order No. 3245966). Available from ProQuest Dissertations and Theses A&amp;I: The Humanities and Social Sciences Collection; ProQuest Dissertations and Theses A&amp;I: The Sciences and Engineering Collection. (304763070). Retrieved from http://search.proquest.com/docview/304763070?accountid=9679</t>
+  </si>
+  <si>
+    <t>Wiley-Khaaliq, R. (1990). A study of the effects of background music on reading comprehension of learning-disabled students (Order No. 9117442). Available from ProQuest Dissertations and Theses A&amp;I: The Humanities and Social Sciences Collection. (303886202). Retrieved from http://search.proquest.com/docview/303886202?accountid=9679</t>
+  </si>
+  <si>
+    <t>Humphrey, J. C. (2014). The effects of mozart's sonata in D major on fourth graders' reading scores (Order No. 3582789). Available from ProQuest Dissertations and Theses A&amp;I: The Humanities and Social Sciences Collection. (1609381703). Retrieved from http://search.proquest.com/docview/1609381703?accountid=9679</t>
+  </si>
+  <si>
+    <t>Oliver, M. D. (1996). The effect of background music on mood and reading comprehension performance of at-risk college freshmen (Order No. 9715893). Available from ProQuest Dissertations and Theses A&amp;I: The Humanities and Social Sciences Collection. (304280987). Retrieved from http://search.proquest.com/docview/304280987?accountid=9679</t>
+  </si>
+  <si>
+    <t>Leguizamon, D. F. (2010). A musical approach to reading fluency: An experimental study in first-grade classrooms (Order No. 3412250). Available from ProQuest Dissertations and Theses A&amp;I: The Humanities and Social Sciences Collection. (737505433). Retrieved from http://search.proquest.com/docview/737505433?accountid=9679</t>
+  </si>
+  <si>
+    <t>Walton, J. P. (2013). The effect of music on the reading achievement of grade 1 students (Order No. 3589782). Available from ProQuest Dissertations and Theses A&amp;I: The Humanities and Social Sciences Collection. (1430910109). Retrieved from http://search.proquest.com/docview/1430910109?accountid=9679</t>
+  </si>
+  <si>
+    <t>Rawls, R. E. (2012). The effects of music tempo on task performances of introverts and extraverts (Order No. 1532105). Available from ProQuest Dissertations and Theses A&amp;I: The Humanities and Social Sciences Collection; ProQuest Dissertations and Theses A&amp;I: The Sciences and Engineering Collection. (1284409282). Retrieved from http://search.proquest.com/docview/1284409282?accountid=9679</t>
+  </si>
+  <si>
+    <t>DEGREGORIS, C. N. (1986). READING COMPREHENSION AND THE INTERACTION OF INDIVIDUAL SOUND PREFERENCES AND VARIED AUDITORY DISTRACTIONS(Order No. 8629819). Available from ProQuest Dissertations and Theses A&amp;I: The Humanities and Social Sciences Collection. (303481481). Retrieved from http://search.proquest.com/docview/303481481?accountid=9679</t>
+  </si>
+  <si>
+    <t>FRANKLIN, J. L. (1976). THE EFFECTS OF ROCK MUSIC ON THE READING COMPREHENSION OF EIGHTH-GRADE STUDENTS (Order No. 7713085). Available from ProQuest Dissertations and Theses A&amp;I: The Humanities and Social Sciences Collection. (302814434). Retrieved from http://search.proquest.com/docview/302814434?accountid=9679</t>
+  </si>
+  <si>
+    <t>Green, M. S. (1984). Effects of background music and field dependence/independence on cognitive achievement of college students (Order No. DP29483). Available from ProQuest Dissertations and Theses A&amp;I: The Humanities and Social Sciences Collection. (1651954101). Retrieved from http://search.proquest.com/docview/1651954101?accountid=9679</t>
+  </si>
+  <si>
+    <t>Johnson, M. B. (1999). The effects of background classical music on junior high school students' academic performance (Order No. 9971836). Available from ProQuest Dissertations and Theses A&amp;I: The Humanities and Social Sciences Collection; ProQuest Dissertations and Theses A&amp;I: The Sciences and Engineering Collection. (304547219). Retrieved from http://search.proquest.com/docview/304547219?accountid=9679</t>
+  </si>
+  <si>
+    <t>Banbury, S. P. (1996). The disruption of office-related tasks by speech and office noise(Order No. U084841). Available from ProQuest Dissertations &amp; Theses: UK &amp; Ireland. (301516201). Retrieved from http://search.proquest.com/docview/301516201?accountid=9679</t>
+  </si>
+  <si>
+    <t>Holmes, H. (2015). The effects of background sound on communication: Speech intelligibility and reading (Order No. 10114658). Available from ProQuest Dissertations &amp; Theses: UK &amp; Ireland. (1792788702). Retrieved from http://search.proquest.com/docview/1792788702?accountid=9679</t>
+  </si>
+  <si>
+    <t>FLAUM, M. P. (1981). THE EFFECTS OF MUSIC AND NOISE UPON VERBAL AND VISUOSPATIAL TASK PERFORMANCE AMONG MALE COLLEGE STUDENTS (Order No. 8111544). Available from ProQuest Dissertations and Theses A&amp;I: The Sciences and Engineering Collection. (303152248). Retrieved from http://search.proquest.com/docview/303152248?accountid=9679</t>
+  </si>
+  <si>
+    <t>not reading, exclude at stage 3</t>
+  </si>
+  <si>
+    <t>Searched for any papers that I don't immediately recognise (I had already read all papers until 2015 at this point)</t>
   </si>
 </sst>
 </file>
@@ -24105,7 +24747,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -24184,6 +24826,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -24198,7 +24846,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -24380,9 +25028,6 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -24472,6 +25117,27 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -24814,7 +25480,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -24824,7 +25490,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C119"/>
   <sheetViews>
-    <sheetView topLeftCell="A106" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A112" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B120" sqref="B120"/>
     </sheetView>
   </sheetViews>
@@ -25418,7 +26084,7 @@
       <c r="A55" s="2">
         <v>52</v>
       </c>
-      <c r="B55" s="71" t="s">
+      <c r="B55" s="70" t="s">
         <v>294</v>
       </c>
       <c r="C55" s="13" t="s">
@@ -25594,7 +26260,7 @@
       <c r="A71" s="2">
         <v>68</v>
       </c>
-      <c r="B71" s="71" t="s">
+      <c r="B71" s="70" t="s">
         <v>310</v>
       </c>
       <c r="C71" s="13" t="s">
@@ -26067,7 +26733,7 @@
       <c r="A114" s="2">
         <v>111</v>
       </c>
-      <c r="B114" s="99" t="s">
+      <c r="B114" s="98" t="s">
         <v>707</v>
       </c>
       <c r="C114" s="13" t="s">
@@ -26078,7 +26744,7 @@
       <c r="A115" s="2">
         <v>112</v>
       </c>
-      <c r="B115" s="99" t="s">
+      <c r="B115" s="98" t="s">
         <v>618</v>
       </c>
       <c r="C115" s="13" t="s">
@@ -26089,7 +26755,7 @@
       <c r="A116" s="2">
         <v>113</v>
       </c>
-      <c r="B116" s="99" t="s">
+      <c r="B116" s="98" t="s">
         <v>708</v>
       </c>
       <c r="C116" s="13" t="s">
@@ -26100,7 +26766,7 @@
       <c r="A117" s="2">
         <v>114</v>
       </c>
-      <c r="B117" s="99" t="s">
+      <c r="B117" s="98" t="s">
         <v>709</v>
       </c>
       <c r="C117" s="13" t="s">
@@ -26111,7 +26777,7 @@
       <c r="A118" s="1">
         <v>115</v>
       </c>
-      <c r="B118" s="99" t="s">
+      <c r="B118" s="98" t="s">
         <v>710</v>
       </c>
       <c r="C118" s="13" t="s">
@@ -26119,7 +26785,7 @@
       </c>
     </row>
     <row r="119" spans="1:3" ht="39" x14ac:dyDescent="0.25">
-      <c r="B119" s="99" t="s">
+      <c r="B119" s="98" t="s">
         <v>708</v>
       </c>
       <c r="C119" s="13" t="s">
@@ -26136,7 +26802,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView topLeftCell="A91" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A96" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C102" sqref="C102"/>
     </sheetView>
   </sheetViews>
@@ -27214,7 +27880,7 @@
       </c>
     </row>
     <row r="99" spans="1:3" ht="39" x14ac:dyDescent="0.25">
-      <c r="B99" s="99" t="s">
+      <c r="B99" s="98" t="s">
         <v>708</v>
       </c>
       <c r="C99" s="13" t="s">
@@ -27222,7 +27888,7 @@
       </c>
     </row>
     <row r="100" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="B100" s="99" t="s">
+      <c r="B100" s="98" t="s">
         <v>618</v>
       </c>
       <c r="C100" s="13" t="s">
@@ -27230,7 +27896,7 @@
       </c>
     </row>
     <row r="101" spans="1:3" ht="39" x14ac:dyDescent="0.25">
-      <c r="B101" s="99" t="s">
+      <c r="B101" s="98" t="s">
         <v>708</v>
       </c>
       <c r="C101" s="13" t="s">
@@ -27248,10 +27914,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C150"/>
+  <dimension ref="A1:C170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D150" sqref="D150"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28812,7 +29478,10 @@
       </c>
     </row>
     <row r="143" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="B143" s="99" t="s">
+      <c r="A143" s="2">
+        <v>140</v>
+      </c>
+      <c r="B143" s="98" t="s">
         <v>711</v>
       </c>
       <c r="C143" s="13" t="s">
@@ -28820,59 +29489,300 @@
       </c>
     </row>
     <row r="144" spans="1:3" ht="39" x14ac:dyDescent="0.25">
-      <c r="B144" s="99" t="s">
+      <c r="A144" s="2">
+        <v>141</v>
+      </c>
+      <c r="B144" s="98" t="s">
         <v>712</v>
       </c>
       <c r="C144" s="13" t="s">
         <v>565</v>
       </c>
     </row>
-    <row r="145" spans="2:3" ht="39" x14ac:dyDescent="0.25">
-      <c r="B145" s="99" t="s">
+    <row r="145" spans="1:3" ht="39" x14ac:dyDescent="0.25">
+      <c r="A145" s="2">
+        <v>142</v>
+      </c>
+      <c r="B145" s="98" t="s">
         <v>713</v>
       </c>
       <c r="C145" s="13" t="s">
         <v>565</v>
       </c>
     </row>
-    <row r="146" spans="2:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="B146" s="99" t="s">
+    <row r="146" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A146" s="2">
+        <v>143</v>
+      </c>
+      <c r="B146" s="98" t="s">
         <v>714</v>
       </c>
       <c r="C146" s="13" t="s">
         <v>565</v>
       </c>
     </row>
-    <row r="147" spans="2:3" ht="51.75" x14ac:dyDescent="0.25">
-      <c r="B147" s="99" t="s">
+    <row r="147" spans="1:3" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A147" s="2">
+        <v>144</v>
+      </c>
+      <c r="B147" s="98" t="s">
         <v>715</v>
       </c>
       <c r="C147" s="13" t="s">
         <v>565</v>
       </c>
     </row>
-    <row r="148" spans="2:3" ht="39" x14ac:dyDescent="0.25">
-      <c r="B148" s="99" t="s">
+    <row r="148" spans="1:3" ht="39" x14ac:dyDescent="0.25">
+      <c r="A148" s="2">
+        <v>145</v>
+      </c>
+      <c r="B148" s="98" t="s">
         <v>716</v>
       </c>
       <c r="C148" s="13" t="s">
         <v>565</v>
       </c>
     </row>
-    <row r="149" spans="2:3" ht="51.75" x14ac:dyDescent="0.25">
-      <c r="B149" s="99" t="s">
+    <row r="149" spans="1:3" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A149" s="2">
+        <v>146</v>
+      </c>
+      <c r="B149" s="98" t="s">
         <v>717</v>
       </c>
       <c r="C149" s="13" t="s">
         <v>565</v>
       </c>
     </row>
-    <row r="150" spans="2:3" ht="51.75" x14ac:dyDescent="0.25">
-      <c r="B150" s="99" t="s">
+    <row r="150" spans="1:3" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A150" s="2">
+        <v>147</v>
+      </c>
+      <c r="B150" s="98" t="s">
         <v>718</v>
       </c>
       <c r="C150" s="13" t="s">
         <v>565</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A151" s="2">
+        <v>148</v>
+      </c>
+      <c r="B151" s="100" t="s">
+        <v>714</v>
+      </c>
+      <c r="C151" s="13" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" ht="39" x14ac:dyDescent="0.25">
+      <c r="A152" s="2">
+        <v>149</v>
+      </c>
+      <c r="B152" s="101" t="s">
+        <v>719</v>
+      </c>
+      <c r="C152" s="13" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" ht="39" x14ac:dyDescent="0.25">
+      <c r="A153" s="2">
+        <v>150</v>
+      </c>
+      <c r="B153" s="101" t="s">
+        <v>720</v>
+      </c>
+      <c r="C153" s="13" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" ht="39" x14ac:dyDescent="0.25">
+      <c r="A154" s="2">
+        <v>151</v>
+      </c>
+      <c r="B154" s="101" t="s">
+        <v>721</v>
+      </c>
+      <c r="C154" s="13" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" ht="39" x14ac:dyDescent="0.25">
+      <c r="A155" s="2">
+        <v>152</v>
+      </c>
+      <c r="B155" s="101" t="s">
+        <v>722</v>
+      </c>
+      <c r="C155" s="13" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A156" s="2">
+        <v>153</v>
+      </c>
+      <c r="B156" s="101" t="s">
+        <v>723</v>
+      </c>
+      <c r="C156" s="13" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" ht="39" x14ac:dyDescent="0.25">
+      <c r="A157" s="2">
+        <v>154</v>
+      </c>
+      <c r="B157" s="101" t="s">
+        <v>724</v>
+      </c>
+      <c r="C157" s="13" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A158" s="2">
+        <v>155</v>
+      </c>
+      <c r="B158" s="101" t="s">
+        <v>725</v>
+      </c>
+      <c r="C158" s="13" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" ht="39" x14ac:dyDescent="0.25">
+      <c r="A159" s="2">
+        <v>156</v>
+      </c>
+      <c r="B159" s="101" t="s">
+        <v>712</v>
+      </c>
+      <c r="C159" s="13" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" ht="39" x14ac:dyDescent="0.25">
+      <c r="A160" s="2">
+        <v>157</v>
+      </c>
+      <c r="B160" s="101" t="s">
+        <v>726</v>
+      </c>
+      <c r="C160" s="13" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" ht="39" x14ac:dyDescent="0.25">
+      <c r="A161" s="2">
+        <v>158</v>
+      </c>
+      <c r="B161" s="101" t="s">
+        <v>713</v>
+      </c>
+      <c r="C161" s="13" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" ht="39" x14ac:dyDescent="0.25">
+      <c r="A162" s="2">
+        <v>159</v>
+      </c>
+      <c r="B162" s="101" t="s">
+        <v>727</v>
+      </c>
+      <c r="C162" s="13" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" ht="39" x14ac:dyDescent="0.25">
+      <c r="A163" s="2">
+        <v>160</v>
+      </c>
+      <c r="B163" s="101" t="s">
+        <v>728</v>
+      </c>
+      <c r="C163" s="13" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A164" s="2">
+        <v>161</v>
+      </c>
+      <c r="B164" s="101" t="s">
+        <v>729</v>
+      </c>
+      <c r="C164" s="13" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A165" s="2">
+        <v>162</v>
+      </c>
+      <c r="B165" s="101" t="s">
+        <v>714</v>
+      </c>
+      <c r="C165" s="13" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A166" s="2">
+        <v>163</v>
+      </c>
+      <c r="B166" s="101" t="s">
+        <v>542</v>
+      </c>
+      <c r="C166" s="13" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" ht="39" x14ac:dyDescent="0.25">
+      <c r="A167" s="2">
+        <v>164</v>
+      </c>
+      <c r="B167" s="101" t="s">
+        <v>707</v>
+      </c>
+      <c r="C167" s="13" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A168" s="2">
+        <v>165</v>
+      </c>
+      <c r="B168" s="101" t="s">
+        <v>730</v>
+      </c>
+      <c r="C168" s="13" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" ht="39" x14ac:dyDescent="0.25">
+      <c r="A169" s="2">
+        <v>166</v>
+      </c>
+      <c r="B169" s="101" t="s">
+        <v>713</v>
+      </c>
+      <c r="C169" s="13" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" ht="39" x14ac:dyDescent="0.25">
+      <c r="A170" s="2">
+        <v>167</v>
+      </c>
+      <c r="B170" s="101" t="s">
+        <v>731</v>
+      </c>
+      <c r="C170" s="13" t="s">
+        <v>290</v>
       </c>
     </row>
   </sheetData>
@@ -28882,6 +29792,263 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D20"/>
+  <sheetViews>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="13"/>
+    <col min="2" max="2" width="127.7109375" style="40" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" style="13" customWidth="1"/>
+    <col min="4" max="4" width="28.7109375" style="40" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="105"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="104" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="104" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="104" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="13">
+        <v>1</v>
+      </c>
+      <c r="B3" s="103" t="s">
+        <v>732</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="13">
+        <v>2</v>
+      </c>
+      <c r="B4" s="102" t="s">
+        <v>733</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="13">
+        <v>3</v>
+      </c>
+      <c r="B5" s="102" t="s">
+        <v>734</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="13">
+        <v>4</v>
+      </c>
+      <c r="B6" s="102" t="s">
+        <v>735</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="13">
+        <v>5</v>
+      </c>
+      <c r="B7" s="102" t="s">
+        <v>736</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="13">
+        <v>6</v>
+      </c>
+      <c r="B8" s="102" t="s">
+        <v>737</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="13">
+        <v>7</v>
+      </c>
+      <c r="B9" s="102" t="s">
+        <v>738</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="13">
+        <v>8</v>
+      </c>
+      <c r="B10" s="102" t="s">
+        <v>739</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="13">
+        <v>9</v>
+      </c>
+      <c r="B11" s="102" t="s">
+        <v>740</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="13">
+        <v>10</v>
+      </c>
+      <c r="B12" s="102" t="s">
+        <v>741</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="13">
+        <v>11</v>
+      </c>
+      <c r="B13" s="102" t="s">
+        <v>742</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="13">
+        <v>12</v>
+      </c>
+      <c r="B14" s="102" t="s">
+        <v>743</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="13">
+        <v>13</v>
+      </c>
+      <c r="B15" s="102" t="s">
+        <v>744</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="13">
+        <v>14</v>
+      </c>
+      <c r="B16" s="102" t="s">
+        <v>745</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="13">
+        <v>15</v>
+      </c>
+      <c r="B17" s="102" t="s">
+        <v>746</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="13">
+        <v>16</v>
+      </c>
+      <c r="B18" s="102" t="s">
+        <v>747</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="13">
+        <v>17</v>
+      </c>
+      <c r="B19" s="102" t="s">
+        <v>748</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="13">
+        <v>18</v>
+      </c>
+      <c r="B20" s="102" t="s">
+        <v>749</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>290</v>
+      </c>
+      <c r="D20" s="40" t="s">
+        <v>750</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>751</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H69"/>
   <sheetViews>
@@ -28896,14 +30063,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="69"/>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
+      <c r="A1" s="99"/>
+      <c r="B1" s="99"/>
+      <c r="C1" s="99"/>
+      <c r="D1" s="99"/>
+      <c r="E1" s="99"/>
+      <c r="F1" s="99"/>
+      <c r="G1" s="99"/>
+      <c r="H1" s="99"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -29371,7 +30538,7 @@
       <c r="A45" s="22">
         <v>42</v>
       </c>
-      <c r="B45" s="72" t="s">
+      <c r="B45" s="71" t="s">
         <v>385</v>
       </c>
       <c r="C45" s="13" t="s">
@@ -29547,7 +30714,7 @@
       <c r="A61" s="22">
         <v>58</v>
       </c>
-      <c r="B61" s="73" t="s">
+      <c r="B61" s="72" t="s">
         <v>130</v>
       </c>
       <c r="C61" s="13" t="s">
@@ -29569,7 +30736,7 @@
       <c r="A63" s="22">
         <v>60</v>
       </c>
-      <c r="B63" s="73" t="s">
+      <c r="B63" s="72" t="s">
         <v>62</v>
       </c>
       <c r="C63" s="13" t="s">
@@ -29651,11 +30818,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E427"/>
   <sheetViews>
-    <sheetView topLeftCell="A410" workbookViewId="0">
+    <sheetView topLeftCell="A285" workbookViewId="0">
       <selection activeCell="C430" sqref="C430"/>
     </sheetView>
   </sheetViews>
@@ -31899,7 +33066,7 @@
       <c r="A167">
         <v>165</v>
       </c>
-      <c r="C167" s="74" t="s">
+      <c r="C167" s="73" t="s">
         <v>400</v>
       </c>
       <c r="D167" s="13" t="s">
@@ -31987,7 +33154,7 @@
       <c r="A175">
         <v>173</v>
       </c>
-      <c r="C175" s="75" t="s">
+      <c r="C175" s="74" t="s">
         <v>404</v>
       </c>
       <c r="D175" s="13" t="s">
@@ -32240,7 +33407,7 @@
       <c r="A198">
         <v>196</v>
       </c>
-      <c r="C198" s="75" t="s">
+      <c r="C198" s="74" t="s">
         <v>409</v>
       </c>
       <c r="D198" s="13" t="s">
@@ -32405,7 +33572,7 @@
       <c r="A213">
         <v>211</v>
       </c>
-      <c r="C213" s="76" t="s">
+      <c r="C213" s="75" t="s">
         <v>413</v>
       </c>
       <c r="D213" s="13" t="s">
@@ -32416,7 +33583,7 @@
       <c r="A214">
         <v>212</v>
       </c>
-      <c r="C214" s="72" t="s">
+      <c r="C214" s="71" t="s">
         <v>385</v>
       </c>
       <c r="D214" s="13" t="s">
@@ -32482,7 +33649,7 @@
       <c r="A220">
         <v>218</v>
       </c>
-      <c r="C220" s="74" t="s">
+      <c r="C220" s="73" t="s">
         <v>415</v>
       </c>
       <c r="D220" s="13" t="s">
@@ -32581,7 +33748,7 @@
       <c r="A229">
         <v>227</v>
       </c>
-      <c r="C229" s="74" t="s">
+      <c r="C229" s="73" t="s">
         <v>419</v>
       </c>
       <c r="D229" s="13" t="s">
@@ -32625,7 +33792,7 @@
       <c r="A233">
         <v>231</v>
       </c>
-      <c r="C233" s="74" t="s">
+      <c r="C233" s="73" t="s">
         <v>143</v>
       </c>
       <c r="D233" s="13" t="s">
@@ -32647,7 +33814,7 @@
       <c r="A235">
         <v>233</v>
       </c>
-      <c r="C235" s="77" t="s">
+      <c r="C235" s="76" t="s">
         <v>144</v>
       </c>
       <c r="D235" s="13" t="s">
@@ -32834,7 +34001,7 @@
       <c r="A252">
         <v>250</v>
       </c>
-      <c r="C252" s="74" t="s">
+      <c r="C252" s="73" t="s">
         <v>425</v>
       </c>
       <c r="D252" s="13" t="s">
@@ -32889,7 +34056,7 @@
       <c r="A257">
         <v>255</v>
       </c>
-      <c r="C257" s="74" t="s">
+      <c r="C257" s="73" t="s">
         <v>428</v>
       </c>
       <c r="D257" s="13" t="s">
@@ -32966,7 +34133,7 @@
       <c r="A264">
         <v>262</v>
       </c>
-      <c r="C264" s="77" t="s">
+      <c r="C264" s="76" t="s">
         <v>130</v>
       </c>
       <c r="D264" s="13" t="s">
@@ -32988,7 +34155,7 @@
       <c r="A266">
         <v>264</v>
       </c>
-      <c r="C266" s="78" t="s">
+      <c r="C266" s="77" t="s">
         <v>130</v>
       </c>
       <c r="D266" s="13" t="s">
@@ -32999,7 +34166,7 @@
       <c r="A267">
         <v>265</v>
       </c>
-      <c r="C267" s="71" t="s">
+      <c r="C267" s="70" t="s">
         <v>310</v>
       </c>
       <c r="D267" s="13" t="s">
@@ -33109,7 +34276,7 @@
       <c r="A277">
         <v>275</v>
       </c>
-      <c r="C277" s="75" t="s">
+      <c r="C277" s="74" t="s">
         <v>432</v>
       </c>
       <c r="D277" s="13" t="s">
@@ -33142,7 +34309,7 @@
       <c r="A280">
         <v>278</v>
       </c>
-      <c r="C280" s="77" t="s">
+      <c r="C280" s="76" t="s">
         <v>62</v>
       </c>
       <c r="D280" s="13" t="s">
@@ -33153,7 +34320,7 @@
       <c r="A281">
         <v>279</v>
       </c>
-      <c r="C281" s="78" t="s">
+      <c r="C281" s="77" t="s">
         <v>62</v>
       </c>
       <c r="D281" s="13" t="s">
@@ -33560,7 +34727,7 @@
       <c r="A318">
         <v>316</v>
       </c>
-      <c r="C318" s="74" t="s">
+      <c r="C318" s="73" t="s">
         <v>439</v>
       </c>
       <c r="D318" s="13" t="s">
@@ -33626,7 +34793,7 @@
       <c r="A324">
         <v>322</v>
       </c>
-      <c r="C324" s="71" t="s">
+      <c r="C324" s="70" t="s">
         <v>294</v>
       </c>
       <c r="D324" s="13" t="s">
@@ -33648,7 +34815,7 @@
       <c r="A326">
         <v>324</v>
       </c>
-      <c r="C326" s="79" t="s">
+      <c r="C326" s="78" t="s">
         <v>443</v>
       </c>
       <c r="D326" s="13" t="s">
@@ -33659,7 +34826,7 @@
       <c r="A327">
         <v>325</v>
       </c>
-      <c r="C327" s="70" t="s">
+      <c r="C327" s="69" t="s">
         <v>270</v>
       </c>
       <c r="D327" s="13" t="s">
@@ -34778,7 +35945,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ319"/>
   <sheetViews>
@@ -37233,7 +38400,7 @@
       <c r="C153" s="13" t="s">
         <v>328</v>
       </c>
-      <c r="D153" s="83" t="s">
+      <c r="D153" s="82" t="s">
         <v>152</v>
       </c>
     </row>
@@ -37409,7 +38576,7 @@
       <c r="A166" s="18">
         <v>164</v>
       </c>
-      <c r="B166" s="76" t="s">
+      <c r="B166" s="75" t="s">
         <v>413</v>
       </c>
       <c r="C166" s="13" t="s">
@@ -37421,7 +38588,7 @@
       <c r="A167" s="18">
         <v>165</v>
       </c>
-      <c r="B167" s="80" t="s">
+      <c r="B167" s="79" t="s">
         <v>385</v>
       </c>
       <c r="C167" s="13" t="s">
@@ -37755,7 +38922,7 @@
       <c r="A191" s="18">
         <v>189</v>
       </c>
-      <c r="B191" s="81" t="s">
+      <c r="B191" s="80" t="s">
         <v>467</v>
       </c>
       <c r="C191" s="13" t="s">
@@ -38298,7 +39465,7 @@
       <c r="A230" s="18">
         <v>228</v>
       </c>
-      <c r="B230" s="81" t="s">
+      <c r="B230" s="80" t="s">
         <v>442</v>
       </c>
       <c r="C230" s="13" t="s">
@@ -38326,7 +39493,7 @@
       <c r="A232" s="18">
         <v>230</v>
       </c>
-      <c r="B232" s="82" t="s">
+      <c r="B232" s="81" t="s">
         <v>486</v>
       </c>
       <c r="C232" s="13" t="s">
@@ -38956,7 +40123,7 @@
       <c r="A277" s="18">
         <v>275</v>
       </c>
-      <c r="B277" s="93" t="s">
+      <c r="B277" s="92" t="s">
         <v>603</v>
       </c>
       <c r="C277" s="13" t="s">
@@ -39096,7 +40263,7 @@
       <c r="A287" s="18">
         <v>285</v>
       </c>
-      <c r="B287" s="94" t="s">
+      <c r="B287" s="93" t="s">
         <v>563</v>
       </c>
       <c r="C287" s="13" t="s">
@@ -39152,13 +40319,13 @@
       <c r="A291" s="18">
         <v>289</v>
       </c>
-      <c r="B291" s="95" t="s">
+      <c r="B291" s="94" t="s">
         <v>542</v>
       </c>
       <c r="C291" s="13" t="s">
         <v>565</v>
       </c>
-      <c r="D291" s="97" t="s">
+      <c r="D291" s="96" t="s">
         <v>694</v>
       </c>
     </row>
@@ -39320,13 +40487,13 @@
       <c r="A303" s="18">
         <v>301</v>
       </c>
-      <c r="B303" s="96" t="s">
+      <c r="B303" s="95" t="s">
         <v>555</v>
       </c>
       <c r="C303" s="13" t="s">
         <v>565</v>
       </c>
-      <c r="D303" s="98" t="s">
+      <c r="D303" s="97" t="s">
         <v>694</v>
       </c>
     </row>
@@ -39564,7 +40731,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z101"/>
   <sheetViews>
@@ -40056,7 +41223,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="60" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A26" s="48">
         <v>24</v>
       </c>
@@ -40505,7 +41672,7 @@
       <c r="D42" s="59" t="s">
         <v>148</v>
       </c>
-      <c r="E42" s="90" t="s">
+      <c r="E42" s="89" t="s">
         <v>533</v>
       </c>
     </row>
@@ -40584,7 +41751,7 @@
       <c r="D47" s="59" t="s">
         <v>148</v>
       </c>
-      <c r="E47" s="90" t="s">
+      <c r="E47" s="89" t="s">
         <v>533</v>
       </c>
     </row>
@@ -40609,7 +41776,7 @@
       <c r="A49" s="48">
         <v>47</v>
       </c>
-      <c r="B49" s="84" t="s">
+      <c r="B49" s="83" t="s">
         <v>371</v>
       </c>
       <c r="C49" s="13" t="s">
@@ -40671,7 +41838,7 @@
       <c r="A53" s="48">
         <v>51</v>
       </c>
-      <c r="B53" s="85" t="s">
+      <c r="B53" s="84" t="s">
         <v>413</v>
       </c>
       <c r="C53" s="13" t="s">
@@ -40680,7 +41847,7 @@
       <c r="D53" s="59" t="s">
         <v>148</v>
       </c>
-      <c r="E53" s="91" t="s">
+      <c r="E53" s="90" t="s">
         <v>539</v>
       </c>
     </row>
@@ -40688,7 +41855,7 @@
       <c r="A54" s="48">
         <v>52</v>
       </c>
-      <c r="B54" s="86" t="s">
+      <c r="B54" s="85" t="s">
         <v>528</v>
       </c>
       <c r="C54" s="13" t="s">
@@ -40697,7 +41864,7 @@
       <c r="D54" s="59" t="s">
         <v>148</v>
       </c>
-      <c r="E54" s="91" t="s">
+      <c r="E54" s="90" t="s">
         <v>539</v>
       </c>
     </row>
@@ -40705,7 +41872,7 @@
       <c r="A55" s="48">
         <v>53</v>
       </c>
-      <c r="B55" s="87" t="s">
+      <c r="B55" s="86" t="s">
         <v>529</v>
       </c>
       <c r="C55" s="13" t="s">
@@ -40714,7 +41881,7 @@
       <c r="D55" s="59" t="s">
         <v>148</v>
       </c>
-      <c r="E55" s="91" t="s">
+      <c r="E55" s="90" t="s">
         <v>539</v>
       </c>
     </row>
@@ -40790,7 +41957,7 @@
       <c r="A60" s="48">
         <v>58</v>
       </c>
-      <c r="B60" s="88" t="s">
+      <c r="B60" s="87" t="s">
         <v>319</v>
       </c>
       <c r="C60" s="13" t="s">
@@ -40816,7 +41983,7 @@
       <c r="D61" s="59" t="s">
         <v>148</v>
       </c>
-      <c r="E61" s="91" t="s">
+      <c r="E61" s="90" t="s">
         <v>539</v>
       </c>
     </row>
@@ -40833,7 +42000,7 @@
       <c r="D62" s="59" t="s">
         <v>148</v>
       </c>
-      <c r="E62" s="91" t="s">
+      <c r="E62" s="90" t="s">
         <v>539</v>
       </c>
     </row>
@@ -40850,7 +42017,7 @@
       <c r="D63" s="59" t="s">
         <v>148</v>
       </c>
-      <c r="E63" s="92" t="s">
+      <c r="E63" s="91" t="s">
         <v>540</v>
       </c>
     </row>
@@ -40957,7 +42124,7 @@
       <c r="D70" s="59" t="s">
         <v>148</v>
       </c>
-      <c r="E70" s="91" t="s">
+      <c r="E70" s="90" t="s">
         <v>539</v>
       </c>
     </row>
@@ -40989,7 +42156,7 @@
       <c r="D72" s="59" t="s">
         <v>148</v>
       </c>
-      <c r="E72" s="91" t="s">
+      <c r="E72" s="90" t="s">
         <v>539</v>
       </c>
     </row>
@@ -40997,7 +42164,7 @@
       <c r="A73" s="48">
         <v>71</v>
       </c>
-      <c r="B73" s="89" t="s">
+      <c r="B73" s="88" t="s">
         <v>357</v>
       </c>
       <c r="C73" s="13" t="s">
@@ -41051,7 +42218,7 @@
       <c r="D76" s="48" t="s">
         <v>490</v>
       </c>
-      <c r="E76" s="90" t="s">
+      <c r="E76" s="89" t="s">
         <v>533</v>
       </c>
     </row>
@@ -41068,7 +42235,7 @@
       <c r="D77" s="48" t="s">
         <v>490</v>
       </c>
-      <c r="E77" s="90" t="s">
+      <c r="E77" s="89" t="s">
         <v>533</v>
       </c>
     </row>
@@ -41379,7 +42546,7 @@
       <c r="C99" s="13" t="s">
         <v>565</v>
       </c>
-      <c r="D99" s="88" t="s">
+      <c r="D99" s="87" t="s">
         <v>148</v>
       </c>
     </row>
@@ -41393,7 +42560,7 @@
       <c r="C100" s="13" t="s">
         <v>565</v>
       </c>
-      <c r="D100" s="88" t="s">
+      <c r="D100" s="87" t="s">
         <v>148</v>
       </c>
     </row>

</xml_diff>

<commit_message>
cleaned up problems with commit
</commit_message>
<xml_diff>
--- a/Literature_search/database.xlsx
+++ b/Literature_search/database.xlsx
@@ -276,7 +276,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="B66" authorId="1">
+    <comment ref="F12" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Martin,Vasilev:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+However, note that 198 is not directly divisible by 4, thus indicating that there would have been a small inbalance. Unfortunately, there is no better way to estimate the sample size given that the study was conducted decades ago. </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B67" authorId="1">
       <text>
         <r>
           <rPr>
@@ -375,7 +399,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5249" uniqueCount="1147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5254" uniqueCount="1151">
   <si>
     <t>ID</t>
   </si>
@@ -36307,6 +36331,18 @@
   </si>
   <si>
     <t>there was a 5-minute interval between reading and comprehension assessment</t>
+  </si>
+  <si>
+    <t>4(background: classical music, popular vocal, popular instrumental music, silence)</t>
+  </si>
+  <si>
+    <t>the number of participants is not given per sound condition; here, I assume that the group sizes were equal; I average out gender</t>
+  </si>
+  <si>
+    <t>2(background:  music vs silence) x 2(individuals: creative, non-creative)</t>
+  </si>
+  <si>
+    <t>it seems that some partcipants did the study online, while others did it in person; the actual type of music is not mentioned- I checked the songs and classified it as vocal; creativity is averaged out</t>
   </si>
 </sst>
 </file>
@@ -37312,9 +37348,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -37349,6 +37382,9 @@
     </xf>
     <xf numFmtId="0" fontId="50" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -37695,7 +37731,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -39015,8 +39051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G129"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39063,7 +39099,7 @@
       <c r="A3" s="47">
         <v>1</v>
       </c>
-      <c r="B3" s="146" t="s">
+      <c r="B3" s="145" t="s">
         <v>1066</v>
       </c>
       <c r="C3" s="47" t="s">
@@ -39080,7 +39116,7 @@
       <c r="A4" s="47">
         <v>2</v>
       </c>
-      <c r="B4" s="146" t="s">
+      <c r="B4" s="145" t="s">
         <v>992</v>
       </c>
       <c r="C4" s="47" t="s">
@@ -39097,7 +39133,7 @@
       <c r="A5" s="47">
         <v>3</v>
       </c>
-      <c r="B5" s="152" t="s">
+      <c r="B5" s="151" t="s">
         <v>517</v>
       </c>
       <c r="C5" s="47" t="s">
@@ -39114,7 +39150,7 @@
       <c r="A6" s="47">
         <v>4</v>
       </c>
-      <c r="B6" s="146" t="s">
+      <c r="B6" s="145" t="s">
         <v>1080</v>
       </c>
       <c r="C6" s="47" t="s">
@@ -39131,7 +39167,7 @@
       <c r="A7" s="58">
         <v>5</v>
       </c>
-      <c r="B7" s="147" t="s">
+      <c r="B7" s="146" t="s">
         <v>908</v>
       </c>
       <c r="C7" s="47" t="s">
@@ -39154,7 +39190,7 @@
       <c r="A8" s="58">
         <v>6</v>
       </c>
-      <c r="B8" s="156" t="s">
+      <c r="B8" s="155" t="s">
         <v>917</v>
       </c>
       <c r="C8" s="47" t="s">
@@ -39177,7 +39213,7 @@
       <c r="A9" s="58">
         <v>7</v>
       </c>
-      <c r="B9" s="145" t="s">
+      <c r="B9" s="144" t="s">
         <v>918</v>
       </c>
       <c r="C9" s="47" t="s">
@@ -39200,7 +39236,7 @@
       <c r="A10" s="58">
         <v>8</v>
       </c>
-      <c r="B10" s="147" t="s">
+      <c r="B10" s="146" t="s">
         <v>1141</v>
       </c>
       <c r="C10" s="47" t="s">
@@ -39212,18 +39248,15 @@
       <c r="E10" s="46" t="s">
         <v>1142</v>
       </c>
-      <c r="F10" s="47" t="s">
+      <c r="G10" s="47" t="s">
         <v>1143</v>
-      </c>
-      <c r="G10" s="47" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="58">
         <v>9</v>
       </c>
-      <c r="B11" s="147" t="s">
+      <c r="B11" s="146" t="s">
         <v>981</v>
       </c>
       <c r="C11" s="47" t="s">
@@ -39242,43 +39275,59 @@
         <v>479</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="47"/>
-      <c r="B12" s="145" t="s">
+    <row r="12" spans="1:7" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="58">
+        <v>10</v>
+      </c>
+      <c r="B12" s="144" t="s">
+        <v>1011</v>
+      </c>
+      <c r="C12" s="47" t="s">
+        <v>320</v>
+      </c>
+      <c r="D12" s="61" t="s">
+        <v>1147</v>
+      </c>
+      <c r="E12" s="58" t="s">
+        <v>1135</v>
+      </c>
+      <c r="F12" s="61" t="s">
+        <v>1148</v>
+      </c>
+      <c r="G12" s="47" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="58">
+        <v>11</v>
+      </c>
+      <c r="B13" s="146" t="s">
+        <v>914</v>
+      </c>
+      <c r="C13" s="47" t="s">
+        <v>320</v>
+      </c>
+      <c r="D13" s="61" t="s">
+        <v>1149</v>
+      </c>
+      <c r="E13" s="58" t="s">
+        <v>1135</v>
+      </c>
+      <c r="F13" s="61" t="s">
+        <v>1150</v>
+      </c>
+      <c r="G13" s="47" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="39" x14ac:dyDescent="0.25">
+      <c r="A14" s="47"/>
+      <c r="B14" s="144" t="s">
         <v>863</v>
       </c>
-      <c r="C12" s="47" t="s">
-        <v>320</v>
-      </c>
-      <c r="D12" s="47"/>
-      <c r="E12" s="47" t="s">
-        <v>479</v>
-      </c>
-      <c r="F12" s="43"/>
-      <c r="G12" s="47"/>
-    </row>
-    <row r="13" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="47"/>
-      <c r="B13" s="145" t="s">
-        <v>864</v>
-      </c>
-      <c r="C13" s="47" t="s">
-        <v>320</v>
-      </c>
-      <c r="D13" s="47"/>
-      <c r="E13" s="47" t="s">
-        <v>479</v>
-      </c>
-      <c r="F13" s="43"/>
-      <c r="G13" s="47"/>
-    </row>
-    <row r="14" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="47"/>
-      <c r="B14" s="146" t="s">
-        <v>866</v>
-      </c>
       <c r="C14" s="47" t="s">
-        <v>554</v>
+        <v>320</v>
       </c>
       <c r="D14" s="47"/>
       <c r="E14" s="47" t="s">
@@ -39287,13 +39336,13 @@
       <c r="F14" s="43"/>
       <c r="G14" s="47"/>
     </row>
-    <row r="15" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="47"/>
-      <c r="B15" s="146" t="s">
-        <v>867</v>
+      <c r="B15" s="144" t="s">
+        <v>864</v>
       </c>
       <c r="C15" s="47" t="s">
-        <v>282</v>
+        <v>320</v>
       </c>
       <c r="D15" s="47"/>
       <c r="E15" s="47" t="s">
@@ -39302,13 +39351,13 @@
       <c r="F15" s="43"/>
       <c r="G15" s="47"/>
     </row>
-    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="47"/>
       <c r="B16" s="145" t="s">
-        <v>870</v>
+        <v>866</v>
       </c>
       <c r="C16" s="47" t="s">
-        <v>320</v>
+        <v>554</v>
       </c>
       <c r="D16" s="47"/>
       <c r="E16" s="47" t="s">
@@ -39317,13 +39366,13 @@
       <c r="F16" s="43"/>
       <c r="G16" s="47"/>
     </row>
-    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A17" s="47"/>
-      <c r="B17" s="146" t="s">
-        <v>873</v>
+      <c r="B17" s="145" t="s">
+        <v>867</v>
       </c>
       <c r="C17" s="47" t="s">
-        <v>554</v>
+        <v>282</v>
       </c>
       <c r="D17" s="47"/>
       <c r="E17" s="47" t="s">
@@ -39334,11 +39383,11 @@
     </row>
     <row r="18" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="47"/>
-      <c r="B18" s="146" t="s">
-        <v>874</v>
+      <c r="B18" s="144" t="s">
+        <v>870</v>
       </c>
       <c r="C18" s="47" t="s">
-        <v>554</v>
+        <v>320</v>
       </c>
       <c r="D18" s="47"/>
       <c r="E18" s="47" t="s">
@@ -39350,10 +39399,10 @@
     <row r="19" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="47"/>
       <c r="B19" s="145" t="s">
-        <v>877</v>
+        <v>873</v>
       </c>
       <c r="C19" s="47" t="s">
-        <v>320</v>
+        <v>554</v>
       </c>
       <c r="D19" s="47"/>
       <c r="E19" s="47" t="s">
@@ -39364,28 +39413,26 @@
     </row>
     <row r="20" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="47"/>
-      <c r="B20" s="146" t="s">
-        <v>879</v>
+      <c r="B20" s="145" t="s">
+        <v>874</v>
       </c>
       <c r="C20" s="47" t="s">
-        <v>282</v>
+        <v>554</v>
       </c>
       <c r="D20" s="47"/>
       <c r="E20" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F20" s="61" t="s">
-        <v>824</v>
-      </c>
-      <c r="G20" s="61"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="47"/>
     </row>
     <row r="21" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="47"/>
-      <c r="B21" s="145" t="s">
-        <v>794</v>
+      <c r="B21" s="144" t="s">
+        <v>877</v>
       </c>
       <c r="C21" s="47" t="s">
-        <v>798</v>
+        <v>320</v>
       </c>
       <c r="D21" s="47"/>
       <c r="E21" s="47" t="s">
@@ -39394,30 +39441,30 @@
       <c r="F21" s="43"/>
       <c r="G21" s="47"/>
     </row>
-    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="47"/>
-      <c r="B22" s="147" t="s">
-        <v>886</v>
+      <c r="B22" s="145" t="s">
+        <v>879</v>
       </c>
       <c r="C22" s="47" t="s">
-        <v>320</v>
+        <v>282</v>
       </c>
       <c r="D22" s="47"/>
       <c r="E22" s="47" t="s">
         <v>479</v>
       </c>
       <c r="F22" s="61" t="s">
-        <v>486</v>
+        <v>824</v>
       </c>
       <c r="G22" s="61"/>
     </row>
-    <row r="23" spans="1:7" ht="39" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="47"/>
-      <c r="B23" s="145" t="s">
-        <v>889</v>
+      <c r="B23" s="144" t="s">
+        <v>794</v>
       </c>
       <c r="C23" s="47" t="s">
-        <v>320</v>
+        <v>798</v>
       </c>
       <c r="D23" s="47"/>
       <c r="E23" s="47" t="s">
@@ -39428,8 +39475,8 @@
     </row>
     <row r="24" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="47"/>
-      <c r="B24" s="145" t="s">
-        <v>894</v>
+      <c r="B24" s="146" t="s">
+        <v>886</v>
       </c>
       <c r="C24" s="47" t="s">
         <v>320</v>
@@ -39438,15 +39485,15 @@
       <c r="E24" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F24" s="47" t="s">
-        <v>1121</v>
-      </c>
-      <c r="G24" s="47"/>
+      <c r="F24" s="61" t="s">
+        <v>486</v>
+      </c>
+      <c r="G24" s="61"/>
     </row>
     <row r="25" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="47"/>
-      <c r="B25" s="145" t="s">
-        <v>895</v>
+      <c r="B25" s="144" t="s">
+        <v>889</v>
       </c>
       <c r="C25" s="47" t="s">
         <v>320</v>
@@ -39460,26 +39507,28 @@
     </row>
     <row r="26" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="47"/>
-      <c r="B26" s="146" t="s">
-        <v>897</v>
+      <c r="B26" s="144" t="s">
+        <v>894</v>
       </c>
       <c r="C26" s="47" t="s">
-        <v>282</v>
+        <v>320</v>
       </c>
       <c r="D26" s="47"/>
       <c r="E26" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F26" s="43"/>
+      <c r="F26" s="47" t="s">
+        <v>1121</v>
+      </c>
       <c r="G26" s="47"/>
     </row>
-    <row r="27" spans="1:7" ht="39" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A27" s="47"/>
-      <c r="B27" s="146" t="s">
-        <v>902</v>
+      <c r="B27" s="144" t="s">
+        <v>895</v>
       </c>
       <c r="C27" s="47" t="s">
-        <v>282</v>
+        <v>320</v>
       </c>
       <c r="D27" s="47"/>
       <c r="E27" s="47" t="s">
@@ -39490,8 +39539,8 @@
     </row>
     <row r="28" spans="1:7" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="47"/>
-      <c r="B28" s="146" t="s">
-        <v>903</v>
+      <c r="B28" s="145" t="s">
+        <v>897</v>
       </c>
       <c r="C28" s="47" t="s">
         <v>282</v>
@@ -39503,10 +39552,10 @@
       <c r="F28" s="43"/>
       <c r="G28" s="47"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="39" x14ac:dyDescent="0.25">
       <c r="A29" s="47"/>
-      <c r="B29" s="146" t="s">
-        <v>904</v>
+      <c r="B29" s="145" t="s">
+        <v>902</v>
       </c>
       <c r="C29" s="47" t="s">
         <v>282</v>
@@ -39518,13 +39567,13 @@
       <c r="F29" s="43"/>
       <c r="G29" s="47"/>
     </row>
-    <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="39" x14ac:dyDescent="0.25">
       <c r="A30" s="47"/>
-      <c r="B30" s="146" t="s">
-        <v>906</v>
+      <c r="B30" s="145" t="s">
+        <v>903</v>
       </c>
       <c r="C30" s="47" t="s">
-        <v>320</v>
+        <v>282</v>
       </c>
       <c r="D30" s="47"/>
       <c r="E30" s="47" t="s">
@@ -39533,27 +39582,25 @@
       <c r="F30" s="43"/>
       <c r="G30" s="47"/>
     </row>
-    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="47"/>
-      <c r="B31" s="147" t="s">
-        <v>724</v>
+      <c r="B31" s="145" t="s">
+        <v>904</v>
       </c>
       <c r="C31" s="47" t="s">
-        <v>320</v>
+        <v>282</v>
       </c>
       <c r="D31" s="47"/>
       <c r="E31" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F31" s="53" t="s">
-        <v>1123</v>
-      </c>
-      <c r="G31" s="61"/>
-    </row>
-    <row r="32" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="F31" s="43"/>
+      <c r="G31" s="47"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="47"/>
       <c r="B32" s="145" t="s">
-        <v>363</v>
+        <v>906</v>
       </c>
       <c r="C32" s="47" t="s">
         <v>320</v>
@@ -39567,85 +39614,87 @@
     </row>
     <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="47"/>
-      <c r="B33" s="148" t="s">
-        <v>90</v>
+      <c r="B33" s="146" t="s">
+        <v>724</v>
       </c>
       <c r="C33" s="47" t="s">
-        <v>282</v>
+        <v>320</v>
       </c>
       <c r="D33" s="47"/>
       <c r="E33" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F33" s="43"/>
-      <c r="G33" s="47"/>
+      <c r="F33" s="53" t="s">
+        <v>1123</v>
+      </c>
+      <c r="G33" s="61"/>
     </row>
     <row r="34" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="121"/>
-      <c r="B34" s="143" t="s">
-        <v>55</v>
-      </c>
-      <c r="C34" s="121" t="s">
-        <v>282</v>
-      </c>
-      <c r="D34" s="121"/>
-      <c r="E34" s="121"/>
-      <c r="F34" s="122" t="s">
-        <v>835</v>
-      </c>
-      <c r="G34" s="157"/>
-    </row>
-    <row r="35" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" s="47"/>
+      <c r="B34" s="144" t="s">
+        <v>363</v>
+      </c>
+      <c r="C34" s="47" t="s">
+        <v>320</v>
+      </c>
+      <c r="D34" s="47"/>
+      <c r="E34" s="47" t="s">
+        <v>479</v>
+      </c>
+      <c r="F34" s="43"/>
+      <c r="G34" s="47"/>
+    </row>
+    <row r="35" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="47"/>
-      <c r="B35" s="149" t="s">
-        <v>721</v>
+      <c r="B35" s="147" t="s">
+        <v>90</v>
       </c>
       <c r="C35" s="47" t="s">
-        <v>320</v>
+        <v>282</v>
       </c>
       <c r="D35" s="47"/>
       <c r="E35" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F35" s="53" t="s">
-        <v>1125</v>
-      </c>
-      <c r="G35" s="61"/>
-    </row>
-    <row r="36" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A36" s="47"/>
-      <c r="B36" s="145" t="s">
-        <v>914</v>
-      </c>
-      <c r="C36" s="47" t="s">
-        <v>320</v>
-      </c>
-      <c r="D36" s="47"/>
-      <c r="E36" s="47" t="s">
-        <v>479</v>
-      </c>
-      <c r="F36" s="43"/>
-      <c r="G36" s="47"/>
-    </row>
-    <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="F35" s="43"/>
+      <c r="G35" s="47"/>
+    </row>
+    <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="121"/>
+      <c r="B36" s="143" t="s">
+        <v>55</v>
+      </c>
+      <c r="C36" s="121" t="s">
+        <v>282</v>
+      </c>
+      <c r="D36" s="121"/>
+      <c r="E36" s="121"/>
+      <c r="F36" s="122" t="s">
+        <v>835</v>
+      </c>
+      <c r="G36" s="156"/>
+    </row>
+    <row r="37" spans="1:7" ht="39" x14ac:dyDescent="0.25">
       <c r="A37" s="47"/>
-      <c r="B37" s="146" t="s">
-        <v>762</v>
+      <c r="B37" s="148" t="s">
+        <v>721</v>
       </c>
       <c r="C37" s="47" t="s">
-        <v>282</v>
+        <v>320</v>
       </c>
       <c r="D37" s="47"/>
       <c r="E37" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F37" s="43"/>
-      <c r="G37" s="47"/>
-    </row>
-    <row r="38" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F37" s="53" t="s">
+        <v>1125</v>
+      </c>
+      <c r="G37" s="61"/>
+    </row>
+    <row r="38" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="47"/>
-      <c r="B38" s="150" t="s">
-        <v>82</v>
+      <c r="B38" s="145" t="s">
+        <v>762</v>
       </c>
       <c r="C38" s="47" t="s">
         <v>282</v>
@@ -39657,10 +39706,10 @@
       <c r="F38" s="43"/>
       <c r="G38" s="47"/>
     </row>
-    <row r="39" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="47"/>
-      <c r="B39" s="145" t="s">
-        <v>81</v>
+      <c r="B39" s="149" t="s">
+        <v>82</v>
       </c>
       <c r="C39" s="47" t="s">
         <v>282</v>
@@ -39674,11 +39723,11 @@
     </row>
     <row r="40" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="47"/>
-      <c r="B40" s="151" t="s">
-        <v>919</v>
+      <c r="B40" s="144" t="s">
+        <v>81</v>
       </c>
       <c r="C40" s="47" t="s">
-        <v>320</v>
+        <v>282</v>
       </c>
       <c r="D40" s="47"/>
       <c r="E40" s="47" t="s">
@@ -39687,10 +39736,10 @@
       <c r="F40" s="43"/>
       <c r="G40" s="47"/>
     </row>
-    <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A41" s="47"/>
-      <c r="B41" s="146" t="s">
-        <v>921</v>
+      <c r="B41" s="150" t="s">
+        <v>919</v>
       </c>
       <c r="C41" s="47" t="s">
         <v>320</v>
@@ -39702,10 +39751,10 @@
       <c r="F41" s="43"/>
       <c r="G41" s="47"/>
     </row>
-    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A42" s="47"/>
-      <c r="B42" s="146" t="s">
-        <v>518</v>
+      <c r="B42" s="145" t="s">
+        <v>921</v>
       </c>
       <c r="C42" s="47" t="s">
         <v>320</v>
@@ -39720,7 +39769,7 @@
     <row r="43" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="47"/>
       <c r="B43" s="145" t="s">
-        <v>923</v>
+        <v>518</v>
       </c>
       <c r="C43" s="47" t="s">
         <v>320</v>
@@ -39734,8 +39783,8 @@
     </row>
     <row r="44" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="47"/>
-      <c r="B44" s="145" t="s">
-        <v>924</v>
+      <c r="B44" s="144" t="s">
+        <v>923</v>
       </c>
       <c r="C44" s="47" t="s">
         <v>320</v>
@@ -39749,8 +39798,8 @@
     </row>
     <row r="45" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="47"/>
-      <c r="B45" s="145" t="s">
-        <v>925</v>
+      <c r="B45" s="144" t="s">
+        <v>924</v>
       </c>
       <c r="C45" s="47" t="s">
         <v>320</v>
@@ -39764,8 +39813,8 @@
     </row>
     <row r="46" spans="1:7" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="47"/>
-      <c r="B46" s="145" t="s">
-        <v>926</v>
+      <c r="B46" s="144" t="s">
+        <v>925</v>
       </c>
       <c r="C46" s="47" t="s">
         <v>320</v>
@@ -39777,13 +39826,13 @@
       <c r="F46" s="43"/>
       <c r="G46" s="47"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A47" s="47"/>
-      <c r="B47" s="146" t="s">
-        <v>927</v>
+      <c r="B47" s="144" t="s">
+        <v>926</v>
       </c>
       <c r="C47" s="47" t="s">
-        <v>282</v>
+        <v>320</v>
       </c>
       <c r="D47" s="47"/>
       <c r="E47" s="47" t="s">
@@ -39792,13 +39841,13 @@
       <c r="F47" s="43"/>
       <c r="G47" s="47"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="47"/>
       <c r="B48" s="145" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="C48" s="47" t="s">
-        <v>320</v>
+        <v>282</v>
       </c>
       <c r="D48" s="47"/>
       <c r="E48" s="47" t="s">
@@ -39809,11 +39858,11 @@
     </row>
     <row r="49" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="47"/>
-      <c r="B49" s="153" t="s">
-        <v>931</v>
+      <c r="B49" s="144" t="s">
+        <v>928</v>
       </c>
       <c r="C49" s="47" t="s">
-        <v>282</v>
+        <v>320</v>
       </c>
       <c r="D49" s="47"/>
       <c r="E49" s="47" t="s">
@@ -39824,11 +39873,11 @@
     </row>
     <row r="50" spans="1:7" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="47"/>
-      <c r="B50" s="145" t="s">
-        <v>703</v>
+      <c r="B50" s="152" t="s">
+        <v>931</v>
       </c>
       <c r="C50" s="47" t="s">
-        <v>320</v>
+        <v>282</v>
       </c>
       <c r="D50" s="47"/>
       <c r="E50" s="47" t="s">
@@ -39839,11 +39888,11 @@
     </row>
     <row r="51" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="47"/>
-      <c r="B51" s="146" t="s">
-        <v>935</v>
+      <c r="B51" s="144" t="s">
+        <v>703</v>
       </c>
       <c r="C51" s="47" t="s">
-        <v>282</v>
+        <v>320</v>
       </c>
       <c r="D51" s="47"/>
       <c r="E51" s="47" t="s">
@@ -39855,10 +39904,10 @@
     <row r="52" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="47"/>
       <c r="B52" s="145" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="C52" s="47" t="s">
-        <v>320</v>
+        <v>282</v>
       </c>
       <c r="D52" s="47"/>
       <c r="E52" s="47" t="s">
@@ -39869,11 +39918,11 @@
     </row>
     <row r="53" spans="1:7" ht="39" x14ac:dyDescent="0.25">
       <c r="A53" s="47"/>
-      <c r="B53" s="146" t="s">
-        <v>937</v>
+      <c r="B53" s="144" t="s">
+        <v>936</v>
       </c>
       <c r="C53" s="47" t="s">
-        <v>554</v>
+        <v>320</v>
       </c>
       <c r="D53" s="47"/>
       <c r="E53" s="47" t="s">
@@ -39884,8 +39933,8 @@
     </row>
     <row r="54" spans="1:7" ht="39" x14ac:dyDescent="0.25">
       <c r="A54" s="47"/>
-      <c r="B54" s="146" t="s">
-        <v>938</v>
+      <c r="B54" s="145" t="s">
+        <v>937</v>
       </c>
       <c r="C54" s="47" t="s">
         <v>554</v>
@@ -39899,8 +39948,8 @@
     </row>
     <row r="55" spans="1:7" ht="39" x14ac:dyDescent="0.25">
       <c r="A55" s="47"/>
-      <c r="B55" s="146" t="s">
-        <v>939</v>
+      <c r="B55" s="145" t="s">
+        <v>938</v>
       </c>
       <c r="C55" s="47" t="s">
         <v>554</v>
@@ -39914,11 +39963,11 @@
     </row>
     <row r="56" spans="1:7" ht="39" x14ac:dyDescent="0.25">
       <c r="A56" s="47"/>
-      <c r="B56" s="150" t="s">
-        <v>940</v>
+      <c r="B56" s="145" t="s">
+        <v>939</v>
       </c>
       <c r="C56" s="47" t="s">
-        <v>282</v>
+        <v>554</v>
       </c>
       <c r="D56" s="47"/>
       <c r="E56" s="47" t="s">
@@ -39927,10 +39976,10 @@
       <c r="F56" s="43"/>
       <c r="G56" s="47"/>
     </row>
-    <row r="57" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" ht="39" x14ac:dyDescent="0.25">
       <c r="A57" s="47"/>
-      <c r="B57" s="146" t="s">
-        <v>941</v>
+      <c r="B57" s="149" t="s">
+        <v>940</v>
       </c>
       <c r="C57" s="47" t="s">
         <v>282</v>
@@ -39944,8 +39993,8 @@
     </row>
     <row r="58" spans="1:7" ht="39" x14ac:dyDescent="0.25">
       <c r="A58" s="47"/>
-      <c r="B58" s="150" t="s">
-        <v>942</v>
+      <c r="B58" s="145" t="s">
+        <v>941</v>
       </c>
       <c r="C58" s="47" t="s">
         <v>282</v>
@@ -39959,8 +40008,8 @@
     </row>
     <row r="59" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A59" s="47"/>
-      <c r="B59" s="150" t="s">
-        <v>943</v>
+      <c r="B59" s="149" t="s">
+        <v>942</v>
       </c>
       <c r="C59" s="47" t="s">
         <v>282</v>
@@ -39972,10 +40021,10 @@
       <c r="F59" s="43"/>
       <c r="G59" s="47"/>
     </row>
-    <row r="60" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" ht="39" x14ac:dyDescent="0.25">
       <c r="A60" s="47"/>
-      <c r="B60" s="146" t="s">
-        <v>944</v>
+      <c r="B60" s="149" t="s">
+        <v>943</v>
       </c>
       <c r="C60" s="47" t="s">
         <v>282</v>
@@ -39989,11 +40038,11 @@
     </row>
     <row r="61" spans="1:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="47"/>
-      <c r="B61" s="146" t="s">
-        <v>945</v>
+      <c r="B61" s="145" t="s">
+        <v>944</v>
       </c>
       <c r="C61" s="47" t="s">
-        <v>554</v>
+        <v>282</v>
       </c>
       <c r="D61" s="47"/>
       <c r="E61" s="47" t="s">
@@ -40002,10 +40051,10 @@
       <c r="F61" s="43"/>
       <c r="G61" s="47"/>
     </row>
-    <row r="62" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A62" s="47"/>
-      <c r="B62" s="146" t="s">
-        <v>946</v>
+      <c r="B62" s="145" t="s">
+        <v>945</v>
       </c>
       <c r="C62" s="47" t="s">
         <v>554</v>
@@ -40020,10 +40069,10 @@
     <row r="63" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="47"/>
       <c r="B63" s="145" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="C63" s="47" t="s">
-        <v>320</v>
+        <v>554</v>
       </c>
       <c r="D63" s="47"/>
       <c r="E63" s="47" t="s">
@@ -40032,10 +40081,10 @@
       <c r="F63" s="43"/>
       <c r="G63" s="47"/>
     </row>
-    <row r="64" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="47"/>
-      <c r="B64" s="145" t="s">
-        <v>950</v>
+      <c r="B64" s="144" t="s">
+        <v>947</v>
       </c>
       <c r="C64" s="47" t="s">
         <v>320</v>
@@ -40044,15 +40093,13 @@
       <c r="E64" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F64" s="61" t="s">
-        <v>497</v>
-      </c>
-      <c r="G64" s="61"/>
+      <c r="F64" s="43"/>
+      <c r="G64" s="47"/>
     </row>
     <row r="65" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="47"/>
-      <c r="B65" s="145" t="s">
-        <v>952</v>
+      <c r="B65" s="144" t="s">
+        <v>950</v>
       </c>
       <c r="C65" s="47" t="s">
         <v>320</v>
@@ -40061,16 +40108,18 @@
       <c r="E65" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F65" s="43"/>
-      <c r="G65" s="47"/>
-    </row>
-    <row r="66" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="F65" s="61" t="s">
+        <v>497</v>
+      </c>
+      <c r="G65" s="61"/>
+    </row>
+    <row r="66" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A66" s="47"/>
-      <c r="B66" s="147" t="s">
-        <v>737</v>
+      <c r="B66" s="144" t="s">
+        <v>952</v>
       </c>
       <c r="C66" s="47" t="s">
-        <v>282</v>
+        <v>320</v>
       </c>
       <c r="D66" s="47"/>
       <c r="E66" s="47" t="s">
@@ -40079,10 +40128,10 @@
       <c r="F66" s="43"/>
       <c r="G66" s="47"/>
     </row>
-    <row r="67" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A67" s="47"/>
       <c r="B67" s="146" t="s">
-        <v>959</v>
+        <v>737</v>
       </c>
       <c r="C67" s="47" t="s">
         <v>282</v>
@@ -40097,7 +40146,7 @@
     <row r="68" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="47"/>
       <c r="B68" s="145" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="C68" s="47" t="s">
         <v>282</v>
@@ -40111,11 +40160,11 @@
     </row>
     <row r="69" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="47"/>
-      <c r="B69" s="145" t="s">
-        <v>745</v>
+      <c r="B69" s="144" t="s">
+        <v>960</v>
       </c>
       <c r="C69" s="47" t="s">
-        <v>798</v>
+        <v>282</v>
       </c>
       <c r="D69" s="47"/>
       <c r="E69" s="47" t="s">
@@ -40126,11 +40175,11 @@
     </row>
     <row r="70" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A70" s="47"/>
-      <c r="B70" s="146" t="s">
-        <v>962</v>
+      <c r="B70" s="144" t="s">
+        <v>745</v>
       </c>
       <c r="C70" s="47" t="s">
-        <v>554</v>
+        <v>798</v>
       </c>
       <c r="D70" s="47"/>
       <c r="E70" s="47" t="s">
@@ -40141,8 +40190,8 @@
     </row>
     <row r="71" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A71" s="47"/>
-      <c r="B71" s="146" t="s">
-        <v>549</v>
+      <c r="B71" s="145" t="s">
+        <v>962</v>
       </c>
       <c r="C71" s="47" t="s">
         <v>554</v>
@@ -40151,30 +40200,30 @@
       <c r="E71" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F71" s="43" t="s">
-        <v>839</v>
-      </c>
+      <c r="F71" s="43"/>
       <c r="G71" s="47"/>
     </row>
-    <row r="72" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A72" s="47"/>
-      <c r="B72" s="146" t="s">
-        <v>966</v>
+      <c r="B72" s="145" t="s">
+        <v>549</v>
       </c>
       <c r="C72" s="47" t="s">
-        <v>282</v>
+        <v>554</v>
       </c>
       <c r="D72" s="47"/>
       <c r="E72" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F72" s="43"/>
+      <c r="F72" s="43" t="s">
+        <v>839</v>
+      </c>
       <c r="G72" s="47"/>
     </row>
     <row r="73" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A73" s="47"/>
-      <c r="B73" s="146" t="s">
-        <v>968</v>
+      <c r="B73" s="145" t="s">
+        <v>966</v>
       </c>
       <c r="C73" s="47" t="s">
         <v>282</v>
@@ -40189,10 +40238,10 @@
     <row r="74" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="47"/>
       <c r="B74" s="145" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="C74" s="47" t="s">
-        <v>320</v>
+        <v>282</v>
       </c>
       <c r="D74" s="47"/>
       <c r="E74" s="47" t="s">
@@ -40203,11 +40252,11 @@
     </row>
     <row r="75" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A75" s="47"/>
-      <c r="B75" s="146" t="s">
-        <v>970</v>
+      <c r="B75" s="144" t="s">
+        <v>969</v>
       </c>
       <c r="C75" s="47" t="s">
-        <v>554</v>
+        <v>320</v>
       </c>
       <c r="D75" s="47"/>
       <c r="E75" s="47" t="s">
@@ -40219,10 +40268,10 @@
     <row r="76" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="47"/>
       <c r="B76" s="145" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="C76" s="47" t="s">
-        <v>320</v>
+        <v>554</v>
       </c>
       <c r="D76" s="47"/>
       <c r="E76" s="47" t="s">
@@ -40231,10 +40280,10 @@
       <c r="F76" s="43"/>
       <c r="G76" s="47"/>
     </row>
-    <row r="77" spans="1:7" ht="39" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A77" s="47"/>
-      <c r="B77" s="146" t="s">
-        <v>975</v>
+      <c r="B77" s="144" t="s">
+        <v>971</v>
       </c>
       <c r="C77" s="47" t="s">
         <v>320</v>
@@ -40249,7 +40298,7 @@
     <row r="78" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="47"/>
       <c r="B78" s="145" t="s">
-        <v>978</v>
+        <v>975</v>
       </c>
       <c r="C78" s="47" t="s">
         <v>320</v>
@@ -40263,8 +40312,8 @@
     </row>
     <row r="79" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="47"/>
-      <c r="B79" s="146" t="s">
-        <v>980</v>
+      <c r="B79" s="144" t="s">
+        <v>978</v>
       </c>
       <c r="C79" s="47" t="s">
         <v>320</v>
@@ -40278,11 +40327,11 @@
     </row>
     <row r="80" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="47"/>
-      <c r="B80" s="146" t="s">
-        <v>984</v>
+      <c r="B80" s="145" t="s">
+        <v>980</v>
       </c>
       <c r="C80" s="47" t="s">
-        <v>282</v>
+        <v>320</v>
       </c>
       <c r="D80" s="47"/>
       <c r="E80" s="47" t="s">
@@ -40293,8 +40342,8 @@
     </row>
     <row r="81" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="47"/>
-      <c r="B81" s="146" t="s">
-        <v>985</v>
+      <c r="B81" s="145" t="s">
+        <v>984</v>
       </c>
       <c r="C81" s="47" t="s">
         <v>282</v>
@@ -40306,13 +40355,13 @@
       <c r="F81" s="43"/>
       <c r="G81" s="47"/>
     </row>
-    <row r="82" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="47"/>
       <c r="B82" s="145" t="s">
-        <v>747</v>
+        <v>985</v>
       </c>
       <c r="C82" s="47" t="s">
-        <v>798</v>
+        <v>282</v>
       </c>
       <c r="D82" s="47"/>
       <c r="E82" s="47" t="s">
@@ -40321,13 +40370,13 @@
       <c r="F82" s="43"/>
       <c r="G82" s="47"/>
     </row>
-    <row r="83" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A83" s="47"/>
-      <c r="B83" s="146" t="s">
-        <v>988</v>
+      <c r="B83" s="144" t="s">
+        <v>747</v>
       </c>
       <c r="C83" s="47" t="s">
-        <v>554</v>
+        <v>798</v>
       </c>
       <c r="D83" s="47"/>
       <c r="E83" s="47" t="s">
@@ -40336,45 +40385,45 @@
       <c r="F83" s="43"/>
       <c r="G83" s="47"/>
     </row>
-    <row r="84" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="47"/>
       <c r="B84" s="145" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
       <c r="C84" s="47" t="s">
-        <v>320</v>
+        <v>554</v>
       </c>
       <c r="D84" s="47"/>
       <c r="E84" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F84" s="47" t="s">
-        <v>861</v>
-      </c>
+      <c r="F84" s="43"/>
       <c r="G84" s="47"/>
     </row>
     <row r="85" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A85" s="47"/>
-      <c r="B85" s="146" t="s">
-        <v>769</v>
+      <c r="B85" s="144" t="s">
+        <v>990</v>
       </c>
       <c r="C85" s="47" t="s">
-        <v>798</v>
+        <v>320</v>
       </c>
       <c r="D85" s="47"/>
       <c r="E85" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F85" s="43"/>
+      <c r="F85" s="47" t="s">
+        <v>861</v>
+      </c>
       <c r="G85" s="47"/>
     </row>
     <row r="86" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="47"/>
-      <c r="B86" s="146" t="s">
-        <v>994</v>
+      <c r="B86" s="145" t="s">
+        <v>769</v>
       </c>
       <c r="C86" s="47" t="s">
-        <v>282</v>
+        <v>798</v>
       </c>
       <c r="D86" s="47"/>
       <c r="E86" s="47" t="s">
@@ -40385,8 +40434,8 @@
     </row>
     <row r="87" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="47"/>
-      <c r="B87" s="150" t="s">
-        <v>139</v>
+      <c r="B87" s="145" t="s">
+        <v>994</v>
       </c>
       <c r="C87" s="47" t="s">
         <v>282</v>
@@ -40400,11 +40449,11 @@
     </row>
     <row r="88" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A88" s="47"/>
-      <c r="B88" s="146" t="s">
-        <v>1004</v>
+      <c r="B88" s="149" t="s">
+        <v>139</v>
       </c>
       <c r="C88" s="47" t="s">
-        <v>554</v>
+        <v>282</v>
       </c>
       <c r="D88" s="47"/>
       <c r="E88" s="47" t="s">
@@ -40415,11 +40464,11 @@
     </row>
     <row r="89" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A89" s="47"/>
-      <c r="B89" s="150" t="s">
-        <v>1005</v>
+      <c r="B89" s="145" t="s">
+        <v>1004</v>
       </c>
       <c r="C89" s="47" t="s">
-        <v>282</v>
+        <v>554</v>
       </c>
       <c r="D89" s="47"/>
       <c r="E89" s="47" t="s">
@@ -40428,10 +40477,10 @@
       <c r="F89" s="43"/>
       <c r="G89" s="47"/>
     </row>
-    <row r="90" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A90" s="47"/>
-      <c r="B90" s="150" t="s">
-        <v>88</v>
+      <c r="B90" s="149" t="s">
+        <v>1005</v>
       </c>
       <c r="C90" s="47" t="s">
         <v>282</v>
@@ -40443,13 +40492,13 @@
       <c r="F90" s="43"/>
       <c r="G90" s="47"/>
     </row>
-    <row r="91" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A91" s="47"/>
-      <c r="B91" s="145" t="s">
-        <v>1011</v>
+      <c r="B91" s="149" t="s">
+        <v>88</v>
       </c>
       <c r="C91" s="47" t="s">
-        <v>320</v>
+        <v>282</v>
       </c>
       <c r="D91" s="47"/>
       <c r="E91" s="47" t="s">
@@ -40458,9 +40507,9 @@
       <c r="F91" s="43"/>
       <c r="G91" s="47"/>
     </row>
-    <row r="92" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A92" s="47"/>
-      <c r="B92" s="146" t="s">
+      <c r="B92" s="145" t="s">
         <v>1012</v>
       </c>
       <c r="C92" s="47" t="s">
@@ -40475,7 +40524,7 @@
     </row>
     <row r="93" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A93" s="47"/>
-      <c r="B93" s="146" t="s">
+      <c r="B93" s="145" t="s">
         <v>1014</v>
       </c>
       <c r="C93" s="47" t="s">
@@ -40490,7 +40539,7 @@
     </row>
     <row r="94" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" s="47"/>
-      <c r="B94" s="145" t="s">
+      <c r="B94" s="144" t="s">
         <v>1017</v>
       </c>
       <c r="C94" s="47" t="s">
@@ -40505,7 +40554,7 @@
     </row>
     <row r="95" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="47"/>
-      <c r="B95" s="146" t="s">
+      <c r="B95" s="145" t="s">
         <v>1020</v>
       </c>
       <c r="C95" s="47" t="s">
@@ -40520,7 +40569,7 @@
     </row>
     <row r="96" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A96" s="47"/>
-      <c r="B96" s="146" t="s">
+      <c r="B96" s="145" t="s">
         <v>767</v>
       </c>
       <c r="C96" s="47" t="s">
@@ -40535,7 +40584,7 @@
     </row>
     <row r="97" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="47"/>
-      <c r="B97" s="150" t="s">
+      <c r="B97" s="149" t="s">
         <v>1025</v>
       </c>
       <c r="C97" s="47" t="s">
@@ -40550,7 +40599,7 @@
     </row>
     <row r="98" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="47"/>
-      <c r="B98" s="145" t="s">
+      <c r="B98" s="144" t="s">
         <v>1026</v>
       </c>
       <c r="C98" s="47" t="s">
@@ -40565,7 +40614,7 @@
     </row>
     <row r="99" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="47"/>
-      <c r="B99" s="145" t="s">
+      <c r="B99" s="144" t="s">
         <v>1030</v>
       </c>
       <c r="C99" s="47" t="s">
@@ -40580,7 +40629,7 @@
     </row>
     <row r="100" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="47"/>
-      <c r="B100" s="145" t="s">
+      <c r="B100" s="144" t="s">
         <v>1033</v>
       </c>
       <c r="C100" s="47" t="s">
@@ -40595,7 +40644,7 @@
     </row>
     <row r="101" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A101" s="47"/>
-      <c r="B101" s="145" t="s">
+      <c r="B101" s="144" t="s">
         <v>1034</v>
       </c>
       <c r="C101" s="47" t="s">
@@ -40610,7 +40659,7 @@
     </row>
     <row r="102" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A102" s="47"/>
-      <c r="B102" s="147" t="s">
+      <c r="B102" s="146" t="s">
         <v>328</v>
       </c>
       <c r="C102" s="47" t="s">
@@ -40627,7 +40676,7 @@
     </row>
     <row r="103" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="47"/>
-      <c r="B103" s="145" t="s">
+      <c r="B103" s="144" t="s">
         <v>1039</v>
       </c>
       <c r="C103" s="47" t="s">
@@ -40642,7 +40691,7 @@
     </row>
     <row r="104" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="47"/>
-      <c r="B104" s="145" t="s">
+      <c r="B104" s="144" t="s">
         <v>58</v>
       </c>
       <c r="C104" s="47" t="s">
@@ -40657,7 +40706,7 @@
     </row>
     <row r="105" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A105" s="47"/>
-      <c r="B105" s="145" t="s">
+      <c r="B105" s="144" t="s">
         <v>96</v>
       </c>
       <c r="C105" s="47" t="s">
@@ -40670,9 +40719,9 @@
       <c r="F105" s="43"/>
       <c r="G105" s="47"/>
     </row>
-    <row r="106" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="47"/>
-      <c r="B106" s="146" t="s">
+      <c r="B106" s="145" t="s">
         <v>1057</v>
       </c>
       <c r="C106" s="47" t="s">
@@ -40687,7 +40736,7 @@
     </row>
     <row r="107" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="47"/>
-      <c r="B107" s="145" t="s">
+      <c r="B107" s="144" t="s">
         <v>775</v>
       </c>
       <c r="C107" s="47" t="s">
@@ -40715,7 +40764,7 @@
     </row>
     <row r="109" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="47"/>
-      <c r="B109" s="145" t="s">
+      <c r="B109" s="144" t="s">
         <v>783</v>
       </c>
       <c r="C109" s="47" t="s">
@@ -40730,7 +40779,7 @@
     </row>
     <row r="110" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A110" s="47"/>
-      <c r="B110" s="145" t="s">
+      <c r="B110" s="144" t="s">
         <v>69</v>
       </c>
       <c r="C110" s="47" t="s">
@@ -40745,7 +40794,7 @@
     </row>
     <row r="111" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A111" s="47"/>
-      <c r="B111" s="150" t="s">
+      <c r="B111" s="149" t="s">
         <v>1058</v>
       </c>
       <c r="C111" s="47" t="s">
@@ -40760,7 +40809,7 @@
     </row>
     <row r="112" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="47"/>
-      <c r="B112" s="154" t="s">
+      <c r="B112" s="153" t="s">
         <v>781</v>
       </c>
       <c r="C112" s="47" t="s">
@@ -40775,7 +40824,7 @@
     </row>
     <row r="113" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A113" s="47"/>
-      <c r="B113" s="145" t="s">
+      <c r="B113" s="144" t="s">
         <v>753</v>
       </c>
       <c r="C113" s="47" t="s">
@@ -40790,7 +40839,7 @@
     </row>
     <row r="114" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A114" s="47"/>
-      <c r="B114" s="145" t="s">
+      <c r="B114" s="144" t="s">
         <v>59</v>
       </c>
       <c r="C114" s="47" t="s">
@@ -40805,7 +40854,7 @@
     </row>
     <row r="115" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="47"/>
-      <c r="B115" s="145" t="s">
+      <c r="B115" s="144" t="s">
         <v>754</v>
       </c>
       <c r="C115" s="47" t="s">
@@ -40820,7 +40869,7 @@
     </row>
     <row r="116" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A116" s="47"/>
-      <c r="B116" s="146" t="s">
+      <c r="B116" s="145" t="s">
         <v>768</v>
       </c>
       <c r="C116" s="47" t="s">
@@ -40837,7 +40886,7 @@
     </row>
     <row r="117" spans="1:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="47"/>
-      <c r="B117" s="146" t="s">
+      <c r="B117" s="145" t="s">
         <v>1065</v>
       </c>
       <c r="C117" s="47" t="s">
@@ -40852,7 +40901,7 @@
     </row>
     <row r="118" spans="1:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="47"/>
-      <c r="B118" s="150" t="s">
+      <c r="B118" s="149" t="s">
         <v>1071</v>
       </c>
       <c r="C118" s="47" t="s">
@@ -40867,7 +40916,7 @@
     </row>
     <row r="119" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A119" s="47"/>
-      <c r="B119" s="146" t="s">
+      <c r="B119" s="145" t="s">
         <v>1072</v>
       </c>
       <c r="C119" s="47" t="s">
@@ -40882,7 +40931,7 @@
     </row>
     <row r="120" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="47"/>
-      <c r="B120" s="145" t="s">
+      <c r="B120" s="144" t="s">
         <v>1077</v>
       </c>
       <c r="C120" s="47" t="s">
@@ -40897,7 +40946,7 @@
     </row>
     <row r="121" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="47"/>
-      <c r="B121" s="146" t="s">
+      <c r="B121" s="145" t="s">
         <v>188</v>
       </c>
       <c r="C121" s="47" t="s">
@@ -40914,7 +40963,7 @@
     </row>
     <row r="122" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A122" s="47"/>
-      <c r="B122" s="145" t="s">
+      <c r="B122" s="144" t="s">
         <v>95</v>
       </c>
       <c r="C122" s="47" t="s">
@@ -40929,7 +40978,7 @@
     </row>
     <row r="123" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A123" s="47"/>
-      <c r="B123" s="146" t="s">
+      <c r="B123" s="145" t="s">
         <v>1087</v>
       </c>
       <c r="C123" s="47" t="s">
@@ -40944,7 +40993,7 @@
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="47"/>
-      <c r="B124" s="153" t="s">
+      <c r="B124" s="152" t="s">
         <v>1090</v>
       </c>
       <c r="C124" s="47" t="s">
@@ -40959,7 +41008,7 @@
     </row>
     <row r="125" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A125" s="47"/>
-      <c r="B125" s="146" t="s">
+      <c r="B125" s="145" t="s">
         <v>1091</v>
       </c>
       <c r="C125" s="47" t="s">
@@ -40974,7 +41023,7 @@
     </row>
     <row r="126" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A126" s="47"/>
-      <c r="B126" s="145" t="s">
+      <c r="B126" s="144" t="s">
         <v>80</v>
       </c>
       <c r="C126" s="47" t="s">
@@ -40989,7 +41038,7 @@
     </row>
     <row r="127" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A127" s="47"/>
-      <c r="B127" s="147" t="s">
+      <c r="B127" s="146" t="s">
         <v>726</v>
       </c>
       <c r="C127" s="47" t="s">
@@ -41006,7 +41055,7 @@
     </row>
     <row r="128" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="47"/>
-      <c r="B128" s="155" t="s">
+      <c r="B128" s="154" t="s">
         <v>137</v>
       </c>
       <c r="C128" s="47" t="s">
@@ -41021,7 +41070,7 @@
     </row>
     <row r="129" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A129" s="47"/>
-      <c r="B129" s="146" t="s">
+      <c r="B129" s="145" t="s">
         <v>1101</v>
       </c>
       <c r="C129" s="47" t="s">
@@ -51515,14 +51564,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="144"/>
-      <c r="B1" s="144"/>
-      <c r="C1" s="144"/>
-      <c r="D1" s="144"/>
-      <c r="E1" s="144"/>
-      <c r="F1" s="144"/>
-      <c r="G1" s="144"/>
-      <c r="H1" s="144"/>
+      <c r="A1" s="157"/>
+      <c r="B1" s="157"/>
+      <c r="C1" s="157"/>
+      <c r="D1" s="157"/>
+      <c r="E1" s="157"/>
+      <c r="F1" s="157"/>
+      <c r="G1" s="157"/>
+      <c r="H1" s="157"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">

</xml_diff>

<commit_message>
some code to calculate effect sizes
</commit_message>
<xml_diff>
--- a/Literature_search/database.xlsx
+++ b/Literature_search/database.xlsx
@@ -399,7 +399,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5257" uniqueCount="1153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5259" uniqueCount="1154">
   <si>
     <t>ID</t>
   </si>
@@ -36348,7 +36348,10 @@
     <t>2(background:  music vs silence)</t>
   </si>
   <si>
-    <t>classified sample as children even though they were 16-17</t>
+    <t>3(background:  music, noise, silence) x 2(personality: introvert vs extravert)</t>
+  </si>
+  <si>
+    <t>classified sample as children even though they were 16-17; personality type was averaged out</t>
   </si>
 </sst>
 </file>
@@ -39058,7 +39061,7 @@
   <dimension ref="A1:G129"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39348,24 +39351,28 @@
         <v>479</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="47">
+    <row r="15" spans="1:7" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="58">
         <v>13</v>
       </c>
-      <c r="B15" s="144" t="s">
+      <c r="B15" s="146" t="s">
         <v>926</v>
       </c>
       <c r="C15" s="47" t="s">
         <v>320</v>
       </c>
-      <c r="D15" s="47"/>
-      <c r="E15" s="47" t="s">
+      <c r="D15" s="61" t="s">
+        <v>1152</v>
+      </c>
+      <c r="E15" s="58" t="s">
+        <v>1135</v>
+      </c>
+      <c r="F15" s="61" t="s">
+        <v>1153</v>
+      </c>
+      <c r="G15" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F15" s="61" t="s">
-        <v>1152</v>
-      </c>
-      <c r="G15" s="47"/>
     </row>
     <row r="16" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="47"/>

</xml_diff>

<commit_message>
updated with more data
</commit_message>
<xml_diff>
--- a/Literature_search/database.xlsx
+++ b/Literature_search/database.xlsx
@@ -390,7 +390,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4893" uniqueCount="1175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4897" uniqueCount="1178">
   <si>
     <t>ID</t>
   </si>
@@ -36406,6 +36406,15 @@
   </si>
   <si>
     <t>personality type is averaged out; description of design is a bit convoluted but it appears it was between-subject</t>
+  </si>
+  <si>
+    <t>2(personality type: extravert vs introvert) x 2 (background: music, silence)</t>
+  </si>
+  <si>
+    <t>although not explicitly mentioned, it appears the design was between-subject; there was a short chat in the music file</t>
+  </si>
+  <si>
+    <t>2(personality type: extravert vs introvert) x 3 (background:  instrumental, vocal music, silence)</t>
   </si>
 </sst>
 </file>
@@ -37446,9 +37455,6 @@
     <xf numFmtId="0" fontId="50" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="41" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -37460,6 +37466,9 @@
     </xf>
     <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -37806,7 +37815,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -49592,14 +49601,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="157"/>
-      <c r="B1" s="157"/>
-      <c r="C1" s="157"/>
-      <c r="D1" s="157"/>
-      <c r="E1" s="157"/>
-      <c r="F1" s="157"/>
-      <c r="G1" s="157"/>
-      <c r="H1" s="157"/>
+      <c r="A1" s="161"/>
+      <c r="B1" s="161"/>
+      <c r="C1" s="161"/>
+      <c r="D1" s="161"/>
+      <c r="E1" s="161"/>
+      <c r="F1" s="161"/>
+      <c r="G1" s="161"/>
+      <c r="H1" s="161"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -62930,8 +62939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -63368,7 +63377,7 @@
       <c r="E21" s="58" t="s">
         <v>1135</v>
       </c>
-      <c r="F21" s="159" t="s">
+      <c r="F21" s="158" t="s">
         <v>1165</v>
       </c>
       <c r="G21" s="47" t="s">
@@ -63400,7 +63409,7 @@
       <c r="A23" s="58">
         <v>21</v>
       </c>
-      <c r="B23" s="160" t="s">
+      <c r="B23" s="159" t="s">
         <v>1170</v>
       </c>
       <c r="C23" s="47" t="s">
@@ -63412,7 +63421,7 @@
       <c r="E23" s="58" t="s">
         <v>1135</v>
       </c>
-      <c r="F23" s="161" t="s">
+      <c r="F23" s="160" t="s">
         <v>1172</v>
       </c>
       <c r="G23" s="12" t="s">
@@ -63442,40 +63451,54 @@
         <v>479</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="47"/>
+    <row r="25" spans="1:7" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="58">
+        <v>23</v>
+      </c>
       <c r="B25" s="144" t="s">
-        <v>863</v>
+        <v>924</v>
       </c>
       <c r="C25" s="47" t="s">
         <v>320</v>
       </c>
-      <c r="D25" s="47"/>
-      <c r="E25" s="47" t="s">
+      <c r="D25" s="61" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E25" s="58" t="s">
+        <v>1135</v>
+      </c>
+      <c r="F25" s="61" t="s">
+        <v>1176</v>
+      </c>
+      <c r="G25" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F25" s="43"/>
-      <c r="G25" s="47"/>
-    </row>
-    <row r="26" spans="1:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="47"/>
+    </row>
+    <row r="26" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="47">
+        <v>24</v>
+      </c>
       <c r="B26" s="144" t="s">
-        <v>877</v>
+        <v>928</v>
       </c>
       <c r="C26" s="47" t="s">
         <v>320</v>
       </c>
-      <c r="D26" s="47"/>
+      <c r="D26" s="61" t="s">
+        <v>1177</v>
+      </c>
       <c r="E26" s="47" t="s">
         <v>479</v>
       </c>
       <c r="F26" s="43"/>
       <c r="G26" s="47"/>
     </row>
-    <row r="27" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A27" s="47"/>
+    <row r="27" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="47">
+        <v>25</v>
+      </c>
       <c r="B27" s="144" t="s">
-        <v>889</v>
+        <v>925</v>
       </c>
       <c r="C27" s="47" t="s">
         <v>320</v>
@@ -63487,10 +63510,10 @@
       <c r="F27" s="43"/>
       <c r="G27" s="47"/>
     </row>
-    <row r="28" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="47"/>
       <c r="B28" s="144" t="s">
-        <v>894</v>
+        <v>863</v>
       </c>
       <c r="C28" s="47" t="s">
         <v>320</v>
@@ -63499,15 +63522,13 @@
       <c r="E28" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F28" s="47" t="s">
-        <v>1121</v>
-      </c>
+      <c r="F28" s="43"/>
       <c r="G28" s="47"/>
     </row>
-    <row r="29" spans="1:7" ht="39" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="47"/>
       <c r="B29" s="144" t="s">
-        <v>895</v>
+        <v>877</v>
       </c>
       <c r="C29" s="47" t="s">
         <v>320</v>
@@ -63519,10 +63540,10 @@
       <c r="F29" s="43"/>
       <c r="G29" s="47"/>
     </row>
-    <row r="30" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="39" x14ac:dyDescent="0.25">
       <c r="A30" s="47"/>
-      <c r="B30" s="145" t="s">
-        <v>906</v>
+      <c r="B30" s="144" t="s">
+        <v>889</v>
       </c>
       <c r="C30" s="47" t="s">
         <v>320</v>
@@ -63536,8 +63557,8 @@
     </row>
     <row r="31" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="47"/>
-      <c r="B31" s="146" t="s">
-        <v>724</v>
+      <c r="B31" s="144" t="s">
+        <v>894</v>
       </c>
       <c r="C31" s="47" t="s">
         <v>320</v>
@@ -63546,15 +63567,15 @@
       <c r="E31" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F31" s="53" t="s">
-        <v>1123</v>
-      </c>
-      <c r="G31" s="61"/>
-    </row>
-    <row r="32" spans="1:7" ht="39" x14ac:dyDescent="0.25">
+      <c r="F31" s="47" t="s">
+        <v>1121</v>
+      </c>
+      <c r="G31" s="47"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="47"/>
       <c r="B32" s="144" t="s">
-        <v>363</v>
+        <v>895</v>
       </c>
       <c r="C32" s="47" t="s">
         <v>320</v>
@@ -63566,10 +63587,10 @@
       <c r="F32" s="43"/>
       <c r="G32" s="47"/>
     </row>
-    <row r="33" spans="1:7" ht="39" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" s="47"/>
-      <c r="B33" s="148" t="s">
-        <v>721</v>
+      <c r="B33" s="145" t="s">
+        <v>906</v>
       </c>
       <c r="C33" s="47" t="s">
         <v>320</v>
@@ -63578,15 +63599,13 @@
       <c r="E33" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F33" s="53" t="s">
-        <v>1125</v>
-      </c>
-      <c r="G33" s="61"/>
+      <c r="F33" s="43"/>
+      <c r="G33" s="47"/>
     </row>
     <row r="34" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="47"/>
-      <c r="B34" s="145" t="s">
-        <v>921</v>
+      <c r="B34" s="146" t="s">
+        <v>724</v>
       </c>
       <c r="C34" s="47" t="s">
         <v>320</v>
@@ -63595,13 +63614,15 @@
       <c r="E34" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F34" s="43"/>
-      <c r="G34" s="47"/>
+      <c r="F34" s="53" t="s">
+        <v>1123</v>
+      </c>
+      <c r="G34" s="61"/>
     </row>
     <row r="35" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="47"/>
       <c r="B35" s="144" t="s">
-        <v>924</v>
+        <v>363</v>
       </c>
       <c r="C35" s="47" t="s">
         <v>320</v>
@@ -63615,8 +63636,8 @@
     </row>
     <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="47"/>
-      <c r="B36" s="144" t="s">
-        <v>925</v>
+      <c r="B36" s="148" t="s">
+        <v>721</v>
       </c>
       <c r="C36" s="47" t="s">
         <v>320</v>
@@ -63625,13 +63646,15 @@
       <c r="E36" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F36" s="43"/>
-      <c r="G36" s="47"/>
-    </row>
-    <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="F36" s="53" t="s">
+        <v>1125</v>
+      </c>
+      <c r="G36" s="61"/>
+    </row>
+    <row r="37" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="47"/>
-      <c r="B37" s="144" t="s">
-        <v>928</v>
+      <c r="B37" s="145" t="s">
+        <v>921</v>
       </c>
       <c r="C37" s="47" t="s">
         <v>320</v>
@@ -63707,7 +63730,7 @@
       </c>
       <c r="G41" s="61"/>
     </row>
-    <row r="42" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="47"/>
       <c r="B42" s="144" t="s">
         <v>969</v>
@@ -63874,7 +63897,7 @@
       <c r="F52" s="43"/>
       <c r="G52" s="47"/>
     </row>
-    <row r="53" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A53" s="47"/>
       <c r="B53" s="146" t="s">
         <v>328</v>
@@ -63891,7 +63914,7 @@
       </c>
       <c r="G53" s="61"/>
     </row>
-    <row r="54" spans="1:7" ht="39" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" s="47"/>
       <c r="B54" s="144" t="s">
         <v>1039</v>
@@ -63906,7 +63929,7 @@
       <c r="F54" s="43"/>
       <c r="G54" s="47"/>
     </row>
-    <row r="55" spans="1:7" ht="39" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="47"/>
       <c r="B55" s="144" t="s">
         <v>1077</v>
@@ -63921,7 +63944,7 @@
       <c r="F55" s="43"/>
       <c r="G55" s="47"/>
     </row>
-    <row r="56" spans="1:7" ht="39" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A56" s="47"/>
       <c r="B56" s="146" t="s">
         <v>726</v>
@@ -63938,7 +63961,7 @@
       </c>
       <c r="G56" s="47"/>
     </row>
-    <row r="57" spans="1:7" ht="39" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A57" s="47"/>
       <c r="B57" s="145" t="s">
         <v>867</v>
@@ -63953,7 +63976,7 @@
       <c r="F57" s="43"/>
       <c r="G57" s="47"/>
     </row>
-    <row r="58" spans="1:7" ht="39" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="47"/>
       <c r="B58" s="145" t="s">
         <v>879</v>
@@ -64015,7 +64038,7 @@
       <c r="F61" s="43"/>
       <c r="G61" s="47"/>
     </row>
-    <row r="62" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" ht="39" x14ac:dyDescent="0.25">
       <c r="A62" s="47"/>
       <c r="B62" s="145" t="s">
         <v>904</v>
@@ -64030,7 +64053,7 @@
       <c r="F62" s="43"/>
       <c r="G62" s="47"/>
     </row>
-    <row r="63" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="47"/>
       <c r="B63" s="147" t="s">
         <v>90</v>
@@ -64075,7 +64098,7 @@
       <c r="F65" s="43"/>
       <c r="G65" s="47"/>
     </row>
-    <row r="66" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A66" s="47"/>
       <c r="B66" s="149" t="s">
         <v>82</v>
@@ -64090,7 +64113,7 @@
       <c r="F66" s="43"/>
       <c r="G66" s="47"/>
     </row>
-    <row r="67" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="47"/>
       <c r="B67" s="144" t="s">
         <v>81</v>
@@ -64135,7 +64158,7 @@
       <c r="F69" s="43"/>
       <c r="G69" s="47"/>
     </row>
-    <row r="70" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A70" s="47"/>
       <c r="B70" s="145" t="s">
         <v>935</v>
@@ -64150,7 +64173,7 @@
       <c r="F70" s="43"/>
       <c r="G70" s="47"/>
     </row>
-    <row r="71" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" ht="39" x14ac:dyDescent="0.25">
       <c r="A71" s="47"/>
       <c r="B71" s="149" t="s">
         <v>940</v>
@@ -64165,7 +64188,7 @@
       <c r="F71" s="43"/>
       <c r="G71" s="47"/>
     </row>
-    <row r="72" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" ht="39" x14ac:dyDescent="0.25">
       <c r="A72" s="47"/>
       <c r="B72" s="145" t="s">
         <v>941</v>
@@ -64180,7 +64203,7 @@
       <c r="F72" s="43"/>
       <c r="G72" s="47"/>
     </row>
-    <row r="73" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" ht="39" x14ac:dyDescent="0.25">
       <c r="A73" s="47"/>
       <c r="B73" s="149" t="s">
         <v>942</v>
@@ -64210,7 +64233,7 @@
       <c r="F74" s="43"/>
       <c r="G74" s="47"/>
     </row>
-    <row r="75" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" ht="39" x14ac:dyDescent="0.25">
       <c r="A75" s="47"/>
       <c r="B75" s="145" t="s">
         <v>944</v>
@@ -64225,7 +64248,7 @@
       <c r="F75" s="43"/>
       <c r="G75" s="47"/>
     </row>
-    <row r="76" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A76" s="47"/>
       <c r="B76" s="146" t="s">
         <v>737</v>
@@ -64240,7 +64263,7 @@
       <c r="F76" s="43"/>
       <c r="G76" s="47"/>
     </row>
-    <row r="77" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A77" s="47"/>
       <c r="B77" s="145" t="s">
         <v>959</v>
@@ -64255,7 +64278,7 @@
       <c r="F77" s="43"/>
       <c r="G77" s="47"/>
     </row>
-    <row r="78" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="47"/>
       <c r="B78" s="144" t="s">
         <v>960</v>
@@ -64330,7 +64353,7 @@
       <c r="F82" s="43"/>
       <c r="G82" s="47"/>
     </row>
-    <row r="83" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A83" s="47"/>
       <c r="B83" s="145" t="s">
         <v>994</v>
@@ -64345,7 +64368,7 @@
       <c r="F83" s="43"/>
       <c r="G83" s="47"/>
     </row>
-    <row r="84" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" ht="39" x14ac:dyDescent="0.25">
       <c r="A84" s="47"/>
       <c r="B84" s="149" t="s">
         <v>139</v>
@@ -64360,7 +64383,7 @@
       <c r="F84" s="43"/>
       <c r="G84" s="47"/>
     </row>
-    <row r="85" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A85" s="47"/>
       <c r="B85" s="149" t="s">
         <v>1005</v>
@@ -64405,7 +64428,7 @@
       <c r="F87" s="43"/>
       <c r="G87" s="47"/>
     </row>
-    <row r="88" spans="1:7" ht="39" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" s="47"/>
       <c r="B88" s="144" t="s">
         <v>58</v>
@@ -64420,7 +64443,7 @@
       <c r="F88" s="43"/>
       <c r="G88" s="47"/>
     </row>
-    <row r="89" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="47"/>
       <c r="B89" s="144" t="s">
         <v>96</v>
@@ -64435,7 +64458,7 @@
       <c r="F89" s="43"/>
       <c r="G89" s="47"/>
     </row>
-    <row r="90" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" ht="39" x14ac:dyDescent="0.25">
       <c r="A90" s="47"/>
       <c r="B90" s="145" t="s">
         <v>1057</v>
@@ -64450,7 +64473,7 @@
       <c r="F90" s="43"/>
       <c r="G90" s="47"/>
     </row>
-    <row r="91" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A91" s="46"/>
       <c r="B91" s="133" t="s">
         <v>68</v>
@@ -64463,7 +64486,7 @@
       <c r="F91" s="32"/>
       <c r="G91" s="46"/>
     </row>
-    <row r="92" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A92" s="47"/>
       <c r="B92" s="144" t="s">
         <v>69</v>
@@ -64600,7 +64623,7 @@
       <c r="F100" s="43"/>
       <c r="G100" s="47"/>
     </row>
-    <row r="101" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="47"/>
       <c r="B101" s="144" t="s">
         <v>80</v>
@@ -64615,7 +64638,7 @@
       <c r="F101" s="43"/>
       <c r="G101" s="47"/>
     </row>
-    <row r="102" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A102" s="47"/>
       <c r="B102" s="154" t="s">
         <v>137</v>
@@ -64705,7 +64728,7 @@
       <c r="F107" s="43"/>
       <c r="G107" s="47"/>
     </row>
-    <row r="108" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A108" s="47"/>
       <c r="B108" s="144" t="s">
         <v>775</v>
@@ -64735,7 +64758,7 @@
       <c r="F109" s="43"/>
       <c r="G109" s="47"/>
     </row>
-    <row r="110" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="47"/>
       <c r="B110" s="153" t="s">
         <v>781</v>
@@ -64750,7 +64773,7 @@
       <c r="F110" s="43"/>
       <c r="G110" s="47"/>
     </row>
-    <row r="111" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A111" s="47"/>
       <c r="B111" s="144" t="s">
         <v>753</v>
@@ -64780,7 +64803,7 @@
       <c r="F112" s="43"/>
       <c r="G112" s="47"/>
     </row>
-    <row r="113" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A113" s="47"/>
       <c r="B113" s="145" t="s">
         <v>768</v>
@@ -64797,7 +64820,7 @@
       </c>
       <c r="G113" s="47"/>
     </row>
-    <row r="114" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" ht="39" x14ac:dyDescent="0.25">
       <c r="A114" s="47"/>
       <c r="B114" s="145" t="s">
         <v>866</v>
@@ -64872,7 +64895,7 @@
       <c r="F118" s="43"/>
       <c r="G118" s="47"/>
     </row>
-    <row r="119" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" ht="39" x14ac:dyDescent="0.25">
       <c r="A119" s="47"/>
       <c r="B119" s="145" t="s">
         <v>939</v>
@@ -64917,7 +64940,7 @@
       <c r="F121" s="43"/>
       <c r="G121" s="47"/>
     </row>
-    <row r="122" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A122" s="47"/>
       <c r="B122" s="145" t="s">
         <v>962</v>
@@ -64966,7 +64989,7 @@
     </row>
     <row r="125" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A125" s="46"/>
-      <c r="B125" s="158" t="s">
+      <c r="B125" s="157" t="s">
         <v>988</v>
       </c>
       <c r="C125" s="46" t="s">
@@ -64981,7 +65004,7 @@
       </c>
       <c r="G125" s="46"/>
     </row>
-    <row r="126" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A126" s="47"/>
       <c r="B126" s="145" t="s">
         <v>1004</v>
@@ -65041,7 +65064,7 @@
       <c r="F129" s="43"/>
       <c r="G129" s="47"/>
     </row>
-    <row r="130" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A130" s="47"/>
       <c r="B130" s="145" t="s">
         <v>1101</v>

</xml_diff>

<commit_message>
changed to effect sizes and more data
</commit_message>
<xml_diff>
--- a/Literature_search/database.xlsx
+++ b/Literature_search/database.xlsx
@@ -22,7 +22,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">' Step 2'!$A$2:$D$526</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">' Step 3'!$A$2:$C$344</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">' Step 4 (meta)'!$A$2:$C$119</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">' Step 4 (meta)'!$A$2:$C$120</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -316,7 +316,83 @@
         </r>
       </text>
     </comment>
-    <comment ref="B84" authorId="1">
+    <comment ref="G60" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Martin,Vasilev:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+- participants adjusted the volume of the music on their own. Therefore, the music level was different for the different subjects
+- the experiment was conducted in a busy university cafeteria, which is a naturally noisy place. In this sense, this confounds the actual music manipulation. Also, in the silence condition, participants will still hear the background noise from the cafeteria. 
+For these reasons, the experiment is not similar to the remaining studies and cannot be included in the meta-analysis
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B62" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Martin,Vasilev:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Exp. 3 only had an arithmetic task
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F63" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Martin,Vasilev:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+response time is not coded as it has a different meaning that reading speed and there are not enough studies for this particular analysis</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B90" authorId="1">
       <text>
         <r>
           <rPr>
@@ -415,7 +491,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4937" uniqueCount="1244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4957" uniqueCount="1260">
   <si>
     <t>ID</t>
   </si>
@@ -36734,13 +36810,139 @@
   </si>
   <si>
     <t>study investigated reverbation times of classrooms, and not experimental/ long-term exposure to noise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 (background: silence, industrial noise, music, speech) </t>
+  </si>
+  <si>
+    <t>not much time passed until reading comprehension assessment due to the fact that passages were very short (around 80 words).</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2 (background: startling music, non-startling music)</t>
+  </si>
+  <si>
+    <t>3 (background: no muisc, fast classical music, slow classical music)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 (background: silence, office noise /w speech, office noise without speech, speech) </t>
+  </si>
+  <si>
+    <t>the task was about learning material rather than reading per se</t>
+  </si>
+  <si>
+    <t>4 (background: silence, Greek speech, office noise with speech, office noise without speech speech) x 2 (background exposure: learning phase, learning &amp; recall phase)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Banbury, S., &amp; Berry, D. C. (1998). Disruption of office‐related tasks by speech and office noise. British Journal of Psychology, 89(3), 499-517., </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Experiment 1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Banbury, S., &amp; Berry, D. C. (1998). Disruption of office‐related tasks by speech and office noise. British Journal of Psychology, 89(3), 499-517., </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Experiment 2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Banbury, S., &amp; Berry, D. C. (1997). Habituation and dishabituation to speech and office noise. Journal of Experimental Psychology: Applied, 3(3), 181., </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Experiment 1</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2 (background: noise, silence)</t>
+  </si>
+  <si>
+    <t>I convert proportion wrong to proportion correct, and variances to standard deviations; I take the average of the two texts</t>
+  </si>
+  <si>
+    <t>very poor reporting of design and materials; not clear what the task measures are</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2 (background: silence, speech)</t>
+  </si>
+  <si>
+    <t>effect sizes were computed/ approximated from the available F statistics (see R files)</t>
+  </si>
+  <si>
+    <r>
+      <t>Martin, R. C., Wogalter, M. S., &amp; Forlano, J. G. (1988). Reading comprehension in the presence of unattended speech and music. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Journal of memory and language</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>27</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(4), 382-398., </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Experiment 1</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="63" x14ac:knownFonts="1">
+  <fonts count="64" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -37189,6 +37391,12 @@
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -38135,7 +38343,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -63289,10 +63497,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G120"/>
+  <dimension ref="A1:G121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -64516,7 +64724,7 @@
       </c>
     </row>
     <row r="58" spans="1:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="47">
+      <c r="A58" s="58">
         <v>56</v>
       </c>
       <c r="B58" s="144" t="s">
@@ -64525,116 +64733,158 @@
       <c r="C58" s="47" t="s">
         <v>554</v>
       </c>
-      <c r="D58" s="47"/>
-      <c r="E58" s="47" t="s">
+      <c r="D58" s="61" t="s">
+        <v>1244</v>
+      </c>
+      <c r="E58" s="46" t="s">
+        <v>1134</v>
+      </c>
+      <c r="F58" s="43"/>
+      <c r="G58" s="61" t="s">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="58">
+        <v>57</v>
+      </c>
+      <c r="B59" s="145" t="s">
+        <v>1035</v>
+      </c>
+      <c r="C59" s="47" t="s">
+        <v>320</v>
+      </c>
+      <c r="D59" s="61" t="s">
+        <v>1246</v>
+      </c>
+      <c r="E59" s="46" t="s">
+        <v>1134</v>
+      </c>
+      <c r="F59" s="61" t="s">
+        <v>1245</v>
+      </c>
+      <c r="G59" s="47" t="s">
+        <v>1172</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="58">
+        <v>58</v>
+      </c>
+      <c r="B60" s="145" t="s">
+        <v>969</v>
+      </c>
+      <c r="C60" s="47" t="s">
+        <v>320</v>
+      </c>
+      <c r="D60" s="62" t="s">
+        <v>1247</v>
+      </c>
+      <c r="E60" s="46" t="s">
+        <v>1134</v>
+      </c>
+      <c r="F60" s="43"/>
+      <c r="G60" s="47" t="s">
+        <v>1196</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="58">
+        <v>59</v>
+      </c>
+      <c r="B61" s="152" t="s">
+        <v>1251</v>
+      </c>
+      <c r="C61" s="47" t="s">
+        <v>554</v>
+      </c>
+      <c r="D61" s="61" t="s">
+        <v>1248</v>
+      </c>
+      <c r="E61" s="46" t="s">
+        <v>1134</v>
+      </c>
+      <c r="F61" s="43"/>
+      <c r="G61" s="61" t="s">
+        <v>1249</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="58">
+        <v>60</v>
+      </c>
+      <c r="B62" s="152" t="s">
+        <v>1252</v>
+      </c>
+      <c r="C62" s="47" t="s">
+        <v>554</v>
+      </c>
+      <c r="D62" s="61" t="s">
+        <v>1250</v>
+      </c>
+      <c r="E62" s="46" t="s">
+        <v>1134</v>
+      </c>
+      <c r="F62" s="43"/>
+      <c r="G62" s="61" t="s">
+        <v>1249</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="58">
+        <v>61</v>
+      </c>
+      <c r="B63" s="158" t="s">
+        <v>1084</v>
+      </c>
+      <c r="C63" s="47" t="s">
+        <v>282</v>
+      </c>
+      <c r="D63" s="61" t="s">
+        <v>1254</v>
+      </c>
+      <c r="E63" s="58" t="s">
+        <v>1127</v>
+      </c>
+      <c r="F63" s="61" t="s">
+        <v>1255</v>
+      </c>
+      <c r="G63" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F58" s="43"/>
-      <c r="G58" s="47"/>
-    </row>
-    <row r="59" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="47">
-        <v>57</v>
-      </c>
-      <c r="B59" s="159" t="s">
-        <v>781</v>
-      </c>
-      <c r="C59" s="47" t="s">
-        <v>798</v>
-      </c>
-      <c r="D59" s="47"/>
-      <c r="E59" s="47" t="s">
+    </row>
+    <row r="64" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="58">
+        <v>62</v>
+      </c>
+      <c r="B64" s="152" t="s">
+        <v>1085</v>
+      </c>
+      <c r="C64" s="47" t="s">
+        <v>282</v>
+      </c>
+      <c r="D64" s="61" t="s">
+        <v>1257</v>
+      </c>
+      <c r="E64" s="58" t="s">
+        <v>1127</v>
+      </c>
+      <c r="F64" s="65" t="s">
+        <v>1258</v>
+      </c>
+      <c r="G64" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F59" s="61" t="s">
-        <v>1232</v>
-      </c>
-      <c r="G59" s="47"/>
-    </row>
-    <row r="60" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="47"/>
-      <c r="B60" s="152" t="s">
-        <v>904</v>
-      </c>
-      <c r="C60" s="47" t="s">
-        <v>320</v>
-      </c>
-      <c r="D60" s="47"/>
-      <c r="E60" s="47" t="s">
-        <v>479</v>
-      </c>
-      <c r="F60" s="43"/>
-      <c r="G60" s="47"/>
-    </row>
-    <row r="61" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A61" s="47"/>
-      <c r="B61" s="145" t="s">
-        <v>923</v>
-      </c>
-      <c r="C61" s="47" t="s">
-        <v>320</v>
-      </c>
-      <c r="D61" s="47"/>
-      <c r="E61" s="47" t="s">
-        <v>479</v>
-      </c>
-      <c r="F61" s="43"/>
-      <c r="G61" s="47"/>
-    </row>
-    <row r="62" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="47"/>
-      <c r="B62" s="145" t="s">
-        <v>945</v>
-      </c>
-      <c r="C62" s="47" t="s">
-        <v>320</v>
-      </c>
-      <c r="D62" s="47"/>
-      <c r="E62" s="47" t="s">
-        <v>479</v>
-      </c>
-      <c r="F62" s="61" t="s">
-        <v>1155</v>
-      </c>
-      <c r="G62" s="47"/>
-    </row>
-    <row r="63" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="47"/>
-      <c r="B63" s="145" t="s">
-        <v>969</v>
-      </c>
-      <c r="C63" s="47" t="s">
-        <v>320</v>
-      </c>
-      <c r="D63" s="47"/>
-      <c r="E63" s="47" t="s">
-        <v>479</v>
-      </c>
-      <c r="F63" s="43"/>
-      <c r="G63" s="47"/>
-    </row>
-    <row r="64" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="47"/>
-      <c r="B64" s="152" t="s">
-        <v>1011</v>
-      </c>
-      <c r="C64" s="47" t="s">
-        <v>320</v>
-      </c>
-      <c r="D64" s="47"/>
-      <c r="E64" s="47" t="s">
-        <v>479</v>
-      </c>
-      <c r="F64" s="43"/>
-      <c r="G64" s="47"/>
-    </row>
-    <row r="65" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="47"/>
-      <c r="B65" s="145" t="s">
-        <v>1029</v>
+    </row>
+    <row r="65" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="47">
+        <v>63</v>
+      </c>
+      <c r="B65" s="152" t="s">
+        <v>1259</v>
       </c>
       <c r="C65" s="47" t="s">
-        <v>320</v>
+        <v>554</v>
       </c>
       <c r="D65" s="47"/>
       <c r="E65" s="47" t="s">
@@ -64643,13 +64893,15 @@
       <c r="F65" s="43"/>
       <c r="G65" s="47"/>
     </row>
-    <row r="66" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="47"/>
-      <c r="B66" s="145" t="s">
-        <v>1030</v>
+    <row r="66" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="47">
+        <v>64</v>
+      </c>
+      <c r="B66" s="152" t="s">
+        <v>1253</v>
       </c>
       <c r="C66" s="47" t="s">
-        <v>320</v>
+        <v>554</v>
       </c>
       <c r="D66" s="47"/>
       <c r="E66" s="47" t="s">
@@ -64658,28 +64910,32 @@
       <c r="F66" s="43"/>
       <c r="G66" s="47"/>
     </row>
-    <row r="67" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="47"/>
-      <c r="B67" s="145" t="s">
-        <v>1035</v>
+    <row r="67" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="47">
+        <v>65</v>
+      </c>
+      <c r="B67" s="159" t="s">
+        <v>781</v>
       </c>
       <c r="C67" s="47" t="s">
-        <v>320</v>
+        <v>798</v>
       </c>
       <c r="D67" s="47"/>
       <c r="E67" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F67" s="43"/>
+      <c r="F67" s="61" t="s">
+        <v>1232</v>
+      </c>
       <c r="G67" s="47"/>
     </row>
-    <row r="68" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="47"/>
       <c r="B68" s="152" t="s">
-        <v>866</v>
+        <v>904</v>
       </c>
       <c r="C68" s="47" t="s">
-        <v>282</v>
+        <v>320</v>
       </c>
       <c r="D68" s="47"/>
       <c r="E68" s="47" t="s">
@@ -64688,13 +64944,13 @@
       <c r="F68" s="43"/>
       <c r="G68" s="47"/>
     </row>
-    <row r="69" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="47"/>
-      <c r="B69" s="144" t="s">
-        <v>895</v>
+      <c r="B69" s="145" t="s">
+        <v>923</v>
       </c>
       <c r="C69" s="47" t="s">
-        <v>282</v>
+        <v>320</v>
       </c>
       <c r="D69" s="47"/>
       <c r="E69" s="47" t="s">
@@ -64703,28 +64959,30 @@
       <c r="F69" s="43"/>
       <c r="G69" s="47"/>
     </row>
-    <row r="70" spans="1:7" ht="39" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="47"/>
-      <c r="B70" s="152" t="s">
-        <v>900</v>
+      <c r="B70" s="145" t="s">
+        <v>945</v>
       </c>
       <c r="C70" s="47" t="s">
-        <v>282</v>
+        <v>320</v>
       </c>
       <c r="D70" s="47"/>
       <c r="E70" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F70" s="43"/>
+      <c r="F70" s="61" t="s">
+        <v>1155</v>
+      </c>
       <c r="G70" s="47"/>
     </row>
-    <row r="71" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A71" s="47"/>
-      <c r="B71" s="144" t="s">
-        <v>901</v>
+      <c r="B71" s="152" t="s">
+        <v>1011</v>
       </c>
       <c r="C71" s="47" t="s">
-        <v>282</v>
+        <v>320</v>
       </c>
       <c r="D71" s="47"/>
       <c r="E71" s="47" t="s">
@@ -64733,13 +64991,13 @@
       <c r="F71" s="43"/>
       <c r="G71" s="47"/>
     </row>
-    <row r="72" spans="1:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="47"/>
-      <c r="B72" s="146" t="s">
-        <v>90</v>
+      <c r="B72" s="145" t="s">
+        <v>1029</v>
       </c>
       <c r="C72" s="47" t="s">
-        <v>282</v>
+        <v>320</v>
       </c>
       <c r="D72" s="47"/>
       <c r="E72" s="47" t="s">
@@ -64748,25 +65006,25 @@
       <c r="F72" s="43"/>
       <c r="G72" s="47"/>
     </row>
-    <row r="73" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="121"/>
-      <c r="B73" s="142" t="s">
-        <v>55</v>
-      </c>
-      <c r="C73" s="121" t="s">
-        <v>282</v>
-      </c>
-      <c r="D73" s="121"/>
-      <c r="E73" s="121"/>
-      <c r="F73" s="122" t="s">
-        <v>835</v>
-      </c>
-      <c r="G73" s="153"/>
-    </row>
-    <row r="74" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="47"/>
+      <c r="B73" s="145" t="s">
+        <v>1030</v>
+      </c>
+      <c r="C73" s="47" t="s">
+        <v>320</v>
+      </c>
+      <c r="D73" s="47"/>
+      <c r="E73" s="47" t="s">
+        <v>479</v>
+      </c>
+      <c r="F73" s="43"/>
+      <c r="G73" s="47"/>
+    </row>
+    <row r="74" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="47"/>
-      <c r="B74" s="144" t="s">
-        <v>762</v>
+      <c r="B74" s="152" t="s">
+        <v>866</v>
       </c>
       <c r="C74" s="47" t="s">
         <v>282</v>
@@ -64778,10 +65036,10 @@
       <c r="F74" s="43"/>
       <c r="G74" s="47"/>
     </row>
-    <row r="75" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="47"/>
-      <c r="B75" s="51" t="s">
-        <v>82</v>
+      <c r="B75" s="144" t="s">
+        <v>895</v>
       </c>
       <c r="C75" s="47" t="s">
         <v>282</v>
@@ -64793,10 +65051,10 @@
       <c r="F75" s="43"/>
       <c r="G75" s="47"/>
     </row>
-    <row r="76" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="47"/>
-      <c r="B76" s="143" t="s">
-        <v>81</v>
+      <c r="B76" s="152" t="s">
+        <v>900</v>
       </c>
       <c r="C76" s="47" t="s">
         <v>282</v>
@@ -64808,10 +65066,10 @@
       <c r="F76" s="43"/>
       <c r="G76" s="47"/>
     </row>
-    <row r="77" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="47"/>
-      <c r="B77" s="158" t="s">
-        <v>929</v>
+      <c r="B77" s="144" t="s">
+        <v>901</v>
       </c>
       <c r="C77" s="47" t="s">
         <v>282</v>
@@ -64823,10 +65081,10 @@
       <c r="F77" s="43"/>
       <c r="G77" s="47"/>
     </row>
-    <row r="78" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="47"/>
-      <c r="B78" s="152" t="s">
-        <v>933</v>
+      <c r="B78" s="146" t="s">
+        <v>90</v>
       </c>
       <c r="C78" s="47" t="s">
         <v>282</v>
@@ -64838,25 +65096,25 @@
       <c r="F78" s="43"/>
       <c r="G78" s="47"/>
     </row>
-    <row r="79" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="47"/>
-      <c r="B79" s="51" t="s">
-        <v>938</v>
-      </c>
-      <c r="C79" s="47" t="s">
-        <v>282</v>
-      </c>
-      <c r="D79" s="47"/>
-      <c r="E79" s="47" t="s">
-        <v>479</v>
-      </c>
-      <c r="F79" s="43"/>
-      <c r="G79" s="47"/>
-    </row>
-    <row r="80" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="121"/>
+      <c r="B79" s="142" t="s">
+        <v>55</v>
+      </c>
+      <c r="C79" s="121" t="s">
+        <v>282</v>
+      </c>
+      <c r="D79" s="121"/>
+      <c r="E79" s="121"/>
+      <c r="F79" s="122" t="s">
+        <v>835</v>
+      </c>
+      <c r="G79" s="153"/>
+    </row>
+    <row r="80" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="47"/>
-      <c r="B80" s="152" t="s">
-        <v>939</v>
+      <c r="B80" s="144" t="s">
+        <v>762</v>
       </c>
       <c r="C80" s="47" t="s">
         <v>282</v>
@@ -64868,10 +65126,10 @@
       <c r="F80" s="43"/>
       <c r="G80" s="47"/>
     </row>
-    <row r="81" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="47"/>
       <c r="B81" s="51" t="s">
-        <v>940</v>
+        <v>82</v>
       </c>
       <c r="C81" s="47" t="s">
         <v>282</v>
@@ -64883,10 +65141,10 @@
       <c r="F81" s="43"/>
       <c r="G81" s="47"/>
     </row>
-    <row r="82" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="47"/>
-      <c r="B82" s="51" t="s">
-        <v>941</v>
+      <c r="B82" s="145" t="s">
+        <v>81</v>
       </c>
       <c r="C82" s="47" t="s">
         <v>282</v>
@@ -64898,10 +65156,10 @@
       <c r="F82" s="43"/>
       <c r="G82" s="47"/>
     </row>
-    <row r="83" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="47"/>
-      <c r="B83" s="152" t="s">
-        <v>942</v>
+      <c r="B83" s="158" t="s">
+        <v>929</v>
       </c>
       <c r="C83" s="47" t="s">
         <v>282</v>
@@ -64913,10 +65171,10 @@
       <c r="F83" s="43"/>
       <c r="G83" s="47"/>
     </row>
-    <row r="84" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="47"/>
-      <c r="B84" s="145" t="s">
-        <v>737</v>
+      <c r="B84" s="152" t="s">
+        <v>933</v>
       </c>
       <c r="C84" s="47" t="s">
         <v>282</v>
@@ -64928,10 +65186,10 @@
       <c r="F84" s="43"/>
       <c r="G84" s="47"/>
     </row>
-    <row r="85" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="47"/>
-      <c r="B85" s="152" t="s">
-        <v>957</v>
+      <c r="B85" s="51" t="s">
+        <v>938</v>
       </c>
       <c r="C85" s="47" t="s">
         <v>282</v>
@@ -64943,10 +65201,10 @@
       <c r="F85" s="43"/>
       <c r="G85" s="47"/>
     </row>
-    <row r="86" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="47"/>
-      <c r="B86" s="145" t="s">
-        <v>958</v>
+      <c r="B86" s="152" t="s">
+        <v>939</v>
       </c>
       <c r="C86" s="47" t="s">
         <v>282</v>
@@ -64958,10 +65216,10 @@
       <c r="F86" s="43"/>
       <c r="G86" s="47"/>
     </row>
-    <row r="87" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="47"/>
-      <c r="B87" s="152" t="s">
-        <v>964</v>
+      <c r="B87" s="51" t="s">
+        <v>940</v>
       </c>
       <c r="C87" s="47" t="s">
         <v>282</v>
@@ -64973,10 +65231,10 @@
       <c r="F87" s="43"/>
       <c r="G87" s="47"/>
     </row>
-    <row r="88" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A88" s="47"/>
-      <c r="B88" s="144" t="s">
-        <v>991</v>
+      <c r="B88" s="51" t="s">
+        <v>941</v>
       </c>
       <c r="C88" s="47" t="s">
         <v>282</v>
@@ -64988,10 +65246,10 @@
       <c r="F88" s="43"/>
       <c r="G88" s="47"/>
     </row>
-    <row r="89" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="47"/>
-      <c r="B89" s="148" t="s">
-        <v>139</v>
+      <c r="B89" s="152" t="s">
+        <v>942</v>
       </c>
       <c r="C89" s="47" t="s">
         <v>282</v>
@@ -65003,10 +65261,10 @@
       <c r="F89" s="43"/>
       <c r="G89" s="47"/>
     </row>
-    <row r="90" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="47"/>
-      <c r="B90" s="148" t="s">
-        <v>1002</v>
+      <c r="B90" s="145" t="s">
+        <v>737</v>
       </c>
       <c r="C90" s="47" t="s">
         <v>282</v>
@@ -65018,10 +65276,10 @@
       <c r="F90" s="43"/>
       <c r="G90" s="47"/>
     </row>
-    <row r="91" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="47"/>
-      <c r="B91" s="51" t="s">
-        <v>88</v>
+      <c r="B91" s="152" t="s">
+        <v>957</v>
       </c>
       <c r="C91" s="47" t="s">
         <v>282</v>
@@ -65033,10 +65291,10 @@
       <c r="F91" s="43"/>
       <c r="G91" s="47"/>
     </row>
-    <row r="92" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="47"/>
-      <c r="B92" s="148" t="s">
-        <v>1021</v>
+      <c r="B92" s="145" t="s">
+        <v>958</v>
       </c>
       <c r="C92" s="47" t="s">
         <v>282</v>
@@ -65048,10 +65306,10 @@
       <c r="F92" s="43"/>
       <c r="G92" s="47"/>
     </row>
-    <row r="93" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="47"/>
-      <c r="B93" s="145" t="s">
-        <v>58</v>
+      <c r="B93" s="152" t="s">
+        <v>964</v>
       </c>
       <c r="C93" s="47" t="s">
         <v>282</v>
@@ -65063,10 +65321,10 @@
       <c r="F93" s="43"/>
       <c r="G93" s="47"/>
     </row>
-    <row r="94" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="47"/>
-      <c r="B94" s="144" t="s">
-        <v>1053</v>
+      <c r="B94" s="152" t="s">
+        <v>991</v>
       </c>
       <c r="C94" s="47" t="s">
         <v>282</v>
@@ -65078,10 +65336,10 @@
       <c r="F94" s="43"/>
       <c r="G94" s="47"/>
     </row>
-    <row r="95" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="47"/>
-      <c r="B95" s="145" t="s">
-        <v>69</v>
+      <c r="B95" s="51" t="s">
+        <v>139</v>
       </c>
       <c r="C95" s="47" t="s">
         <v>282</v>
@@ -65093,10 +65351,10 @@
       <c r="F95" s="43"/>
       <c r="G95" s="47"/>
     </row>
-    <row r="96" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="47"/>
       <c r="B96" s="51" t="s">
-        <v>1054</v>
+        <v>1002</v>
       </c>
       <c r="C96" s="47" t="s">
         <v>282</v>
@@ -65108,10 +65366,10 @@
       <c r="F96" s="43"/>
       <c r="G96" s="47"/>
     </row>
-    <row r="97" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A97" s="47"/>
-      <c r="B97" s="148" t="s">
-        <v>1066</v>
+      <c r="B97" s="51" t="s">
+        <v>88</v>
       </c>
       <c r="C97" s="47" t="s">
         <v>282</v>
@@ -65123,10 +65381,10 @@
       <c r="F97" s="43"/>
       <c r="G97" s="47"/>
     </row>
-    <row r="98" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="47"/>
-      <c r="B98" s="152" t="s">
-        <v>188</v>
+      <c r="B98" s="148" t="s">
+        <v>1021</v>
       </c>
       <c r="C98" s="47" t="s">
         <v>282</v>
@@ -65135,15 +65393,13 @@
       <c r="E98" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F98" s="47" t="s">
-        <v>848</v>
-      </c>
+      <c r="F98" s="43"/>
       <c r="G98" s="47"/>
     </row>
-    <row r="99" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="47"/>
-      <c r="B99" s="158" t="s">
-        <v>1084</v>
+      <c r="B99" s="145" t="s">
+        <v>58</v>
       </c>
       <c r="C99" s="47" t="s">
         <v>282</v>
@@ -65155,10 +65411,10 @@
       <c r="F99" s="43"/>
       <c r="G99" s="47"/>
     </row>
-    <row r="100" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="47"/>
-      <c r="B100" s="152" t="s">
-        <v>1085</v>
+      <c r="B100" s="144" t="s">
+        <v>1053</v>
       </c>
       <c r="C100" s="47" t="s">
         <v>282</v>
@@ -65170,10 +65426,10 @@
       <c r="F100" s="43"/>
       <c r="G100" s="47"/>
     </row>
-    <row r="101" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="47"/>
       <c r="B101" s="145" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="C101" s="47" t="s">
         <v>282</v>
@@ -65185,10 +65441,10 @@
       <c r="F101" s="43"/>
       <c r="G101" s="47"/>
     </row>
-    <row r="102" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="47"/>
-      <c r="B102" s="151" t="s">
-        <v>1218</v>
+      <c r="B102" s="51" t="s">
+        <v>1054</v>
       </c>
       <c r="C102" s="47" t="s">
         <v>282</v>
@@ -65200,13 +65456,13 @@
       <c r="F102" s="43"/>
       <c r="G102" s="47"/>
     </row>
-    <row r="103" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A103" s="47"/>
-      <c r="B103" s="143" t="s">
-        <v>794</v>
+      <c r="B103" s="148" t="s">
+        <v>1066</v>
       </c>
       <c r="C103" s="47" t="s">
-        <v>798</v>
+        <v>282</v>
       </c>
       <c r="D103" s="47"/>
       <c r="E103" s="47" t="s">
@@ -65215,28 +65471,30 @@
       <c r="F103" s="43"/>
       <c r="G103" s="47"/>
     </row>
-    <row r="104" spans="1:7" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="47"/>
-      <c r="B104" s="144" t="s">
-        <v>769</v>
+      <c r="B104" s="152" t="s">
+        <v>188</v>
       </c>
       <c r="C104" s="47" t="s">
-        <v>798</v>
+        <v>282</v>
       </c>
       <c r="D104" s="47"/>
       <c r="E104" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F104" s="43"/>
+      <c r="F104" s="47" t="s">
+        <v>848</v>
+      </c>
       <c r="G104" s="47"/>
     </row>
-    <row r="105" spans="1:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="47"/>
-      <c r="B105" s="143" t="s">
-        <v>775</v>
+      <c r="B105" s="145" t="s">
+        <v>80</v>
       </c>
       <c r="C105" s="47" t="s">
-        <v>798</v>
+        <v>282</v>
       </c>
       <c r="D105" s="47"/>
       <c r="E105" s="47" t="s">
@@ -65245,13 +65503,13 @@
       <c r="F105" s="43"/>
       <c r="G105" s="47"/>
     </row>
-    <row r="106" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="47"/>
-      <c r="B106" s="145" t="s">
-        <v>783</v>
+      <c r="B106" s="151" t="s">
+        <v>1218</v>
       </c>
       <c r="C106" s="47" t="s">
-        <v>798</v>
+        <v>282</v>
       </c>
       <c r="D106" s="47"/>
       <c r="E106" s="47" t="s">
@@ -65260,10 +65518,10 @@
       <c r="F106" s="43"/>
       <c r="G106" s="47"/>
     </row>
-    <row r="107" spans="1:7" ht="39" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A107" s="47"/>
-      <c r="B107" s="144" t="s">
-        <v>768</v>
+      <c r="B107" s="145" t="s">
+        <v>794</v>
       </c>
       <c r="C107" s="47" t="s">
         <v>798</v>
@@ -65272,18 +65530,16 @@
       <c r="E107" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F107" s="43" t="s">
-        <v>846</v>
-      </c>
+      <c r="F107" s="43"/>
       <c r="G107" s="47"/>
     </row>
-    <row r="108" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A108" s="47"/>
-      <c r="B108" s="144" t="s">
-        <v>865</v>
+      <c r="B108" s="152" t="s">
+        <v>769</v>
       </c>
       <c r="C108" s="47" t="s">
-        <v>554</v>
+        <v>798</v>
       </c>
       <c r="D108" s="47"/>
       <c r="E108" s="47" t="s">
@@ -65292,13 +65548,13 @@
       <c r="F108" s="43"/>
       <c r="G108" s="47"/>
     </row>
-    <row r="109" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="47"/>
-      <c r="B109" s="144" t="s">
-        <v>872</v>
+      <c r="B109" s="143" t="s">
+        <v>775</v>
       </c>
       <c r="C109" s="47" t="s">
-        <v>554</v>
+        <v>798</v>
       </c>
       <c r="D109" s="47"/>
       <c r="E109" s="47" t="s">
@@ -65307,13 +65563,13 @@
       <c r="F109" s="43"/>
       <c r="G109" s="47"/>
     </row>
-    <row r="110" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A110" s="47"/>
-      <c r="B110" s="144" t="s">
-        <v>873</v>
+      <c r="B110" s="145" t="s">
+        <v>783</v>
       </c>
       <c r="C110" s="47" t="s">
-        <v>554</v>
+        <v>798</v>
       </c>
       <c r="D110" s="47"/>
       <c r="E110" s="47" t="s">
@@ -65322,25 +65578,27 @@
       <c r="F110" s="43"/>
       <c r="G110" s="47"/>
     </row>
-    <row r="111" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="47"/>
-      <c r="B111" s="152" t="s">
-        <v>935</v>
+      <c r="B111" s="144" t="s">
+        <v>768</v>
       </c>
       <c r="C111" s="47" t="s">
-        <v>554</v>
+        <v>798</v>
       </c>
       <c r="D111" s="47"/>
       <c r="E111" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F111" s="43"/>
+      <c r="F111" s="43" t="s">
+        <v>846</v>
+      </c>
       <c r="G111" s="47"/>
     </row>
-    <row r="112" spans="1:7" ht="39" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="47"/>
-      <c r="B112" s="152" t="s">
-        <v>936</v>
+      <c r="B112" s="144" t="s">
+        <v>865</v>
       </c>
       <c r="C112" s="47" t="s">
         <v>554</v>
@@ -65352,10 +65610,10 @@
       <c r="F112" s="43"/>
       <c r="G112" s="47"/>
     </row>
-    <row r="113" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A113" s="47"/>
-      <c r="B113" s="144" t="s">
-        <v>937</v>
+      <c r="B113" s="152" t="s">
+        <v>935</v>
       </c>
       <c r="C113" s="47" t="s">
         <v>554</v>
@@ -65367,10 +65625,10 @@
       <c r="F113" s="43"/>
       <c r="G113" s="47"/>
     </row>
-    <row r="114" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="47"/>
-      <c r="B114" s="144" t="s">
-        <v>943</v>
+      <c r="B114" s="152" t="s">
+        <v>936</v>
       </c>
       <c r="C114" s="47" t="s">
         <v>554</v>
@@ -65382,10 +65640,10 @@
       <c r="F114" s="43"/>
       <c r="G114" s="47"/>
     </row>
-    <row r="115" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="47"/>
       <c r="B115" s="144" t="s">
-        <v>944</v>
+        <v>937</v>
       </c>
       <c r="C115" s="47" t="s">
         <v>554</v>
@@ -65397,10 +65655,10 @@
       <c r="F115" s="43"/>
       <c r="G115" s="47"/>
     </row>
-    <row r="116" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A116" s="47"/>
       <c r="B116" s="144" t="s">
-        <v>960</v>
+        <v>943</v>
       </c>
       <c r="C116" s="47" t="s">
         <v>554</v>
@@ -65412,10 +65670,10 @@
       <c r="F116" s="43"/>
       <c r="G116" s="47"/>
     </row>
-    <row r="117" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="47"/>
       <c r="B117" s="144" t="s">
-        <v>968</v>
+        <v>944</v>
       </c>
       <c r="C117" s="47" t="s">
         <v>554</v>
@@ -65427,27 +65685,25 @@
       <c r="F117" s="43"/>
       <c r="G117" s="47"/>
     </row>
-    <row r="118" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A118" s="46"/>
-      <c r="B118" s="154" t="s">
-        <v>985</v>
-      </c>
-      <c r="C118" s="46" t="s">
+    <row r="118" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A118" s="47"/>
+      <c r="B118" s="144" t="s">
+        <v>960</v>
+      </c>
+      <c r="C118" s="47" t="s">
         <v>554</v>
       </c>
-      <c r="D118" s="46"/>
-      <c r="E118" s="46" t="s">
+      <c r="D118" s="47"/>
+      <c r="E118" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F118" s="46" t="s">
-        <v>1148</v>
-      </c>
-      <c r="G118" s="46"/>
+      <c r="F118" s="43"/>
+      <c r="G118" s="47"/>
     </row>
     <row r="119" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A119" s="47"/>
-      <c r="B119" s="152" t="s">
-        <v>1001</v>
+      <c r="B119" s="144" t="s">
+        <v>968</v>
       </c>
       <c r="C119" s="47" t="s">
         <v>554</v>
@@ -65459,26 +65715,43 @@
       <c r="F119" s="43"/>
       <c r="G119" s="47"/>
     </row>
-    <row r="120" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A120" s="47"/>
-      <c r="B120" s="144" t="s">
+    <row r="120" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A120" s="46"/>
+      <c r="B120" s="154" t="s">
+        <v>985</v>
+      </c>
+      <c r="C120" s="46" t="s">
+        <v>554</v>
+      </c>
+      <c r="D120" s="46"/>
+      <c r="E120" s="46" t="s">
+        <v>479</v>
+      </c>
+      <c r="F120" s="46" t="s">
+        <v>1148</v>
+      </c>
+      <c r="G120" s="46"/>
+    </row>
+    <row r="121" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A121" s="47"/>
+      <c r="B121" s="144" t="s">
         <v>1081</v>
       </c>
-      <c r="C120" s="47" t="s">
+      <c r="C121" s="47" t="s">
         <v>554</v>
       </c>
-      <c r="D120" s="47"/>
-      <c r="E120" s="47" t="s">
+      <c r="D121" s="47"/>
+      <c r="E121" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F120" s="43"/>
-      <c r="G120" s="47"/>
+      <c r="F121" s="43"/>
+      <c r="G121" s="47"/>
     </row>
   </sheetData>
-  <sortState ref="A3:G120">
-    <sortCondition ref="A3:A120"/>
-    <sortCondition ref="C3:C120"/>
-    <sortCondition ref="B3:B120"/>
+  <sortState ref="A3:G121">
+    <sortCondition ref="A3:A121"/>
+    <sortCondition ref="C3:C121"/>
+    <sortCondition ref="B3:B121"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>

</xml_diff>

<commit_message>
changes to effect sizes and more data
</commit_message>
<xml_diff>
--- a/Literature_search/database.xlsx
+++ b/Literature_search/database.xlsx
@@ -22,7 +22,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">' Step 2'!$A$2:$D$526</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">' Step 3'!$A$2:$C$344</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">' Step 4 (meta)'!$A$2:$C$120</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">' Step 4 (meta)'!$A$2:$C$121</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -392,7 +392,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B90" authorId="1">
+    <comment ref="B91" authorId="1">
       <text>
         <r>
           <rPr>
@@ -491,7 +491,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4957" uniqueCount="1260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4966" uniqueCount="1265">
   <si>
     <t>ID</t>
   </si>
@@ -36936,6 +36936,66 @@
       </rPr>
       <t>Experiment 1</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6 (background: silence, continuous speech, random speech, instrumental music, random tones, white noise)</t>
+  </si>
+  <si>
+    <t>only the 2 speech conditions can be coded due to the insufficiently reported statistics</t>
+  </si>
+  <si>
+    <r>
+      <t>Martin, R. C., Wogalter, M. S., &amp; Forlano, J. G. (1988). Reading comprehension in the presence of unattended speech and music. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Journal of memory and language</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>27</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(4), 382-398., </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Experiment 2</t>
+    </r>
+  </si>
+  <si>
+    <t>only the instrumental music condition (vs silence) can be coded. Due to the crossed design, there were not other comparisons to silence</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2 (instrumental: yes, no) x 3 (verbal factor: sung lyrics, spoken lyrics, no lyrics)</t>
   </si>
 </sst>
 </file>
@@ -37400,7 +37460,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -37497,6 +37557,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -37548,7 +37614,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="161">
+  <cellXfs count="162">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -37998,6 +38064,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="41" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -63497,10 +63566,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G121"/>
+  <dimension ref="A1:G122"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66"/>
+      <selection activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -64876,78 +64945,92 @@
         <v>479</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="47">
+    <row r="65" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="58">
         <v>63</v>
       </c>
-      <c r="B65" s="152" t="s">
+      <c r="B65" s="161" t="s">
         <v>1259</v>
       </c>
       <c r="C65" s="47" t="s">
         <v>554</v>
       </c>
-      <c r="D65" s="47"/>
-      <c r="E65" s="47" t="s">
+      <c r="D65" s="61" t="s">
+        <v>1260</v>
+      </c>
+      <c r="E65" s="58" t="s">
+        <v>1127</v>
+      </c>
+      <c r="F65" s="61" t="s">
+        <v>1261</v>
+      </c>
+      <c r="G65" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F65" s="43"/>
-      <c r="G65" s="47"/>
-    </row>
-    <row r="66" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="47">
+    </row>
+    <row r="66" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="58">
         <v>64</v>
       </c>
       <c r="B66" s="152" t="s">
-        <v>1253</v>
+        <v>1262</v>
       </c>
       <c r="C66" s="47" t="s">
         <v>554</v>
       </c>
-      <c r="D66" s="47"/>
-      <c r="E66" s="47" t="s">
+      <c r="D66" s="61" t="s">
+        <v>1264</v>
+      </c>
+      <c r="E66" s="58" t="s">
+        <v>1127</v>
+      </c>
+      <c r="F66" s="61" t="s">
+        <v>1263</v>
+      </c>
+      <c r="G66" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F66" s="43"/>
-      <c r="G66" s="47"/>
-    </row>
-    <row r="67" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="47">
         <v>65</v>
       </c>
-      <c r="B67" s="159" t="s">
-        <v>781</v>
+      <c r="B67" s="152" t="s">
+        <v>1253</v>
       </c>
       <c r="C67" s="47" t="s">
-        <v>798</v>
+        <v>554</v>
       </c>
       <c r="D67" s="47"/>
       <c r="E67" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F67" s="61" t="s">
-        <v>1232</v>
-      </c>
+      <c r="F67" s="43"/>
       <c r="G67" s="47"/>
     </row>
-    <row r="68" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="47"/>
-      <c r="B68" s="152" t="s">
-        <v>904</v>
+    <row r="68" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="47">
+        <v>66</v>
+      </c>
+      <c r="B68" s="159" t="s">
+        <v>781</v>
       </c>
       <c r="C68" s="47" t="s">
-        <v>320</v>
+        <v>798</v>
       </c>
       <c r="D68" s="47"/>
       <c r="E68" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F68" s="43"/>
+      <c r="F68" s="61" t="s">
+        <v>1232</v>
+      </c>
       <c r="G68" s="47"/>
     </row>
-    <row r="69" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="47"/>
-      <c r="B69" s="145" t="s">
-        <v>923</v>
+      <c r="B69" s="152" t="s">
+        <v>904</v>
       </c>
       <c r="C69" s="47" t="s">
         <v>320</v>
@@ -64959,10 +65042,10 @@
       <c r="F69" s="43"/>
       <c r="G69" s="47"/>
     </row>
-    <row r="70" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="47"/>
       <c r="B70" s="145" t="s">
-        <v>945</v>
+        <v>923</v>
       </c>
       <c r="C70" s="47" t="s">
         <v>320</v>
@@ -64971,15 +65054,13 @@
       <c r="E70" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F70" s="61" t="s">
-        <v>1155</v>
-      </c>
+      <c r="F70" s="43"/>
       <c r="G70" s="47"/>
     </row>
-    <row r="71" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="47"/>
-      <c r="B71" s="152" t="s">
-        <v>1011</v>
+      <c r="B71" s="145" t="s">
+        <v>945</v>
       </c>
       <c r="C71" s="47" t="s">
         <v>320</v>
@@ -64988,13 +65069,15 @@
       <c r="E71" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F71" s="43"/>
+      <c r="F71" s="61" t="s">
+        <v>1155</v>
+      </c>
       <c r="G71" s="47"/>
     </row>
-    <row r="72" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A72" s="47"/>
-      <c r="B72" s="145" t="s">
-        <v>1029</v>
+      <c r="B72" s="152" t="s">
+        <v>1011</v>
       </c>
       <c r="C72" s="47" t="s">
         <v>320</v>
@@ -65006,10 +65089,10 @@
       <c r="F72" s="43"/>
       <c r="G72" s="47"/>
     </row>
-    <row r="73" spans="1:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="47"/>
       <c r="B73" s="145" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="C73" s="47" t="s">
         <v>320</v>
@@ -65021,13 +65104,13 @@
       <c r="F73" s="43"/>
       <c r="G73" s="47"/>
     </row>
-    <row r="74" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="47"/>
-      <c r="B74" s="152" t="s">
-        <v>866</v>
+      <c r="B74" s="145" t="s">
+        <v>1030</v>
       </c>
       <c r="C74" s="47" t="s">
-        <v>282</v>
+        <v>320</v>
       </c>
       <c r="D74" s="47"/>
       <c r="E74" s="47" t="s">
@@ -65036,10 +65119,10 @@
       <c r="F74" s="43"/>
       <c r="G74" s="47"/>
     </row>
-    <row r="75" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="47"/>
-      <c r="B75" s="144" t="s">
-        <v>895</v>
+      <c r="B75" s="152" t="s">
+        <v>866</v>
       </c>
       <c r="C75" s="47" t="s">
         <v>282</v>
@@ -65051,10 +65134,10 @@
       <c r="F75" s="43"/>
       <c r="G75" s="47"/>
     </row>
-    <row r="76" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="47"/>
-      <c r="B76" s="152" t="s">
-        <v>900</v>
+      <c r="B76" s="144" t="s">
+        <v>895</v>
       </c>
       <c r="C76" s="47" t="s">
         <v>282</v>
@@ -65066,10 +65149,10 @@
       <c r="F76" s="43"/>
       <c r="G76" s="47"/>
     </row>
-    <row r="77" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="47"/>
-      <c r="B77" s="144" t="s">
-        <v>901</v>
+      <c r="B77" s="152" t="s">
+        <v>900</v>
       </c>
       <c r="C77" s="47" t="s">
         <v>282</v>
@@ -65081,10 +65164,10 @@
       <c r="F77" s="43"/>
       <c r="G77" s="47"/>
     </row>
-    <row r="78" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="47"/>
-      <c r="B78" s="146" t="s">
-        <v>90</v>
+      <c r="B78" s="144" t="s">
+        <v>901</v>
       </c>
       <c r="C78" s="47" t="s">
         <v>282</v>
@@ -65096,40 +65179,40 @@
       <c r="F78" s="43"/>
       <c r="G78" s="47"/>
     </row>
-    <row r="79" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="121"/>
-      <c r="B79" s="142" t="s">
+    <row r="79" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="47"/>
+      <c r="B79" s="146" t="s">
+        <v>90</v>
+      </c>
+      <c r="C79" s="47" t="s">
+        <v>282</v>
+      </c>
+      <c r="D79" s="47"/>
+      <c r="E79" s="47" t="s">
+        <v>479</v>
+      </c>
+      <c r="F79" s="43"/>
+      <c r="G79" s="47"/>
+    </row>
+    <row r="80" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="121"/>
+      <c r="B80" s="142" t="s">
         <v>55</v>
       </c>
-      <c r="C79" s="121" t="s">
-        <v>282</v>
-      </c>
-      <c r="D79" s="121"/>
-      <c r="E79" s="121"/>
-      <c r="F79" s="122" t="s">
+      <c r="C80" s="121" t="s">
+        <v>282</v>
+      </c>
+      <c r="D80" s="121"/>
+      <c r="E80" s="121"/>
+      <c r="F80" s="122" t="s">
         <v>835</v>
       </c>
-      <c r="G79" s="153"/>
-    </row>
-    <row r="80" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="47"/>
-      <c r="B80" s="144" t="s">
+      <c r="G80" s="153"/>
+    </row>
+    <row r="81" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="47"/>
+      <c r="B81" s="144" t="s">
         <v>762</v>
-      </c>
-      <c r="C80" s="47" t="s">
-        <v>282</v>
-      </c>
-      <c r="D80" s="47"/>
-      <c r="E80" s="47" t="s">
-        <v>479</v>
-      </c>
-      <c r="F80" s="43"/>
-      <c r="G80" s="47"/>
-    </row>
-    <row r="81" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="47"/>
-      <c r="B81" s="51" t="s">
-        <v>82</v>
       </c>
       <c r="C81" s="47" t="s">
         <v>282</v>
@@ -65141,10 +65224,10 @@
       <c r="F81" s="43"/>
       <c r="G81" s="47"/>
     </row>
-    <row r="82" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="47"/>
-      <c r="B82" s="145" t="s">
-        <v>81</v>
+      <c r="B82" s="51" t="s">
+        <v>82</v>
       </c>
       <c r="C82" s="47" t="s">
         <v>282</v>
@@ -65156,10 +65239,10 @@
       <c r="F82" s="43"/>
       <c r="G82" s="47"/>
     </row>
-    <row r="83" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="47"/>
-      <c r="B83" s="158" t="s">
-        <v>929</v>
+      <c r="B83" s="145" t="s">
+        <v>81</v>
       </c>
       <c r="C83" s="47" t="s">
         <v>282</v>
@@ -65171,10 +65254,10 @@
       <c r="F83" s="43"/>
       <c r="G83" s="47"/>
     </row>
-    <row r="84" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="47"/>
-      <c r="B84" s="152" t="s">
-        <v>933</v>
+      <c r="B84" s="158" t="s">
+        <v>929</v>
       </c>
       <c r="C84" s="47" t="s">
         <v>282</v>
@@ -65186,10 +65269,10 @@
       <c r="F84" s="43"/>
       <c r="G84" s="47"/>
     </row>
-    <row r="85" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="47"/>
-      <c r="B85" s="51" t="s">
-        <v>938</v>
+      <c r="B85" s="152" t="s">
+        <v>933</v>
       </c>
       <c r="C85" s="47" t="s">
         <v>282</v>
@@ -65201,10 +65284,10 @@
       <c r="F85" s="43"/>
       <c r="G85" s="47"/>
     </row>
-    <row r="86" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="47"/>
-      <c r="B86" s="152" t="s">
-        <v>939</v>
+      <c r="B86" s="51" t="s">
+        <v>938</v>
       </c>
       <c r="C86" s="47" t="s">
         <v>282</v>
@@ -65218,8 +65301,8 @@
     </row>
     <row r="87" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="47"/>
-      <c r="B87" s="51" t="s">
-        <v>940</v>
+      <c r="B87" s="152" t="s">
+        <v>939</v>
       </c>
       <c r="C87" s="47" t="s">
         <v>282</v>
@@ -65231,10 +65314,10 @@
       <c r="F87" s="43"/>
       <c r="G87" s="47"/>
     </row>
-    <row r="88" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="47"/>
       <c r="B88" s="51" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="C88" s="47" t="s">
         <v>282</v>
@@ -65246,10 +65329,10 @@
       <c r="F88" s="43"/>
       <c r="G88" s="47"/>
     </row>
-    <row r="89" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A89" s="47"/>
-      <c r="B89" s="152" t="s">
-        <v>942</v>
+      <c r="B89" s="51" t="s">
+        <v>941</v>
       </c>
       <c r="C89" s="47" t="s">
         <v>282</v>
@@ -65261,10 +65344,10 @@
       <c r="F89" s="43"/>
       <c r="G89" s="47"/>
     </row>
-    <row r="90" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="47"/>
-      <c r="B90" s="145" t="s">
-        <v>737</v>
+      <c r="B90" s="152" t="s">
+        <v>942</v>
       </c>
       <c r="C90" s="47" t="s">
         <v>282</v>
@@ -65276,10 +65359,10 @@
       <c r="F90" s="43"/>
       <c r="G90" s="47"/>
     </row>
-    <row r="91" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="47"/>
-      <c r="B91" s="152" t="s">
-        <v>957</v>
+      <c r="B91" s="145" t="s">
+        <v>737</v>
       </c>
       <c r="C91" s="47" t="s">
         <v>282</v>
@@ -65291,10 +65374,10 @@
       <c r="F91" s="43"/>
       <c r="G91" s="47"/>
     </row>
-    <row r="92" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="47"/>
-      <c r="B92" s="145" t="s">
-        <v>958</v>
+      <c r="B92" s="152" t="s">
+        <v>957</v>
       </c>
       <c r="C92" s="47" t="s">
         <v>282</v>
@@ -65306,10 +65389,10 @@
       <c r="F92" s="43"/>
       <c r="G92" s="47"/>
     </row>
-    <row r="93" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="47"/>
-      <c r="B93" s="152" t="s">
-        <v>964</v>
+      <c r="B93" s="145" t="s">
+        <v>958</v>
       </c>
       <c r="C93" s="47" t="s">
         <v>282</v>
@@ -65321,10 +65404,10 @@
       <c r="F93" s="43"/>
       <c r="G93" s="47"/>
     </row>
-    <row r="94" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="47"/>
       <c r="B94" s="152" t="s">
-        <v>991</v>
+        <v>964</v>
       </c>
       <c r="C94" s="47" t="s">
         <v>282</v>
@@ -65336,10 +65419,10 @@
       <c r="F94" s="43"/>
       <c r="G94" s="47"/>
     </row>
-    <row r="95" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="47"/>
-      <c r="B95" s="51" t="s">
-        <v>139</v>
+      <c r="B95" s="152" t="s">
+        <v>991</v>
       </c>
       <c r="C95" s="47" t="s">
         <v>282</v>
@@ -65351,10 +65434,10 @@
       <c r="F95" s="43"/>
       <c r="G95" s="47"/>
     </row>
-    <row r="96" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="47"/>
       <c r="B96" s="51" t="s">
-        <v>1002</v>
+        <v>139</v>
       </c>
       <c r="C96" s="47" t="s">
         <v>282</v>
@@ -65366,10 +65449,10 @@
       <c r="F96" s="43"/>
       <c r="G96" s="47"/>
     </row>
-    <row r="97" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="47"/>
       <c r="B97" s="51" t="s">
-        <v>88</v>
+        <v>1002</v>
       </c>
       <c r="C97" s="47" t="s">
         <v>282</v>
@@ -65381,10 +65464,10 @@
       <c r="F97" s="43"/>
       <c r="G97" s="47"/>
     </row>
-    <row r="98" spans="1:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A98" s="47"/>
-      <c r="B98" s="148" t="s">
-        <v>1021</v>
+      <c r="B98" s="51" t="s">
+        <v>88</v>
       </c>
       <c r="C98" s="47" t="s">
         <v>282</v>
@@ -65396,10 +65479,10 @@
       <c r="F98" s="43"/>
       <c r="G98" s="47"/>
     </row>
-    <row r="99" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="47"/>
-      <c r="B99" s="145" t="s">
-        <v>58</v>
+      <c r="B99" s="148" t="s">
+        <v>1021</v>
       </c>
       <c r="C99" s="47" t="s">
         <v>282</v>
@@ -65411,10 +65494,10 @@
       <c r="F99" s="43"/>
       <c r="G99" s="47"/>
     </row>
-    <row r="100" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="47"/>
-      <c r="B100" s="144" t="s">
-        <v>1053</v>
+      <c r="B100" s="145" t="s">
+        <v>58</v>
       </c>
       <c r="C100" s="47" t="s">
         <v>282</v>
@@ -65426,10 +65509,10 @@
       <c r="F100" s="43"/>
       <c r="G100" s="47"/>
     </row>
-    <row r="101" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="47"/>
-      <c r="B101" s="145" t="s">
-        <v>69</v>
+      <c r="B101" s="144" t="s">
+        <v>1053</v>
       </c>
       <c r="C101" s="47" t="s">
         <v>282</v>
@@ -65441,10 +65524,10 @@
       <c r="F101" s="43"/>
       <c r="G101" s="47"/>
     </row>
-    <row r="102" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="47"/>
-      <c r="B102" s="51" t="s">
-        <v>1054</v>
+      <c r="B102" s="145" t="s">
+        <v>69</v>
       </c>
       <c r="C102" s="47" t="s">
         <v>282</v>
@@ -65456,10 +65539,10 @@
       <c r="F102" s="43"/>
       <c r="G102" s="47"/>
     </row>
-    <row r="103" spans="1:7" ht="24" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="47"/>
-      <c r="B103" s="148" t="s">
-        <v>1066</v>
+      <c r="B103" s="51" t="s">
+        <v>1054</v>
       </c>
       <c r="C103" s="47" t="s">
         <v>282</v>
@@ -65471,10 +65554,10 @@
       <c r="F103" s="43"/>
       <c r="G103" s="47"/>
     </row>
-    <row r="104" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A104" s="47"/>
-      <c r="B104" s="152" t="s">
-        <v>188</v>
+      <c r="B104" s="148" t="s">
+        <v>1066</v>
       </c>
       <c r="C104" s="47" t="s">
         <v>282</v>
@@ -65483,15 +65566,13 @@
       <c r="E104" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F104" s="47" t="s">
-        <v>848</v>
-      </c>
+      <c r="F104" s="43"/>
       <c r="G104" s="47"/>
     </row>
-    <row r="105" spans="1:7" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="47"/>
-      <c r="B105" s="145" t="s">
-        <v>80</v>
+      <c r="B105" s="152" t="s">
+        <v>188</v>
       </c>
       <c r="C105" s="47" t="s">
         <v>282</v>
@@ -65500,13 +65581,15 @@
       <c r="E105" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F105" s="43"/>
+      <c r="F105" s="47" t="s">
+        <v>848</v>
+      </c>
       <c r="G105" s="47"/>
     </row>
-    <row r="106" spans="1:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="47"/>
-      <c r="B106" s="151" t="s">
-        <v>1218</v>
+      <c r="B106" s="145" t="s">
+        <v>80</v>
       </c>
       <c r="C106" s="47" t="s">
         <v>282</v>
@@ -65518,13 +65601,13 @@
       <c r="F106" s="43"/>
       <c r="G106" s="47"/>
     </row>
-    <row r="107" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="47"/>
-      <c r="B107" s="145" t="s">
-        <v>794</v>
+      <c r="B107" s="151" t="s">
+        <v>1218</v>
       </c>
       <c r="C107" s="47" t="s">
-        <v>798</v>
+        <v>282</v>
       </c>
       <c r="D107" s="47"/>
       <c r="E107" s="47" t="s">
@@ -65533,10 +65616,10 @@
       <c r="F107" s="43"/>
       <c r="G107" s="47"/>
     </row>
-    <row r="108" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A108" s="47"/>
-      <c r="B108" s="152" t="s">
-        <v>769</v>
+      <c r="B108" s="145" t="s">
+        <v>794</v>
       </c>
       <c r="C108" s="47" t="s">
         <v>798</v>
@@ -65548,10 +65631,10 @@
       <c r="F108" s="43"/>
       <c r="G108" s="47"/>
     </row>
-    <row r="109" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A109" s="47"/>
-      <c r="B109" s="143" t="s">
-        <v>775</v>
+      <c r="B109" s="152" t="s">
+        <v>769</v>
       </c>
       <c r="C109" s="47" t="s">
         <v>798</v>
@@ -65563,10 +65646,10 @@
       <c r="F109" s="43"/>
       <c r="G109" s="47"/>
     </row>
-    <row r="110" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="47"/>
-      <c r="B110" s="145" t="s">
-        <v>783</v>
+      <c r="B110" s="143" t="s">
+        <v>775</v>
       </c>
       <c r="C110" s="47" t="s">
         <v>798</v>
@@ -65578,10 +65661,10 @@
       <c r="F110" s="43"/>
       <c r="G110" s="47"/>
     </row>
-    <row r="111" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A111" s="47"/>
-      <c r="B111" s="144" t="s">
-        <v>768</v>
+      <c r="B111" s="145" t="s">
+        <v>783</v>
       </c>
       <c r="C111" s="47" t="s">
         <v>798</v>
@@ -65590,30 +65673,30 @@
       <c r="E111" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F111" s="43" t="s">
-        <v>846</v>
-      </c>
+      <c r="F111" s="43"/>
       <c r="G111" s="47"/>
     </row>
-    <row r="112" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="47"/>
       <c r="B112" s="144" t="s">
-        <v>865</v>
+        <v>768</v>
       </c>
       <c r="C112" s="47" t="s">
-        <v>554</v>
+        <v>798</v>
       </c>
       <c r="D112" s="47"/>
       <c r="E112" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F112" s="43"/>
+      <c r="F112" s="43" t="s">
+        <v>846</v>
+      </c>
       <c r="G112" s="47"/>
     </row>
-    <row r="113" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="47"/>
-      <c r="B113" s="152" t="s">
-        <v>935</v>
+      <c r="B113" s="144" t="s">
+        <v>865</v>
       </c>
       <c r="C113" s="47" t="s">
         <v>554</v>
@@ -65625,10 +65708,10 @@
       <c r="F113" s="43"/>
       <c r="G113" s="47"/>
     </row>
-    <row r="114" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A114" s="47"/>
       <c r="B114" s="152" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="C114" s="47" t="s">
         <v>554</v>
@@ -65640,10 +65723,10 @@
       <c r="F114" s="43"/>
       <c r="G114" s="47"/>
     </row>
-    <row r="115" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="47"/>
-      <c r="B115" s="144" t="s">
-        <v>937</v>
+      <c r="B115" s="152" t="s">
+        <v>936</v>
       </c>
       <c r="C115" s="47" t="s">
         <v>554</v>
@@ -65655,10 +65738,10 @@
       <c r="F115" s="43"/>
       <c r="G115" s="47"/>
     </row>
-    <row r="116" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="47"/>
       <c r="B116" s="144" t="s">
-        <v>943</v>
+        <v>937</v>
       </c>
       <c r="C116" s="47" t="s">
         <v>554</v>
@@ -65670,10 +65753,10 @@
       <c r="F116" s="43"/>
       <c r="G116" s="47"/>
     </row>
-    <row r="117" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A117" s="47"/>
       <c r="B117" s="144" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="C117" s="47" t="s">
         <v>554</v>
@@ -65685,10 +65768,10 @@
       <c r="F117" s="43"/>
       <c r="G117" s="47"/>
     </row>
-    <row r="118" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="47"/>
       <c r="B118" s="144" t="s">
-        <v>960</v>
+        <v>944</v>
       </c>
       <c r="C118" s="47" t="s">
         <v>554</v>
@@ -65703,7 +65786,7 @@
     <row r="119" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A119" s="47"/>
       <c r="B119" s="144" t="s">
-        <v>968</v>
+        <v>960</v>
       </c>
       <c r="C119" s="47" t="s">
         <v>554</v>
@@ -65715,37 +65798,52 @@
       <c r="F119" s="43"/>
       <c r="G119" s="47"/>
     </row>
-    <row r="120" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A120" s="46"/>
-      <c r="B120" s="154" t="s">
+    <row r="120" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A120" s="47"/>
+      <c r="B120" s="144" t="s">
+        <v>968</v>
+      </c>
+      <c r="C120" s="47" t="s">
+        <v>554</v>
+      </c>
+      <c r="D120" s="47"/>
+      <c r="E120" s="47" t="s">
+        <v>479</v>
+      </c>
+      <c r="F120" s="43"/>
+      <c r="G120" s="47"/>
+    </row>
+    <row r="121" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A121" s="46"/>
+      <c r="B121" s="154" t="s">
         <v>985</v>
       </c>
-      <c r="C120" s="46" t="s">
+      <c r="C121" s="46" t="s">
         <v>554</v>
       </c>
-      <c r="D120" s="46"/>
-      <c r="E120" s="46" t="s">
+      <c r="D121" s="46"/>
+      <c r="E121" s="46" t="s">
         <v>479</v>
       </c>
-      <c r="F120" s="46" t="s">
+      <c r="F121" s="46" t="s">
         <v>1148</v>
       </c>
-      <c r="G120" s="46"/>
-    </row>
-    <row r="121" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A121" s="47"/>
-      <c r="B121" s="144" t="s">
+      <c r="G121" s="46"/>
+    </row>
+    <row r="122" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A122" s="47"/>
+      <c r="B122" s="144" t="s">
         <v>1081</v>
       </c>
-      <c r="C121" s="47" t="s">
+      <c r="C122" s="47" t="s">
         <v>554</v>
       </c>
-      <c r="D121" s="47"/>
-      <c r="E121" s="47" t="s">
+      <c r="D122" s="47"/>
+      <c r="E122" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F121" s="43"/>
-      <c r="G121" s="47"/>
+      <c r="F122" s="43"/>
+      <c r="G122" s="47"/>
     </row>
   </sheetData>
   <sortState ref="A3:G121">

</xml_diff>

<commit_message>
small fix to previous log of stage 4
</commit_message>
<xml_diff>
--- a/Literature_search/database.xlsx
+++ b/Literature_search/database.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin Vasilev\SkyDrive\R\reading_sounds\Literature_search\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="120" windowWidth="16380" windowHeight="8070" tabRatio="987" activeTab="8"/>
   </bookViews>
@@ -34,7 +39,7 @@
     <author>Martin R. Vasilev</author>
   </authors>
   <commentList>
-    <comment ref="B19" authorId="0">
+    <comment ref="B19" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -69,7 +74,7 @@
     <author>Martin R. Vasilev</author>
   </authors>
   <commentList>
-    <comment ref="B219" authorId="0">
+    <comment ref="B219" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -105,7 +110,7 @@
     <author>Martin R. Vasilev</author>
   </authors>
   <commentList>
-    <comment ref="D2" authorId="0">
+    <comment ref="D2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -129,7 +134,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D67" authorId="0">
+    <comment ref="D67" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -154,7 +159,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B135" authorId="1">
+    <comment ref="B135" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -186,11 +191,35 @@
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
+    <author>Martin R. Vasilev</author>
     <author>Martin,Vasilev</author>
-    <author>Martin R. Vasilev</author>
   </authors>
   <commentList>
-    <comment ref="F9" authorId="0">
+    <comment ref="G2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Martin R. Vasilev:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+NA means it wasn't excluded</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F9" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -214,7 +243,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F12" authorId="0">
+    <comment ref="F12" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -238,7 +267,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G21" authorId="0">
+    <comment ref="G21" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -263,7 +292,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G22" authorId="0">
+    <comment ref="G22" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -291,7 +320,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G41" authorId="0">
+    <comment ref="G41" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -316,7 +345,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G60" authorId="0">
+    <comment ref="G60" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -343,7 +372,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B62" authorId="0">
+    <comment ref="B62" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -368,7 +397,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F63" authorId="0">
+    <comment ref="F63" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -392,7 +421,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B67" authorId="0">
+    <comment ref="B67" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -417,7 +446,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B68" authorId="0">
+    <comment ref="B68" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -442,7 +471,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D69" authorId="0">
+    <comment ref="D69" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -466,7 +495,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G69" authorId="0">
+    <comment ref="G69" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -490,7 +519,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B93" authorId="1">
+    <comment ref="B95" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -525,7 +554,7 @@
     <author>Martin,Vasilev</author>
   </authors>
   <commentList>
-    <comment ref="D175" authorId="0">
+    <comment ref="D175" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -559,7 +588,7 @@
     <author>Martin R. Vasilev</author>
   </authors>
   <commentList>
-    <comment ref="B73" authorId="0">
+    <comment ref="B73" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -589,7 +618,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4980" uniqueCount="1271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4990" uniqueCount="1277">
   <si>
     <t>ID</t>
   </si>
@@ -37203,11 +37232,29 @@
   <si>
     <t xml:space="preserve"> 4 (background: silence (?), negatively-affective, possitively-affective, ambiguously affective music)</t>
   </si>
+  <si>
+    <t>2(background: silence, speech)</t>
+  </si>
+  <si>
+    <t>also investigated WMC</t>
+  </si>
+  <si>
+    <t>3(background: silence, speech, road traffic noise)</t>
+  </si>
+  <si>
+    <t>2(background: silence, pop music)</t>
+  </si>
+  <si>
+    <t>the division into "bright" and "non-bright" students is averaged out</t>
+  </si>
+  <si>
+    <t>2(background: silence, rock and roll music)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="64" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -38237,9 +38284,6 @@
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -38270,10 +38314,13 @@
     <xf numFmtId="0" fontId="41" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="50" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -38621,7 +38668,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -63777,8 +63824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="D72" sqref="D72"/>
+    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -63820,7 +63867,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="47">
+      <c r="A3" s="58">
         <v>1</v>
       </c>
       <c r="B3" s="144" t="s">
@@ -63829,15 +63876,21 @@
       <c r="C3" s="47" t="s">
         <v>554</v>
       </c>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47" t="s">
+      <c r="D3" s="61" t="s">
+        <v>1271</v>
+      </c>
+      <c r="E3" s="58" t="s">
+        <v>1127</v>
+      </c>
+      <c r="F3" s="47" t="s">
+        <v>1272</v>
+      </c>
+      <c r="G3" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F3" s="43"/>
-      <c r="G3" s="47"/>
     </row>
     <row r="4" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="47">
+      <c r="A4" s="58">
         <v>2</v>
       </c>
       <c r="B4" s="144" t="s">
@@ -63846,32 +63899,42 @@
       <c r="C4" s="47" t="s">
         <v>554</v>
       </c>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47" t="s">
+      <c r="D4" s="61" t="s">
+        <v>1273</v>
+      </c>
+      <c r="E4" s="58" t="s">
+        <v>1127</v>
+      </c>
+      <c r="F4" s="43"/>
+      <c r="G4" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F4" s="43"/>
-      <c r="G4" s="47"/>
     </row>
     <row r="5" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="47">
+      <c r="A5" s="58">
         <v>3</v>
       </c>
-      <c r="B5" s="150" t="s">
+      <c r="B5" s="162" t="s">
         <v>517</v>
       </c>
       <c r="C5" s="47" t="s">
         <v>320</v>
       </c>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47" t="s">
+      <c r="D5" s="61" t="s">
+        <v>1274</v>
+      </c>
+      <c r="E5" s="58" t="s">
+        <v>1127</v>
+      </c>
+      <c r="F5" s="61" t="s">
+        <v>1275</v>
+      </c>
+      <c r="G5" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F5" s="43"/>
-      <c r="G5" s="47"/>
-    </row>
-    <row r="6" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="47">
+    </row>
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="58">
         <v>4</v>
       </c>
       <c r="B6" s="144" t="s">
@@ -63880,12 +63943,16 @@
       <c r="C6" s="47" t="s">
         <v>320</v>
       </c>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47" t="s">
+      <c r="D6" s="61" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E6" s="58" t="s">
+        <v>1127</v>
+      </c>
+      <c r="F6" s="43"/>
+      <c r="G6" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F6" s="43"/>
-      <c r="G6" s="47"/>
     </row>
     <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="58">
@@ -63914,7 +63981,7 @@
       <c r="A8" s="58">
         <v>6</v>
       </c>
-      <c r="B8" s="152" t="s">
+      <c r="B8" s="151" t="s">
         <v>915</v>
       </c>
       <c r="C8" s="47" t="s">
@@ -64159,7 +64226,7 @@
       <c r="A19" s="58">
         <v>17</v>
       </c>
-      <c r="B19" s="152" t="s">
+      <c r="B19" s="151" t="s">
         <v>518</v>
       </c>
       <c r="C19" s="47" t="s">
@@ -64215,7 +64282,7 @@
       <c r="E21" s="58" t="s">
         <v>1127</v>
       </c>
-      <c r="F21" s="155" t="s">
+      <c r="F21" s="154" t="s">
         <v>1157</v>
       </c>
       <c r="G21" s="47" t="s">
@@ -64247,7 +64314,7 @@
       <c r="A23" s="58">
         <v>21</v>
       </c>
-      <c r="B23" s="156" t="s">
+      <c r="B23" s="155" t="s">
         <v>1162</v>
       </c>
       <c r="C23" s="47" t="s">
@@ -64259,7 +64326,7 @@
       <c r="E23" s="58" t="s">
         <v>1127</v>
       </c>
-      <c r="F23" s="157" t="s">
+      <c r="F23" s="156" t="s">
         <v>1164</v>
       </c>
       <c r="G23" s="12" t="s">
@@ -64761,7 +64828,7 @@
       <c r="A47" s="58">
         <v>45</v>
       </c>
-      <c r="B47" s="152" t="s">
+      <c r="B47" s="151" t="s">
         <v>925</v>
       </c>
       <c r="C47" s="47" t="s">
@@ -64784,7 +64851,7 @@
       <c r="A48" s="58">
         <v>46</v>
       </c>
-      <c r="B48" s="152" t="s">
+      <c r="B48" s="151" t="s">
         <v>966</v>
       </c>
       <c r="C48" s="47" t="s">
@@ -64807,7 +64874,7 @@
       <c r="A49" s="58">
         <v>47</v>
       </c>
-      <c r="B49" s="156" t="s">
+      <c r="B49" s="155" t="s">
         <v>1211</v>
       </c>
       <c r="C49" s="47" t="s">
@@ -64853,7 +64920,7 @@
       <c r="A51" s="58">
         <v>49</v>
       </c>
-      <c r="B51" s="152" t="s">
+      <c r="B51" s="151" t="s">
         <v>878</v>
       </c>
       <c r="C51" s="47" t="s">
@@ -64873,7 +64940,7 @@
       <c r="A52" s="58">
         <v>50</v>
       </c>
-      <c r="B52" s="152" t="s">
+      <c r="B52" s="151" t="s">
         <v>902</v>
       </c>
       <c r="C52" s="47" t="s">
@@ -65070,7 +65137,7 @@
       <c r="A61" s="58">
         <v>59</v>
       </c>
-      <c r="B61" s="152" t="s">
+      <c r="B61" s="151" t="s">
         <v>1251</v>
       </c>
       <c r="C61" s="47" t="s">
@@ -65091,7 +65158,7 @@
       <c r="A62" s="58">
         <v>60</v>
       </c>
-      <c r="B62" s="152" t="s">
+      <c r="B62" s="151" t="s">
         <v>1252</v>
       </c>
       <c r="C62" s="47" t="s">
@@ -65112,7 +65179,7 @@
       <c r="A63" s="58">
         <v>61</v>
       </c>
-      <c r="B63" s="158" t="s">
+      <c r="B63" s="157" t="s">
         <v>1084</v>
       </c>
       <c r="C63" s="47" t="s">
@@ -65135,7 +65202,7 @@
       <c r="A64" s="58">
         <v>62</v>
       </c>
-      <c r="B64" s="152" t="s">
+      <c r="B64" s="151" t="s">
         <v>1085</v>
       </c>
       <c r="C64" s="47" t="s">
@@ -65158,7 +65225,7 @@
       <c r="A65" s="58">
         <v>63</v>
       </c>
-      <c r="B65" s="160" t="s">
+      <c r="B65" s="159" t="s">
         <v>1259</v>
       </c>
       <c r="C65" s="47" t="s">
@@ -65181,7 +65248,7 @@
       <c r="A66" s="58">
         <v>64</v>
       </c>
-      <c r="B66" s="152" t="s">
+      <c r="B66" s="151" t="s">
         <v>1262</v>
       </c>
       <c r="C66" s="47" t="s">
@@ -65204,7 +65271,7 @@
       <c r="A67" s="58">
         <v>65</v>
       </c>
-      <c r="B67" s="152" t="s">
+      <c r="B67" s="151" t="s">
         <v>1265</v>
       </c>
       <c r="C67" s="47" t="s">
@@ -65227,7 +65294,7 @@
       <c r="A68" s="58">
         <v>66</v>
       </c>
-      <c r="B68" s="152" t="s">
+      <c r="B68" s="151" t="s">
         <v>1268</v>
       </c>
       <c r="C68" s="47" t="s">
@@ -65250,7 +65317,7 @@
       <c r="A69" s="58">
         <v>67</v>
       </c>
-      <c r="B69" s="162" t="s">
+      <c r="B69" s="160" t="s">
         <v>923</v>
       </c>
       <c r="C69" s="47" t="s">
@@ -65271,11 +65338,11 @@
       <c r="A70" s="47">
         <v>68</v>
       </c>
-      <c r="B70" s="152" t="s">
-        <v>1253</v>
+      <c r="B70" s="150" t="s">
+        <v>1218</v>
       </c>
       <c r="C70" s="47" t="s">
-        <v>554</v>
+        <v>282</v>
       </c>
       <c r="D70" s="47"/>
       <c r="E70" s="47" t="s">
@@ -65288,57 +65355,59 @@
       <c r="A71" s="47">
         <v>69</v>
       </c>
-      <c r="B71" s="159" t="s">
-        <v>781</v>
+      <c r="B71" s="151" t="s">
+        <v>1253</v>
       </c>
       <c r="C71" s="47" t="s">
-        <v>798</v>
+        <v>554</v>
       </c>
       <c r="D71" s="47"/>
       <c r="E71" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F71" s="61" t="s">
-        <v>1232</v>
-      </c>
+      <c r="F71" s="43"/>
       <c r="G71" s="47"/>
     </row>
     <row r="72" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="47"/>
-      <c r="B72" s="152" t="s">
-        <v>904</v>
+      <c r="A72" s="47">
+        <v>70</v>
+      </c>
+      <c r="B72" s="158" t="s">
+        <v>781</v>
       </c>
       <c r="C72" s="47" t="s">
-        <v>320</v>
+        <v>798</v>
       </c>
       <c r="D72" s="47"/>
       <c r="E72" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F72" s="43"/>
+      <c r="F72" s="61" t="s">
+        <v>1232</v>
+      </c>
       <c r="G72" s="47"/>
     </row>
     <row r="73" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="47"/>
-      <c r="B73" s="145" t="s">
-        <v>945</v>
+      <c r="A73" s="47">
+        <v>71</v>
+      </c>
+      <c r="B73" s="144" t="s">
+        <v>968</v>
       </c>
       <c r="C73" s="47" t="s">
-        <v>320</v>
+        <v>554</v>
       </c>
       <c r="D73" s="47"/>
       <c r="E73" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F73" s="61" t="s">
-        <v>1155</v>
-      </c>
+      <c r="F73" s="43"/>
       <c r="G73" s="47"/>
     </row>
-    <row r="74" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A74" s="47"/>
-      <c r="B74" s="152" t="s">
-        <v>1011</v>
+      <c r="B74" s="151" t="s">
+        <v>904</v>
       </c>
       <c r="C74" s="47" t="s">
         <v>320</v>
@@ -65353,7 +65422,7 @@
     <row r="75" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="47"/>
       <c r="B75" s="145" t="s">
-        <v>1029</v>
+        <v>945</v>
       </c>
       <c r="C75" s="47" t="s">
         <v>320</v>
@@ -65362,13 +65431,15 @@
       <c r="E75" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F75" s="43"/>
+      <c r="F75" s="61" t="s">
+        <v>1155</v>
+      </c>
       <c r="G75" s="47"/>
     </row>
     <row r="76" spans="1:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="47"/>
-      <c r="B76" s="145" t="s">
-        <v>1030</v>
+      <c r="B76" s="151" t="s">
+        <v>1011</v>
       </c>
       <c r="C76" s="47" t="s">
         <v>320</v>
@@ -65382,11 +65453,11 @@
     </row>
     <row r="77" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="47"/>
-      <c r="B77" s="152" t="s">
-        <v>866</v>
+      <c r="B77" s="145" t="s">
+        <v>1029</v>
       </c>
       <c r="C77" s="47" t="s">
-        <v>282</v>
+        <v>320</v>
       </c>
       <c r="D77" s="47"/>
       <c r="E77" s="47" t="s">
@@ -65397,11 +65468,11 @@
     </row>
     <row r="78" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="47"/>
-      <c r="B78" s="144" t="s">
-        <v>895</v>
+      <c r="B78" s="145" t="s">
+        <v>1030</v>
       </c>
       <c r="C78" s="47" t="s">
-        <v>282</v>
+        <v>320</v>
       </c>
       <c r="D78" s="47"/>
       <c r="E78" s="47" t="s">
@@ -65412,8 +65483,8 @@
     </row>
     <row r="79" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="47"/>
-      <c r="B79" s="152" t="s">
-        <v>900</v>
+      <c r="B79" s="151" t="s">
+        <v>866</v>
       </c>
       <c r="C79" s="47" t="s">
         <v>282</v>
@@ -65428,7 +65499,7 @@
     <row r="80" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="47"/>
       <c r="B80" s="144" t="s">
-        <v>901</v>
+        <v>895</v>
       </c>
       <c r="C80" s="47" t="s">
         <v>282</v>
@@ -65442,8 +65513,8 @@
     </row>
     <row r="81" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="47"/>
-      <c r="B81" s="146" t="s">
-        <v>90</v>
+      <c r="B81" s="151" t="s">
+        <v>900</v>
       </c>
       <c r="C81" s="47" t="s">
         <v>282</v>
@@ -65456,24 +65527,24 @@
       <c r="G81" s="47"/>
     </row>
     <row r="82" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="121"/>
-      <c r="B82" s="142" t="s">
-        <v>55</v>
-      </c>
-      <c r="C82" s="121" t="s">
-        <v>282</v>
-      </c>
-      <c r="D82" s="121"/>
-      <c r="E82" s="121"/>
-      <c r="F82" s="122" t="s">
-        <v>835</v>
-      </c>
-      <c r="G82" s="153"/>
+      <c r="A82" s="47"/>
+      <c r="B82" s="144" t="s">
+        <v>901</v>
+      </c>
+      <c r="C82" s="47" t="s">
+        <v>282</v>
+      </c>
+      <c r="D82" s="47"/>
+      <c r="E82" s="47" t="s">
+        <v>479</v>
+      </c>
+      <c r="F82" s="43"/>
+      <c r="G82" s="47"/>
     </row>
     <row r="83" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="47"/>
-      <c r="B83" s="144" t="s">
-        <v>762</v>
+      <c r="B83" s="146" t="s">
+        <v>90</v>
       </c>
       <c r="C83" s="47" t="s">
         <v>282</v>
@@ -65486,24 +65557,24 @@
       <c r="G83" s="47"/>
     </row>
     <row r="84" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="47"/>
-      <c r="B84" s="51" t="s">
-        <v>82</v>
-      </c>
-      <c r="C84" s="47" t="s">
-        <v>282</v>
-      </c>
-      <c r="D84" s="47"/>
-      <c r="E84" s="47" t="s">
-        <v>479</v>
-      </c>
-      <c r="F84" s="43"/>
-      <c r="G84" s="47"/>
+      <c r="A84" s="121"/>
+      <c r="B84" s="142" t="s">
+        <v>55</v>
+      </c>
+      <c r="C84" s="121" t="s">
+        <v>282</v>
+      </c>
+      <c r="D84" s="121"/>
+      <c r="E84" s="121"/>
+      <c r="F84" s="122" t="s">
+        <v>835</v>
+      </c>
+      <c r="G84" s="152"/>
     </row>
     <row r="85" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="47"/>
-      <c r="B85" s="145" t="s">
-        <v>81</v>
+      <c r="B85" s="144" t="s">
+        <v>762</v>
       </c>
       <c r="C85" s="47" t="s">
         <v>282</v>
@@ -65517,8 +65588,8 @@
     </row>
     <row r="86" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="47"/>
-      <c r="B86" s="158" t="s">
-        <v>929</v>
+      <c r="B86" s="51" t="s">
+        <v>82</v>
       </c>
       <c r="C86" s="47" t="s">
         <v>282</v>
@@ -65532,8 +65603,8 @@
     </row>
     <row r="87" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="47"/>
-      <c r="B87" s="152" t="s">
-        <v>933</v>
+      <c r="B87" s="145" t="s">
+        <v>81</v>
       </c>
       <c r="C87" s="47" t="s">
         <v>282</v>
@@ -65547,8 +65618,8 @@
     </row>
     <row r="88" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="47"/>
-      <c r="B88" s="51" t="s">
-        <v>938</v>
+      <c r="B88" s="157" t="s">
+        <v>929</v>
       </c>
       <c r="C88" s="47" t="s">
         <v>282</v>
@@ -65562,8 +65633,8 @@
     </row>
     <row r="89" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="47"/>
-      <c r="B89" s="152" t="s">
-        <v>939</v>
+      <c r="B89" s="151" t="s">
+        <v>933</v>
       </c>
       <c r="C89" s="47" t="s">
         <v>282</v>
@@ -65578,7 +65649,7 @@
     <row r="90" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="47"/>
       <c r="B90" s="51" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
       <c r="C90" s="47" t="s">
         <v>282</v>
@@ -65590,10 +65661,10 @@
       <c r="F90" s="43"/>
       <c r="G90" s="47"/>
     </row>
-    <row r="91" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A91" s="47"/>
-      <c r="B91" s="51" t="s">
-        <v>941</v>
+      <c r="B91" s="151" t="s">
+        <v>939</v>
       </c>
       <c r="C91" s="47" t="s">
         <v>282</v>
@@ -65607,8 +65678,8 @@
     </row>
     <row r="92" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="47"/>
-      <c r="B92" s="152" t="s">
-        <v>942</v>
+      <c r="B92" s="51" t="s">
+        <v>940</v>
       </c>
       <c r="C92" s="47" t="s">
         <v>282</v>
@@ -65622,8 +65693,8 @@
     </row>
     <row r="93" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="47"/>
-      <c r="B93" s="145" t="s">
-        <v>737</v>
+      <c r="B93" s="51" t="s">
+        <v>941</v>
       </c>
       <c r="C93" s="47" t="s">
         <v>282</v>
@@ -65637,8 +65708,8 @@
     </row>
     <row r="94" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="47"/>
-      <c r="B94" s="152" t="s">
-        <v>957</v>
+      <c r="B94" s="151" t="s">
+        <v>942</v>
       </c>
       <c r="C94" s="47" t="s">
         <v>282</v>
@@ -65653,7 +65724,7 @@
     <row r="95" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="47"/>
       <c r="B95" s="145" t="s">
-        <v>958</v>
+        <v>737</v>
       </c>
       <c r="C95" s="47" t="s">
         <v>282</v>
@@ -65667,8 +65738,8 @@
     </row>
     <row r="96" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="47"/>
-      <c r="B96" s="152" t="s">
-        <v>964</v>
+      <c r="B96" s="151" t="s">
+        <v>957</v>
       </c>
       <c r="C96" s="47" t="s">
         <v>282</v>
@@ -65682,8 +65753,8 @@
     </row>
     <row r="97" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="47"/>
-      <c r="B97" s="152" t="s">
-        <v>991</v>
+      <c r="B97" s="145" t="s">
+        <v>958</v>
       </c>
       <c r="C97" s="47" t="s">
         <v>282</v>
@@ -65697,8 +65768,8 @@
     </row>
     <row r="98" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="47"/>
-      <c r="B98" s="51" t="s">
-        <v>139</v>
+      <c r="B98" s="151" t="s">
+        <v>964</v>
       </c>
       <c r="C98" s="47" t="s">
         <v>282</v>
@@ -65712,8 +65783,8 @@
     </row>
     <row r="99" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="47"/>
-      <c r="B99" s="51" t="s">
-        <v>1002</v>
+      <c r="B99" s="151" t="s">
+        <v>991</v>
       </c>
       <c r="C99" s="47" t="s">
         <v>282</v>
@@ -65725,10 +65796,10 @@
       <c r="F99" s="43"/>
       <c r="G99" s="47"/>
     </row>
-    <row r="100" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A100" s="47"/>
       <c r="B100" s="51" t="s">
-        <v>88</v>
+        <v>139</v>
       </c>
       <c r="C100" s="47" t="s">
         <v>282</v>
@@ -65742,8 +65813,8 @@
     </row>
     <row r="101" spans="1:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="47"/>
-      <c r="B101" s="148" t="s">
-        <v>1021</v>
+      <c r="B101" s="51" t="s">
+        <v>1002</v>
       </c>
       <c r="C101" s="47" t="s">
         <v>282</v>
@@ -65757,8 +65828,8 @@
     </row>
     <row r="102" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="47"/>
-      <c r="B102" s="145" t="s">
-        <v>58</v>
+      <c r="B102" s="51" t="s">
+        <v>88</v>
       </c>
       <c r="C102" s="47" t="s">
         <v>282</v>
@@ -65772,8 +65843,8 @@
     </row>
     <row r="103" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="47"/>
-      <c r="B103" s="144" t="s">
-        <v>1053</v>
+      <c r="B103" s="148" t="s">
+        <v>1021</v>
       </c>
       <c r="C103" s="47" t="s">
         <v>282</v>
@@ -65788,7 +65859,7 @@
     <row r="104" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="47"/>
       <c r="B104" s="145" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C104" s="47" t="s">
         <v>282</v>
@@ -65802,8 +65873,8 @@
     </row>
     <row r="105" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="47"/>
-      <c r="B105" s="51" t="s">
-        <v>1054</v>
+      <c r="B105" s="144" t="s">
+        <v>1053</v>
       </c>
       <c r="C105" s="47" t="s">
         <v>282</v>
@@ -65815,10 +65886,10 @@
       <c r="F105" s="43"/>
       <c r="G105" s="47"/>
     </row>
-    <row r="106" spans="1:7" ht="39" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A106" s="47"/>
-      <c r="B106" s="148" t="s">
-        <v>1066</v>
+      <c r="B106" s="145" t="s">
+        <v>69</v>
       </c>
       <c r="C106" s="47" t="s">
         <v>282</v>
@@ -65832,8 +65903,8 @@
     </row>
     <row r="107" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="47"/>
-      <c r="B107" s="152" t="s">
-        <v>188</v>
+      <c r="B107" s="51" t="s">
+        <v>1054</v>
       </c>
       <c r="C107" s="47" t="s">
         <v>282</v>
@@ -65842,15 +65913,13 @@
       <c r="E107" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F107" s="47" t="s">
-        <v>848</v>
-      </c>
+      <c r="F107" s="43"/>
       <c r="G107" s="47"/>
     </row>
     <row r="108" spans="1:7" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="47"/>
-      <c r="B108" s="145" t="s">
-        <v>80</v>
+      <c r="B108" s="148" t="s">
+        <v>1066</v>
       </c>
       <c r="C108" s="47" t="s">
         <v>282</v>
@@ -65865,7 +65934,7 @@
     <row r="109" spans="1:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="47"/>
       <c r="B109" s="151" t="s">
-        <v>1218</v>
+        <v>188</v>
       </c>
       <c r="C109" s="47" t="s">
         <v>282</v>
@@ -65874,16 +65943,18 @@
       <c r="E109" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F109" s="43"/>
+      <c r="F109" s="47" t="s">
+        <v>848</v>
+      </c>
       <c r="G109" s="47"/>
     </row>
     <row r="110" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A110" s="47"/>
       <c r="B110" s="145" t="s">
-        <v>794</v>
+        <v>80</v>
       </c>
       <c r="C110" s="47" t="s">
-        <v>798</v>
+        <v>282</v>
       </c>
       <c r="D110" s="47"/>
       <c r="E110" s="47" t="s">
@@ -65892,10 +65963,10 @@
       <c r="F110" s="43"/>
       <c r="G110" s="47"/>
     </row>
-    <row r="111" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A111" s="47"/>
-      <c r="B111" s="152" t="s">
-        <v>769</v>
+      <c r="B111" s="145" t="s">
+        <v>794</v>
       </c>
       <c r="C111" s="47" t="s">
         <v>798</v>
@@ -65909,8 +65980,8 @@
     </row>
     <row r="112" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="47"/>
-      <c r="B112" s="143" t="s">
-        <v>775</v>
+      <c r="B112" s="151" t="s">
+        <v>769</v>
       </c>
       <c r="C112" s="47" t="s">
         <v>798</v>
@@ -65922,10 +65993,10 @@
       <c r="F112" s="43"/>
       <c r="G112" s="47"/>
     </row>
-    <row r="113" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A113" s="47"/>
-      <c r="B113" s="145" t="s">
-        <v>783</v>
+      <c r="B113" s="143" t="s">
+        <v>775</v>
       </c>
       <c r="C113" s="47" t="s">
         <v>798</v>
@@ -65939,8 +66010,8 @@
     </row>
     <row r="114" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="47"/>
-      <c r="B114" s="144" t="s">
-        <v>768</v>
+      <c r="B114" s="145" t="s">
+        <v>783</v>
       </c>
       <c r="C114" s="47" t="s">
         <v>798</v>
@@ -65949,30 +66020,30 @@
       <c r="E114" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F114" s="43" t="s">
-        <v>846</v>
-      </c>
+      <c r="F114" s="43"/>
       <c r="G114" s="47"/>
     </row>
     <row r="115" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="47"/>
       <c r="B115" s="144" t="s">
-        <v>865</v>
+        <v>768</v>
       </c>
       <c r="C115" s="47" t="s">
-        <v>554</v>
+        <v>798</v>
       </c>
       <c r="D115" s="47"/>
       <c r="E115" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F115" s="43"/>
+      <c r="F115" s="43" t="s">
+        <v>846</v>
+      </c>
       <c r="G115" s="47"/>
     </row>
-    <row r="116" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" ht="39" x14ac:dyDescent="0.25">
       <c r="A116" s="47"/>
-      <c r="B116" s="152" t="s">
-        <v>935</v>
+      <c r="B116" s="144" t="s">
+        <v>865</v>
       </c>
       <c r="C116" s="47" t="s">
         <v>554</v>
@@ -65986,8 +66057,8 @@
     </row>
     <row r="117" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="47"/>
-      <c r="B117" s="152" t="s">
-        <v>936</v>
+      <c r="B117" s="151" t="s">
+        <v>935</v>
       </c>
       <c r="C117" s="47" t="s">
         <v>554</v>
@@ -66001,8 +66072,8 @@
     </row>
     <row r="118" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="47"/>
-      <c r="B118" s="144" t="s">
-        <v>937</v>
+      <c r="B118" s="151" t="s">
+        <v>936</v>
       </c>
       <c r="C118" s="47" t="s">
         <v>554</v>
@@ -66014,10 +66085,10 @@
       <c r="F118" s="43"/>
       <c r="G118" s="47"/>
     </row>
-    <row r="119" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" ht="39" x14ac:dyDescent="0.25">
       <c r="A119" s="47"/>
       <c r="B119" s="144" t="s">
-        <v>943</v>
+        <v>937</v>
       </c>
       <c r="C119" s="47" t="s">
         <v>554</v>
@@ -66032,7 +66103,7 @@
     <row r="120" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="47"/>
       <c r="B120" s="144" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="C120" s="47" t="s">
         <v>554</v>
@@ -66047,7 +66118,7 @@
     <row r="121" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A121" s="47"/>
       <c r="B121" s="144" t="s">
-        <v>960</v>
+        <v>944</v>
       </c>
       <c r="C121" s="47" t="s">
         <v>554</v>
@@ -66062,7 +66133,7 @@
     <row r="122" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A122" s="47"/>
       <c r="B122" s="144" t="s">
-        <v>968</v>
+        <v>960</v>
       </c>
       <c r="C122" s="47" t="s">
         <v>554</v>
@@ -66076,7 +66147,7 @@
     </row>
     <row r="123" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A123" s="46"/>
-      <c r="B123" s="154" t="s">
+      <c r="B123" s="153" t="s">
         <v>985</v>
       </c>
       <c r="C123" s="46" t="s">

</xml_diff>

<commit_message>
fixed problems with Excel file
</commit_message>
<xml_diff>
--- a/Literature_search/database.xlsx
+++ b/Literature_search/database.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="16380" windowHeight="8070" tabRatio="987" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7515" tabRatio="987" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="WoS" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">' Step 2'!$A$2:$D$526</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">' Step 3'!$A$2:$C$344</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">' Step 4 (meta)'!$A$2:$C$123</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">' Step 4 (meta)'!$A$2:$C$126</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -191,11 +191,10 @@
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Martin R. Vasilev</author>
     <author>Martin,Vasilev</author>
   </authors>
   <commentList>
-    <comment ref="G2" authorId="0" shapeId="0">
+    <comment ref="B2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -203,23 +202,23 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
-          <t>Martin R. Vasilev:</t>
+          <t>Martin,Vasilev:</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-NA means it wasn't excluded</t>
+Orange colouring means that the study had data that is eligible for inclusion, but effect sizes cannot be calculated due to reporting bias</t>
         </r>
       </text>
     </comment>
-    <comment ref="F9" authorId="1" shapeId="0">
+    <comment ref="F9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -243,7 +242,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F12" authorId="1" shapeId="0">
+    <comment ref="F12" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -267,7 +266,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G21" authorId="1" shapeId="0">
+    <comment ref="G21" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -292,7 +291,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G22" authorId="1" shapeId="0">
+    <comment ref="G22" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -320,7 +319,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G41" authorId="1" shapeId="0">
+    <comment ref="G41" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -345,7 +344,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G60" authorId="1" shapeId="0">
+    <comment ref="G60" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -372,7 +371,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B62" authorId="1" shapeId="0">
+    <comment ref="B62" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -397,7 +396,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F63" authorId="1" shapeId="0">
+    <comment ref="F63" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -421,7 +420,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B67" authorId="1" shapeId="0">
+    <comment ref="B67" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -446,7 +445,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B68" authorId="1" shapeId="0">
+    <comment ref="B68" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -471,7 +470,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D69" authorId="1" shapeId="0">
+    <comment ref="D69" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -495,7 +494,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G69" authorId="1" shapeId="0">
+    <comment ref="G69" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -519,7 +518,32 @@
         </r>
       </text>
     </comment>
-    <comment ref="B95" authorId="0" shapeId="0">
+    <comment ref="G70" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Martin,Vasilev:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+The descriptive statistics and ANOVAS are reported only for each personality group, but there is no way to get to the descriptives of every participant who took part in the study (n= 178). Basically, since each participants fell into more than one personality group, any averaging over the personality groups will produce big confounds because the score of each participant will be used multiple times to calculate the effect size. Also, the very big sample size that will result from this will not be the actual number of people who took part in the study. This will make the study have a much bigger influence in a meta-analysis because it will have a way bigger precision than it actually did. The only way out of this is to have the actual raw data. However, both authors seem to be out of academia (1st author appears to have been an (undergraduate?) student, while the second author seems to have retired). 
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G71" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -529,7 +553,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Martin R. Vasilev:</t>
+          <t>Martin,Vasilev:</t>
         </r>
         <r>
           <rPr>
@@ -539,8 +563,129 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-full-text found
+study is too old to get the data
 </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D72" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Martin,Vasilev:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+not fully-factorial design</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F73" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Martin,Vasilev:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+One issue in this experiment is how to classify the sound conditions. One complication is that participants were free to change radio stations and TV channels. However, based on the description in the paper, it appears that the radio can be best classified as background music and TV as background speech.  </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F77" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Martin,Vasilev:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+both background sounds here classify as speech
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D79" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Martin,Vasilev:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Instruction was also varied for the participants who completed the task with the TV on (ignore the TV , allowed to watch it occasionally). </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B84" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Martin,Vasilev:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Experiment 5 did not have a proofreading task</t>
         </r>
       </text>
     </comment>
@@ -618,7 +763,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4990" uniqueCount="1277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5035" uniqueCount="1312">
   <si>
     <t>ID</t>
   </si>
@@ -36428,9 +36573,6 @@
     <t>age of participants is not mentioned, but I assume that they were adults given that they were undergraduates</t>
   </si>
   <si>
-    <t>music type unknown; SDs nor reported</t>
-  </si>
-  <si>
     <t>2(background: semi-classical music, silence)</t>
   </si>
   <si>
@@ -37231,6 +37373,522 @@
   </si>
   <si>
     <t xml:space="preserve"> 4 (background: silence (?), negatively-affective, possitively-affective, ambiguously affective music)</t>
+  </si>
+  <si>
+    <t>same sample &amp; test as another (bigger) study?</t>
+  </si>
+  <si>
+    <t>2 (background: silence, speech)</t>
+  </si>
+  <si>
+    <t>impossible to extract effect sizes or to get in touch with the authors</t>
+  </si>
+  <si>
+    <t>it can be deduced that there were 16 participants per schedule (2 groups of 8)</t>
+  </si>
+  <si>
+    <r>
+      <t>Gawron, V. J. (1984). Noise: Effect and aftereffect. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Ergonomics</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>27</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(1), 5-18. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Experiment 1</t>
+    </r>
+  </si>
+  <si>
+    <t>lack of reported means for the different exposure conditions  makes it impossible to know the direction of the effect size</t>
+  </si>
+  <si>
+    <t>neither descriptives nor test statistics are reported</t>
+  </si>
+  <si>
+    <t>3 (background: silence, average noise, noisy) x  2(situation: classroom, experimental) x 2(task: homework, test)</t>
+  </si>
+  <si>
+    <r>
+      <t>Cool, V. A., Yarbrough, D. B., Patton, J. E., Runde, R., &amp; Keith, T. Z. (1994). Experimental effects of radio and television distractors on children's performance on mathematics and reading assignments. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>The Journal of experimental education</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>62</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(3), 181-194.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Experiment 2</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">2 (task difficulty: easy, less easy) x 3 (background: silence, radio TV) </t>
+  </si>
+  <si>
+    <t>impossible to calculate effect sizes- only % increase is reported, but no variance or test statistics</t>
+  </si>
+  <si>
+    <t>music type unknown; SDs not reported</t>
+  </si>
+  <si>
+    <t>2 (background: high noise, low noise) x 4 (restoration: movie, river, silence, noise)</t>
+  </si>
+  <si>
+    <t>2 (background: silence, music)</t>
+  </si>
+  <si>
+    <t>Only qualitative description of results, no descriptives or test statistics are reported; no silence baseline</t>
+  </si>
+  <si>
+    <t>the variety program is not coded as it is not very clear what it contained and how it should be classified</t>
+  </si>
+  <si>
+    <t>3 (background: silence, variety radio program, music radio program)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 (comprehension assessment: immediate, after a 5-min intervening task) x 3(background: silence, TV drama, TV ads)  </t>
+  </si>
+  <si>
+    <t>I average out the two assessment conditions because 5-min delay is not untypical and has been used in a number of other studies that were included</t>
+  </si>
+  <si>
+    <t>the other armstring paper (also add in all previous tabs!!!!)</t>
+  </si>
+  <si>
+    <t>2 (task: easy, difficult)  x3 (background: silence, music videos, soap opera)</t>
+  </si>
+  <si>
+    <t>task difficulty is averaged out</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Pool, M. M., Koolstra, C. M., &amp; Voort, T. H. (2003). The impact of background radio and television on high school students' homework performance. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Journal of Communication</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>53</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(1), 74-87. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Pool, M. M., Van der Voort, T. H., Beentjes, J. W., &amp; Koolstra, C. M. (2000). Background television as an inhibitor of performance on easy and difficult homework assignments. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Communication Research</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>27</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(3), 293-326. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Experiment 1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Pool, M. M., Van der Voort, T. H., Beentjes, J. W., &amp; Koolstra, C. M. (2000). Background television as an inhibitor of performance on easy and difficult homework assignments. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Communication Research</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>27</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(3), 293-326. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Experiment 2</t>
+    </r>
+  </si>
+  <si>
+    <t>4 (background: silence, soap opera, music videos, music radios) x 2 (assignment: paper-and-pencil, memory task)</t>
+  </si>
+  <si>
+    <t>the dependent measure is confounded here as the reading task also contained foreign language reading tests (English); it's impossible to get the ES for dutch texts only</t>
+  </si>
+  <si>
+    <r>
+      <t>Jones, D. M., Miles, C., &amp; Page, J. (1990). Disruption of proofreading by irrelevant speech: Effects of attention, arousal or memory?. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Applied Cognitive Psychology</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(2), 89-108.,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Experiment 1</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2 (background: native speech, reversed native speech) x 2 (sound intensity: 50 dBA, 70 dBA)</t>
+  </si>
+  <si>
+    <r>
+      <t>Jones, D. M., Miles, C., &amp; Page, J. (1990). Disruption of proofreading by irrelevant speech: Effects of attention, arousal or memory?. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Applied Cognitive Psychology</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(2), 89-108.,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Experiment 2</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2 (background: silence, reversed native speech)</t>
+  </si>
+  <si>
+    <t>impossible to calculate effect sizes- only means and descriptive summary of results (i.e. not sign.)</t>
+  </si>
+  <si>
+    <r>
+      <t>Jones, D. M., Miles, C., &amp; Page, J. (1990). Disruption of proofreading by irrelevant speech: Effects of attention, arousal or memory?. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Applied Cognitive Psychology</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(2), 89-108.,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Experiment 3</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4 (background: Binaural , Stereophonic,  moving voice or stationary voice speech)</t>
+  </si>
+  <si>
+    <r>
+      <t>Jones, D. M., Miles, C., &amp; Page, J. (1990). Disruption of proofreading by irrelevant speech: Effects of attention, arousal or memory?. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Applied Cognitive Psychology</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(2), 89-108.,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Experiment 4</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2 (background: native speech, reversed native speech) x 2 (lines of display: 1, 5)</t>
   </si>
   <si>
     <t>2(background: silence, speech)</t>
@@ -37255,7 +37913,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="64" x14ac:knownFonts="1">
+  <fonts count="65" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -37712,6 +38370,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="18">
     <fill>
@@ -37867,7 +38531,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="163">
+  <cellXfs count="166">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -38308,14 +38972,23 @@
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="41" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="50" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -50454,14 +51127,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="161"/>
-      <c r="B1" s="161"/>
-      <c r="C1" s="161"/>
-      <c r="D1" s="161"/>
-      <c r="E1" s="161"/>
-      <c r="F1" s="161"/>
-      <c r="G1" s="161"/>
-      <c r="H1" s="161"/>
+      <c r="A1" s="164"/>
+      <c r="B1" s="164"/>
+      <c r="C1" s="164"/>
+      <c r="D1" s="164"/>
+      <c r="E1" s="164"/>
+      <c r="F1" s="164"/>
+      <c r="G1" s="164"/>
+      <c r="H1" s="164"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -51205,7 +51878,7 @@
         <v>67</v>
       </c>
       <c r="B70" s="10" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="C70" s="12" t="s">
         <v>320</v>
@@ -51216,7 +51889,7 @@
         <v>68</v>
       </c>
       <c r="B71" s="10" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
     </row>
   </sheetData>
@@ -53952,7 +54625,7 @@
     </row>
     <row r="195" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
       <c r="B195" s="10" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="C195" s="12" t="s">
         <v>282</v>
@@ -58597,7 +59270,7 @@
     </row>
     <row r="527" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
       <c r="B527" s="10" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="C527" s="12" t="s">
         <v>320</v>
@@ -58623,8 +59296,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E344"/>
   <sheetViews>
-    <sheetView topLeftCell="A293" workbookViewId="0">
-      <selection activeCell="B301" sqref="B301"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:XFD31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -59084,14 +59757,14 @@
       <c r="A31" s="58">
         <v>29</v>
       </c>
-      <c r="B31" s="126" t="s">
+      <c r="B31" s="128" t="s">
         <v>794</v>
       </c>
       <c r="C31" s="58" t="s">
         <v>798</v>
       </c>
       <c r="D31" s="58" t="s">
-        <v>479</v>
+        <v>1222</v>
       </c>
       <c r="E31" s="17"/>
     </row>
@@ -59297,13 +59970,13 @@
         <v>43</v>
       </c>
       <c r="B45" s="128" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="C45" s="58" t="s">
         <v>320</v>
       </c>
       <c r="D45" s="58" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="E45" s="58"/>
     </row>
@@ -60411,7 +61084,7 @@
         <v>117</v>
       </c>
       <c r="B119" s="20" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="C119" s="58" t="s">
         <v>282</v>
@@ -60854,7 +61527,7 @@
         <v>554</v>
       </c>
       <c r="D148" s="60" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="E148" s="17"/>
     </row>
@@ -61253,7 +61926,7 @@
         <v>173</v>
       </c>
       <c r="B175" s="119" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="C175" s="58" t="s">
         <v>282</v>
@@ -61947,7 +62620,7 @@
         <v>219</v>
       </c>
       <c r="B221" s="20" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="C221" s="58" t="s">
         <v>320</v>
@@ -62097,7 +62770,7 @@
         <v>229</v>
       </c>
       <c r="B231" s="119" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="C231" s="58" t="s">
         <v>554</v>
@@ -62187,7 +62860,7 @@
         <v>235</v>
       </c>
       <c r="B237" s="119" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="C237" s="58" t="s">
         <v>798</v>
@@ -63005,7 +63678,7 @@
         <v>798</v>
       </c>
       <c r="D291" s="58" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="E291" s="17"/>
     </row>
@@ -63035,7 +63708,7 @@
         <v>282</v>
       </c>
       <c r="D293" s="58" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="E293" s="17"/>
     </row>
@@ -63151,13 +63824,13 @@
         <v>299</v>
       </c>
       <c r="B301" s="119" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
       <c r="C301" s="58" t="s">
         <v>554</v>
       </c>
       <c r="D301" s="58" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
       <c r="E301" s="17"/>
     </row>
@@ -63256,13 +63929,13 @@
         <v>306</v>
       </c>
       <c r="B308" s="119" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="C308" s="58" t="s">
         <v>282</v>
       </c>
       <c r="D308" s="58" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="E308" s="17"/>
     </row>
@@ -63669,10 +64342,10 @@
         <v>320</v>
       </c>
       <c r="D335" s="60" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="E335" s="58" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="336" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -63822,10 +64495,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G124"/>
+  <dimension ref="A1:G128"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -63877,13 +64550,13 @@
         <v>554</v>
       </c>
       <c r="D3" s="61" t="s">
-        <v>1271</v>
+        <v>1306</v>
       </c>
       <c r="E3" s="58" t="s">
         <v>1127</v>
       </c>
       <c r="F3" s="47" t="s">
-        <v>1272</v>
+        <v>1307</v>
       </c>
       <c r="G3" s="47" t="s">
         <v>479</v>
@@ -63900,7 +64573,7 @@
         <v>554</v>
       </c>
       <c r="D4" s="61" t="s">
-        <v>1273</v>
+        <v>1308</v>
       </c>
       <c r="E4" s="58" t="s">
         <v>1127</v>
@@ -63914,20 +64587,20 @@
       <c r="A5" s="58">
         <v>3</v>
       </c>
-      <c r="B5" s="162" t="s">
+      <c r="B5" s="165" t="s">
         <v>517</v>
       </c>
       <c r="C5" s="47" t="s">
         <v>320</v>
       </c>
       <c r="D5" s="61" t="s">
-        <v>1274</v>
+        <v>1309</v>
       </c>
       <c r="E5" s="58" t="s">
         <v>1127</v>
       </c>
       <c r="F5" s="61" t="s">
-        <v>1275</v>
+        <v>1310</v>
       </c>
       <c r="G5" s="47" t="s">
         <v>479</v>
@@ -63944,7 +64617,7 @@
         <v>320</v>
       </c>
       <c r="D6" s="61" t="s">
-        <v>1276</v>
+        <v>1311</v>
       </c>
       <c r="E6" s="58" t="s">
         <v>1127</v>
@@ -64256,7 +64929,7 @@
         <v>320</v>
       </c>
       <c r="D20" s="61" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="E20" s="58" t="s">
         <v>1127</v>
@@ -64277,13 +64950,13 @@
         <v>320</v>
       </c>
       <c r="D21" s="61" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="E21" s="58" t="s">
         <v>1127</v>
       </c>
       <c r="F21" s="154" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="G21" s="47" t="s">
         <v>479</v>
@@ -64300,14 +64973,14 @@
         <v>320</v>
       </c>
       <c r="D22" s="61" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="E22" s="46" t="s">
         <v>1134</v>
       </c>
       <c r="F22" s="43"/>
       <c r="G22" s="61" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.25">
@@ -64315,19 +64988,19 @@
         <v>21</v>
       </c>
       <c r="B23" s="155" t="s">
+        <v>1161</v>
+      </c>
+      <c r="C23" s="47" t="s">
+        <v>320</v>
+      </c>
+      <c r="D23" s="61" t="s">
         <v>1162</v>
-      </c>
-      <c r="C23" s="47" t="s">
-        <v>320</v>
-      </c>
-      <c r="D23" s="61" t="s">
-        <v>1163</v>
       </c>
       <c r="E23" s="58" t="s">
         <v>1127</v>
       </c>
       <c r="F23" s="156" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="G23" s="12" t="s">
         <v>479</v>
@@ -64344,13 +65017,13 @@
         <v>320</v>
       </c>
       <c r="D24" s="61" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="E24" s="58" t="s">
         <v>1127</v>
       </c>
       <c r="F24" s="61" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="G24" s="47" t="s">
         <v>479</v>
@@ -64367,13 +65040,13 @@
         <v>320</v>
       </c>
       <c r="D25" s="61" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="E25" s="58" t="s">
         <v>1127</v>
       </c>
       <c r="F25" s="61" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="G25" s="47" t="s">
         <v>479</v>
@@ -64390,7 +65063,7 @@
         <v>320</v>
       </c>
       <c r="D26" s="61" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="E26" s="58" t="s">
         <v>1127</v>
@@ -64411,14 +65084,14 @@
         <v>282</v>
       </c>
       <c r="D27" s="47" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="E27" s="46" t="s">
         <v>1134</v>
       </c>
       <c r="F27" s="43"/>
       <c r="G27" s="61" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -64432,14 +65105,14 @@
         <v>320</v>
       </c>
       <c r="D28" s="61" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="E28" s="46" t="s">
         <v>1134</v>
       </c>
       <c r="F28" s="47"/>
       <c r="G28" s="47" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -64453,14 +65126,14 @@
         <v>320</v>
       </c>
       <c r="D29" s="61" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="E29" s="46" t="s">
         <v>1134</v>
       </c>
       <c r="F29" s="43"/>
       <c r="G29" s="61" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -64474,14 +65147,14 @@
         <v>320</v>
       </c>
       <c r="D30" s="61" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="E30" s="46" t="s">
         <v>1134</v>
       </c>
       <c r="F30" s="43"/>
       <c r="G30" s="61" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -64500,7 +65173,7 @@
       </c>
       <c r="F31" s="43"/>
       <c r="G31" s="61" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -64514,14 +65187,14 @@
         <v>320</v>
       </c>
       <c r="D32" s="61" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
       <c r="E32" s="46" t="s">
         <v>1134</v>
       </c>
       <c r="F32" s="61"/>
       <c r="G32" s="61" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -64529,7 +65202,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="145" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="C33" s="47" t="s">
         <v>320</v>
@@ -64542,7 +65215,7 @@
       </c>
       <c r="F33" s="43"/>
       <c r="G33" s="61" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -64556,14 +65229,14 @@
         <v>320</v>
       </c>
       <c r="D34" s="61" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="E34" s="46" t="s">
         <v>1134</v>
       </c>
       <c r="F34" s="43"/>
       <c r="G34" s="61" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -64577,14 +65250,14 @@
         <v>320</v>
       </c>
       <c r="D35" s="61" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="E35" s="46" t="s">
         <v>1134</v>
       </c>
       <c r="F35" s="43"/>
       <c r="G35" s="61" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -64598,14 +65271,14 @@
         <v>320</v>
       </c>
       <c r="D36" s="47" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="E36" s="46" t="s">
         <v>1134</v>
       </c>
       <c r="F36" s="43"/>
       <c r="G36" s="61" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -64619,14 +65292,14 @@
         <v>320</v>
       </c>
       <c r="D37" s="61" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="E37" s="46" t="s">
         <v>1134</v>
       </c>
       <c r="F37" s="43"/>
       <c r="G37" s="61" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -64640,14 +65313,14 @@
         <v>320</v>
       </c>
       <c r="D38" s="61" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="E38" s="46" t="s">
         <v>1134</v>
       </c>
       <c r="F38" s="43"/>
       <c r="G38" s="61" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -64661,14 +65334,14 @@
         <v>320</v>
       </c>
       <c r="D39" s="61" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="E39" s="46" t="s">
         <v>1134</v>
       </c>
       <c r="F39" s="43"/>
       <c r="G39" s="61" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -64682,13 +65355,13 @@
         <v>320</v>
       </c>
       <c r="D40" s="61" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="E40" s="58" t="s">
         <v>1127</v>
       </c>
       <c r="F40" s="61" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="G40" s="47" t="s">
         <v>479</v>
@@ -64705,14 +65378,14 @@
         <v>320</v>
       </c>
       <c r="D41" s="47" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="E41" s="46" t="s">
         <v>1134</v>
       </c>
       <c r="F41" s="43"/>
       <c r="G41" s="61" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -64726,13 +65399,13 @@
         <v>320</v>
       </c>
       <c r="D42" s="61" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="E42" s="58" t="s">
         <v>1127</v>
       </c>
       <c r="F42" s="61" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="G42" s="47" t="s">
         <v>479</v>
@@ -64743,19 +65416,19 @@
         <v>41</v>
       </c>
       <c r="B43" s="147" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="C43" s="47" t="s">
         <v>320</v>
       </c>
       <c r="D43" s="61" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="E43" s="58" t="s">
         <v>1127</v>
       </c>
       <c r="F43" s="65" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="G43" s="61" t="s">
         <v>479</v>
@@ -64766,7 +65439,7 @@
         <v>42</v>
       </c>
       <c r="B44" s="145" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="C44" s="47" t="s">
         <v>320</v>
@@ -64779,7 +65452,7 @@
       </c>
       <c r="F44" s="53"/>
       <c r="G44" s="61" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -64793,14 +65466,14 @@
         <v>320</v>
       </c>
       <c r="D45" s="61" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="E45" s="46" t="s">
         <v>1134</v>
       </c>
       <c r="F45" s="61"/>
       <c r="G45" s="61" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -64814,14 +65487,14 @@
         <v>282</v>
       </c>
       <c r="D46" s="61" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="E46" s="46" t="s">
         <v>1134</v>
       </c>
       <c r="F46" s="43"/>
       <c r="G46" s="47" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -64835,13 +65508,13 @@
         <v>554</v>
       </c>
       <c r="D47" s="61" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="E47" s="58" t="s">
         <v>1127</v>
       </c>
       <c r="F47" s="61" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="G47" s="47" t="s">
         <v>479</v>
@@ -64858,13 +65531,13 @@
         <v>282</v>
       </c>
       <c r="D48" s="61" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="E48" s="58" t="s">
         <v>1127</v>
       </c>
       <c r="F48" s="61" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="G48" s="47" t="s">
         <v>479</v>
@@ -64875,19 +65548,19 @@
         <v>47</v>
       </c>
       <c r="B49" s="155" t="s">
+        <v>1210</v>
+      </c>
+      <c r="C49" s="47" t="s">
+        <v>282</v>
+      </c>
+      <c r="D49" s="61" t="s">
         <v>1211</v>
-      </c>
-      <c r="C49" s="47" t="s">
-        <v>282</v>
-      </c>
-      <c r="D49" s="61" t="s">
-        <v>1212</v>
       </c>
       <c r="E49" s="58" t="s">
         <v>1127</v>
       </c>
       <c r="F49" s="61" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="G49" s="47" t="s">
         <v>479</v>
@@ -64904,13 +65577,13 @@
         <v>798</v>
       </c>
       <c r="D50" s="61" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="E50" s="58" t="s">
         <v>1127</v>
       </c>
       <c r="F50" s="61" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="G50" s="47" t="s">
         <v>479</v>
@@ -64927,13 +65600,13 @@
         <v>282</v>
       </c>
       <c r="D51" s="61" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="E51" s="46" t="s">
         <v>1134</v>
       </c>
       <c r="G51" s="61" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="75" customHeight="1" x14ac:dyDescent="0.25">
@@ -64947,14 +65620,14 @@
         <v>282</v>
       </c>
       <c r="D52" s="61" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="E52" s="46" t="s">
         <v>1134</v>
       </c>
       <c r="F52" s="43"/>
       <c r="G52" s="61" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -64968,13 +65641,13 @@
         <v>320</v>
       </c>
       <c r="D53" s="61" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="E53" s="58" t="s">
         <v>1127</v>
       </c>
       <c r="F53" s="61" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="G53" s="12" t="s">
         <v>479</v>
@@ -64991,13 +65664,13 @@
         <v>320</v>
       </c>
       <c r="D54" s="61" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="E54" s="58" t="s">
         <v>1127</v>
       </c>
       <c r="F54" s="65" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="G54" s="47" t="s">
         <v>479</v>
@@ -65014,16 +65687,16 @@
         <v>798</v>
       </c>
       <c r="D55" s="61" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="E55" s="46" t="s">
         <v>1134</v>
       </c>
       <c r="F55" s="65" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="G55" s="61" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -65037,14 +65710,14 @@
         <v>798</v>
       </c>
       <c r="D56" s="61" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="E56" s="46" t="s">
         <v>1134</v>
       </c>
       <c r="F56" s="43"/>
       <c r="G56" s="61" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
@@ -65058,14 +65731,14 @@
         <v>282</v>
       </c>
       <c r="D57" s="47" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="E57" s="46" t="s">
         <v>1134</v>
       </c>
       <c r="F57" s="43"/>
       <c r="G57" s="61" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -65079,14 +65752,14 @@
         <v>554</v>
       </c>
       <c r="D58" s="61" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="E58" s="46" t="s">
         <v>1134</v>
       </c>
       <c r="F58" s="43"/>
       <c r="G58" s="61" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -65100,16 +65773,16 @@
         <v>320</v>
       </c>
       <c r="D59" s="61" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="E59" s="46" t="s">
         <v>1134</v>
       </c>
       <c r="F59" s="61" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="G59" s="47" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -65123,14 +65796,14 @@
         <v>320</v>
       </c>
       <c r="D60" s="62" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="E60" s="46" t="s">
         <v>1134</v>
       </c>
       <c r="F60" s="43"/>
       <c r="G60" s="47" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -65138,20 +65811,20 @@
         <v>59</v>
       </c>
       <c r="B61" s="151" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="C61" s="47" t="s">
         <v>554</v>
       </c>
       <c r="D61" s="61" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="E61" s="46" t="s">
         <v>1134</v>
       </c>
       <c r="F61" s="43"/>
       <c r="G61" s="61" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -65159,20 +65832,20 @@
         <v>60</v>
       </c>
       <c r="B62" s="151" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="C62" s="47" t="s">
         <v>554</v>
       </c>
       <c r="D62" s="61" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="E62" s="46" t="s">
         <v>1134</v>
       </c>
       <c r="F62" s="43"/>
       <c r="G62" s="61" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -65186,13 +65859,13 @@
         <v>282</v>
       </c>
       <c r="D63" s="61" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="E63" s="58" t="s">
         <v>1127</v>
       </c>
       <c r="F63" s="61" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="G63" s="47" t="s">
         <v>479</v>
@@ -65209,13 +65882,13 @@
         <v>282</v>
       </c>
       <c r="D64" s="61" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="E64" s="58" t="s">
         <v>1127</v>
       </c>
       <c r="F64" s="65" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="G64" s="47" t="s">
         <v>479</v>
@@ -65225,20 +65898,20 @@
       <c r="A65" s="58">
         <v>63</v>
       </c>
-      <c r="B65" s="159" t="s">
-        <v>1259</v>
+      <c r="B65" s="158" t="s">
+        <v>1258</v>
       </c>
       <c r="C65" s="47" t="s">
         <v>554</v>
       </c>
       <c r="D65" s="61" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="E65" s="58" t="s">
         <v>1127</v>
       </c>
       <c r="F65" s="61" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="G65" s="47" t="s">
         <v>479</v>
@@ -65249,19 +65922,19 @@
         <v>64</v>
       </c>
       <c r="B66" s="151" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="C66" s="47" t="s">
         <v>554</v>
       </c>
       <c r="D66" s="61" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="E66" s="58" t="s">
         <v>1127</v>
       </c>
       <c r="F66" s="61" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="G66" s="47" t="s">
         <v>479</v>
@@ -65272,19 +65945,19 @@
         <v>65</v>
       </c>
       <c r="B67" s="151" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="C67" s="47" t="s">
         <v>554</v>
       </c>
       <c r="D67" s="61" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="E67" s="58" t="s">
         <v>1127</v>
       </c>
       <c r="F67" s="61" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="G67" s="47" t="s">
         <v>479</v>
@@ -65295,19 +65968,19 @@
         <v>66</v>
       </c>
       <c r="B68" s="151" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
       <c r="C68" s="47" t="s">
         <v>554</v>
       </c>
       <c r="D68" s="61" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="E68" s="58" t="s">
         <v>1127</v>
       </c>
       <c r="F68" s="61" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="G68" s="47" t="s">
         <v>479</v>
@@ -65317,267 +65990,359 @@
       <c r="A69" s="58">
         <v>67</v>
       </c>
-      <c r="B69" s="160" t="s">
+      <c r="B69" s="159" t="s">
         <v>923</v>
       </c>
       <c r="C69" s="47" t="s">
         <v>320</v>
       </c>
       <c r="D69" s="61" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="E69" s="46" t="s">
         <v>1134</v>
       </c>
       <c r="F69" s="43"/>
       <c r="G69" s="47" t="s">
-        <v>1196</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="47">
+        <v>1195</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="58">
         <v>68</v>
       </c>
       <c r="B70" s="150" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="C70" s="47" t="s">
         <v>282</v>
       </c>
-      <c r="D70" s="47"/>
-      <c r="E70" s="47" t="s">
-        <v>479</v>
+      <c r="D70" s="61" t="s">
+        <v>1271</v>
+      </c>
+      <c r="E70" s="46" t="s">
+        <v>1134</v>
       </c>
       <c r="F70" s="43"/>
-      <c r="G70" s="47"/>
-    </row>
-    <row r="71" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="47">
+      <c r="G70" s="61" t="s">
+        <v>1272</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="58">
         <v>69</v>
       </c>
-      <c r="B71" s="151" t="s">
-        <v>1253</v>
+      <c r="B71" s="160" t="s">
+        <v>1274</v>
       </c>
       <c r="C71" s="47" t="s">
-        <v>554</v>
-      </c>
-      <c r="D71" s="47"/>
-      <c r="E71" s="47" t="s">
-        <v>479</v>
-      </c>
-      <c r="F71" s="43"/>
-      <c r="G71" s="47"/>
-    </row>
-    <row r="72" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="47">
+        <v>282</v>
+      </c>
+      <c r="E71" s="46" t="s">
+        <v>1134</v>
+      </c>
+      <c r="F71" s="61" t="s">
+        <v>1273</v>
+      </c>
+      <c r="G71" s="61" t="s">
+        <v>1275</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="58">
         <v>70</v>
       </c>
-      <c r="B72" s="158" t="s">
+      <c r="B72" s="161" t="s">
         <v>781</v>
       </c>
       <c r="C72" s="47" t="s">
         <v>798</v>
       </c>
-      <c r="D72" s="47"/>
-      <c r="E72" s="47" t="s">
+      <c r="D72" s="61" t="s">
+        <v>1277</v>
+      </c>
+      <c r="E72" s="46" t="s">
+        <v>1134</v>
+      </c>
+      <c r="F72" s="61" t="s">
+        <v>1231</v>
+      </c>
+      <c r="G72" s="61" t="s">
+        <v>1276</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="58">
+        <v>71</v>
+      </c>
+      <c r="B73" s="151" t="s">
+        <v>1278</v>
+      </c>
+      <c r="C73" s="47" t="s">
+        <v>320</v>
+      </c>
+      <c r="D73" s="61" t="s">
+        <v>1279</v>
+      </c>
+      <c r="E73" s="58" t="s">
+        <v>1127</v>
+      </c>
+      <c r="F73" s="61" t="s">
+        <v>1195</v>
+      </c>
+      <c r="G73" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F72" s="61" t="s">
-        <v>1232</v>
-      </c>
-      <c r="G72" s="47"/>
-    </row>
-    <row r="73" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="47">
-        <v>71</v>
-      </c>
-      <c r="B73" s="144" t="s">
-        <v>968</v>
-      </c>
-      <c r="C73" s="47" t="s">
-        <v>554</v>
-      </c>
-      <c r="D73" s="47"/>
-      <c r="E73" s="47" t="s">
-        <v>479</v>
-      </c>
-      <c r="F73" s="43"/>
-      <c r="G73" s="47"/>
-    </row>
-    <row r="74" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A74" s="47"/>
-      <c r="B74" s="151" t="s">
-        <v>904</v>
+    </row>
+    <row r="74" spans="1:7" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="58">
+        <v>72</v>
+      </c>
+      <c r="B74" s="145" t="s">
+        <v>945</v>
       </c>
       <c r="C74" s="47" t="s">
         <v>320</v>
       </c>
-      <c r="D74" s="47"/>
-      <c r="E74" s="47" t="s">
-        <v>479</v>
-      </c>
-      <c r="F74" s="43"/>
-      <c r="G74" s="47"/>
-    </row>
-    <row r="75" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="47"/>
-      <c r="B75" s="145" t="s">
-        <v>945</v>
+      <c r="D74" s="61" t="s">
+        <v>1283</v>
+      </c>
+      <c r="E74" s="46" t="s">
+        <v>1134</v>
+      </c>
+      <c r="F74" s="61" t="s">
+        <v>1281</v>
+      </c>
+      <c r="G74" s="61" t="s">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="58">
+        <v>73</v>
+      </c>
+      <c r="B75" s="162" t="s">
+        <v>964</v>
       </c>
       <c r="C75" s="47" t="s">
-        <v>320</v>
-      </c>
-      <c r="D75" s="47"/>
-      <c r="E75" s="47" t="s">
-        <v>479</v>
-      </c>
-      <c r="F75" s="61" t="s">
-        <v>1155</v>
-      </c>
-      <c r="G75" s="47"/>
+        <v>282</v>
+      </c>
+      <c r="D75" s="61" t="s">
+        <v>1282</v>
+      </c>
+      <c r="E75" s="46" t="s">
+        <v>1134</v>
+      </c>
+      <c r="F75" s="43"/>
+      <c r="G75" s="61" t="s">
+        <v>1284</v>
+      </c>
     </row>
     <row r="76" spans="1:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="47"/>
+      <c r="A76" s="58">
+        <v>74</v>
+      </c>
       <c r="B76" s="151" t="s">
         <v>1011</v>
       </c>
       <c r="C76" s="47" t="s">
         <v>320</v>
       </c>
-      <c r="D76" s="47"/>
-      <c r="E76" s="47" t="s">
+      <c r="D76" s="61" t="s">
+        <v>1286</v>
+      </c>
+      <c r="E76" s="58" t="s">
+        <v>1127</v>
+      </c>
+      <c r="F76" s="61" t="s">
+        <v>1285</v>
+      </c>
+      <c r="G76" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F76" s="43"/>
-      <c r="G76" s="47"/>
-    </row>
-    <row r="77" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="47"/>
-      <c r="B77" s="145" t="s">
-        <v>1029</v>
+    </row>
+    <row r="77" spans="1:7" ht="78" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="58">
+        <v>75</v>
+      </c>
+      <c r="B77" s="151" t="s">
+        <v>866</v>
       </c>
       <c r="C77" s="47" t="s">
-        <v>320</v>
-      </c>
-      <c r="D77" s="47"/>
-      <c r="E77" s="47" t="s">
+        <v>282</v>
+      </c>
+      <c r="D77" s="61" t="s">
+        <v>1287</v>
+      </c>
+      <c r="E77" s="58" t="s">
+        <v>1127</v>
+      </c>
+      <c r="F77" s="61" t="s">
+        <v>1288</v>
+      </c>
+      <c r="G77" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F77" s="43"/>
-      <c r="G77" s="47"/>
-    </row>
-    <row r="78" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="47"/>
+    </row>
+    <row r="78" spans="1:7" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="58">
+        <v>76</v>
+      </c>
       <c r="B78" s="145" t="s">
-        <v>1030</v>
+        <v>1293</v>
       </c>
       <c r="C78" s="47" t="s">
         <v>320</v>
       </c>
-      <c r="D78" s="47"/>
-      <c r="E78" s="47" t="s">
+      <c r="D78" s="61" t="s">
+        <v>1290</v>
+      </c>
+      <c r="E78" s="58" t="s">
+        <v>1127</v>
+      </c>
+      <c r="F78" s="61" t="s">
+        <v>1291</v>
+      </c>
+      <c r="G78" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F78" s="43"/>
-      <c r="G78" s="47"/>
-    </row>
-    <row r="79" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="47"/>
-      <c r="B79" s="151" t="s">
-        <v>866</v>
+    </row>
+    <row r="79" spans="1:7" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="58">
+        <v>77</v>
+      </c>
+      <c r="B79" s="145" t="s">
+        <v>1294</v>
       </c>
       <c r="C79" s="47" t="s">
-        <v>282</v>
-      </c>
-      <c r="D79" s="47"/>
-      <c r="E79" s="47" t="s">
+        <v>320</v>
+      </c>
+      <c r="D79" s="61" t="s">
+        <v>1290</v>
+      </c>
+      <c r="E79" s="58" t="s">
+        <v>1127</v>
+      </c>
+      <c r="F79" s="61" t="s">
+        <v>1291</v>
+      </c>
+      <c r="G79" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F79" s="43"/>
-      <c r="G79" s="47"/>
-    </row>
-    <row r="80" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="47"/>
-      <c r="B80" s="144" t="s">
-        <v>895</v>
+    </row>
+    <row r="80" spans="1:7" ht="87" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="58">
+        <v>78</v>
+      </c>
+      <c r="B80" s="145" t="s">
+        <v>1292</v>
       </c>
       <c r="C80" s="47" t="s">
-        <v>282</v>
-      </c>
-      <c r="D80" s="47"/>
-      <c r="E80" s="47" t="s">
-        <v>479</v>
-      </c>
-      <c r="F80" s="43"/>
-      <c r="G80" s="47"/>
-    </row>
-    <row r="81" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="47"/>
-      <c r="B81" s="151" t="s">
-        <v>900</v>
+        <v>320</v>
+      </c>
+      <c r="D80" s="61" t="s">
+        <v>1295</v>
+      </c>
+      <c r="E80" s="46" t="s">
+        <v>1134</v>
+      </c>
+      <c r="G80" s="61" t="s">
+        <v>1296</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="58">
+        <v>79</v>
+      </c>
+      <c r="B81" s="144" t="s">
+        <v>1297</v>
       </c>
       <c r="C81" s="47" t="s">
-        <v>282</v>
-      </c>
-      <c r="D81" s="47"/>
-      <c r="E81" s="47" t="s">
-        <v>479</v>
+        <v>554</v>
+      </c>
+      <c r="D81" s="61" t="s">
+        <v>1298</v>
+      </c>
+      <c r="E81" s="46" t="s">
+        <v>1134</v>
       </c>
       <c r="F81" s="43"/>
-      <c r="G81" s="47"/>
-    </row>
-    <row r="82" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="47"/>
-      <c r="B82" s="144" t="s">
-        <v>901</v>
+      <c r="G81" s="47" t="s">
+        <v>1205</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="58">
+        <v>80</v>
+      </c>
+      <c r="B82" s="163" t="s">
+        <v>1299</v>
       </c>
       <c r="C82" s="47" t="s">
-        <v>282</v>
-      </c>
-      <c r="D82" s="47"/>
-      <c r="E82" s="47" t="s">
-        <v>479</v>
+        <v>554</v>
+      </c>
+      <c r="D82" s="61" t="s">
+        <v>1300</v>
+      </c>
+      <c r="E82" s="46" t="s">
+        <v>1134</v>
       </c>
       <c r="F82" s="43"/>
-      <c r="G82" s="47"/>
-    </row>
-    <row r="83" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="47"/>
-      <c r="B83" s="146" t="s">
-        <v>90</v>
+      <c r="G82" s="61" t="s">
+        <v>1301</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="58">
+        <v>81</v>
+      </c>
+      <c r="B83" s="144" t="s">
+        <v>1302</v>
       </c>
       <c r="C83" s="47" t="s">
-        <v>282</v>
-      </c>
-      <c r="D83" s="47"/>
-      <c r="E83" s="47" t="s">
-        <v>479</v>
+        <v>554</v>
+      </c>
+      <c r="D83" s="61" t="s">
+        <v>1303</v>
+      </c>
+      <c r="E83" s="46" t="s">
+        <v>1134</v>
       </c>
       <c r="F83" s="43"/>
-      <c r="G83" s="47"/>
-    </row>
-    <row r="84" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="121"/>
-      <c r="B84" s="142" t="s">
-        <v>55</v>
-      </c>
-      <c r="C84" s="121" t="s">
-        <v>282</v>
-      </c>
-      <c r="D84" s="121"/>
-      <c r="E84" s="121"/>
-      <c r="F84" s="122" t="s">
-        <v>835</v>
-      </c>
-      <c r="G84" s="152"/>
-    </row>
-    <row r="85" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="47"/>
-      <c r="B85" s="144" t="s">
-        <v>762</v>
+      <c r="G83" s="61" t="s">
+        <v>1205</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="58">
+        <v>82</v>
+      </c>
+      <c r="B84" s="144" t="s">
+        <v>1304</v>
+      </c>
+      <c r="C84" s="47" t="s">
+        <v>554</v>
+      </c>
+      <c r="D84" s="61" t="s">
+        <v>1305</v>
+      </c>
+      <c r="E84" s="46" t="s">
+        <v>1134</v>
+      </c>
+      <c r="F84" s="43"/>
+      <c r="G84" s="61" t="s">
+        <v>1205</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="47">
+        <v>83</v>
+      </c>
+      <c r="B85" s="151" t="s">
+        <v>936</v>
       </c>
       <c r="C85" s="47" t="s">
-        <v>282</v>
+        <v>554</v>
       </c>
       <c r="D85" s="47"/>
       <c r="E85" s="47" t="s">
@@ -65586,10 +66351,10 @@
       <c r="F85" s="43"/>
       <c r="G85" s="47"/>
     </row>
-    <row r="86" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="47"/>
-      <c r="B86" s="51" t="s">
-        <v>82</v>
+      <c r="B86" s="144" t="s">
+        <v>895</v>
       </c>
       <c r="C86" s="47" t="s">
         <v>282</v>
@@ -65601,10 +66366,10 @@
       <c r="F86" s="43"/>
       <c r="G86" s="47"/>
     </row>
-    <row r="87" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="47"/>
-      <c r="B87" s="145" t="s">
-        <v>81</v>
+      <c r="B87" s="151" t="s">
+        <v>900</v>
       </c>
       <c r="C87" s="47" t="s">
         <v>282</v>
@@ -65616,10 +66381,10 @@
       <c r="F87" s="43"/>
       <c r="G87" s="47"/>
     </row>
-    <row r="88" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="47"/>
-      <c r="B88" s="157" t="s">
-        <v>929</v>
+      <c r="B88" s="144" t="s">
+        <v>901</v>
       </c>
       <c r="C88" s="47" t="s">
         <v>282</v>
@@ -65631,10 +66396,10 @@
       <c r="F88" s="43"/>
       <c r="G88" s="47"/>
     </row>
-    <row r="89" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="47"/>
-      <c r="B89" s="151" t="s">
-        <v>933</v>
+      <c r="B89" s="146" t="s">
+        <v>90</v>
       </c>
       <c r="C89" s="47" t="s">
         <v>282</v>
@@ -65646,25 +66411,25 @@
       <c r="F89" s="43"/>
       <c r="G89" s="47"/>
     </row>
-    <row r="90" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="47"/>
-      <c r="B90" s="51" t="s">
-        <v>938</v>
-      </c>
-      <c r="C90" s="47" t="s">
-        <v>282</v>
-      </c>
-      <c r="D90" s="47"/>
-      <c r="E90" s="47" t="s">
-        <v>479</v>
-      </c>
-      <c r="F90" s="43"/>
-      <c r="G90" s="47"/>
-    </row>
-    <row r="91" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="121"/>
+      <c r="B90" s="142" t="s">
+        <v>55</v>
+      </c>
+      <c r="C90" s="121" t="s">
+        <v>282</v>
+      </c>
+      <c r="D90" s="121"/>
+      <c r="E90" s="121"/>
+      <c r="F90" s="122" t="s">
+        <v>835</v>
+      </c>
+      <c r="G90" s="152"/>
+    </row>
+    <row r="91" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="47"/>
-      <c r="B91" s="151" t="s">
-        <v>939</v>
+      <c r="B91" s="144" t="s">
+        <v>762</v>
       </c>
       <c r="C91" s="47" t="s">
         <v>282</v>
@@ -65676,10 +66441,10 @@
       <c r="F91" s="43"/>
       <c r="G91" s="47"/>
     </row>
-    <row r="92" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="47"/>
       <c r="B92" s="51" t="s">
-        <v>940</v>
+        <v>82</v>
       </c>
       <c r="C92" s="47" t="s">
         <v>282</v>
@@ -65691,10 +66456,10 @@
       <c r="F92" s="43"/>
       <c r="G92" s="47"/>
     </row>
-    <row r="93" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="47"/>
-      <c r="B93" s="51" t="s">
-        <v>941</v>
+      <c r="B93" s="145" t="s">
+        <v>81</v>
       </c>
       <c r="C93" s="47" t="s">
         <v>282</v>
@@ -65706,10 +66471,10 @@
       <c r="F93" s="43"/>
       <c r="G93" s="47"/>
     </row>
-    <row r="94" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A94" s="47"/>
       <c r="B94" s="151" t="s">
-        <v>942</v>
+        <v>933</v>
       </c>
       <c r="C94" s="47" t="s">
         <v>282</v>
@@ -65721,10 +66486,10 @@
       <c r="F94" s="43"/>
       <c r="G94" s="47"/>
     </row>
-    <row r="95" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="47"/>
-      <c r="B95" s="145" t="s">
-        <v>737</v>
+      <c r="B95" s="51" t="s">
+        <v>938</v>
       </c>
       <c r="C95" s="47" t="s">
         <v>282</v>
@@ -65736,10 +66501,10 @@
       <c r="F95" s="43"/>
       <c r="G95" s="47"/>
     </row>
-    <row r="96" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="47"/>
       <c r="B96" s="151" t="s">
-        <v>957</v>
+        <v>939</v>
       </c>
       <c r="C96" s="47" t="s">
         <v>282</v>
@@ -65751,10 +66516,10 @@
       <c r="F96" s="43"/>
       <c r="G96" s="47"/>
     </row>
-    <row r="97" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="47"/>
-      <c r="B97" s="145" t="s">
-        <v>958</v>
+      <c r="B97" s="51" t="s">
+        <v>940</v>
       </c>
       <c r="C97" s="47" t="s">
         <v>282</v>
@@ -65768,8 +66533,8 @@
     </row>
     <row r="98" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="47"/>
-      <c r="B98" s="151" t="s">
-        <v>964</v>
+      <c r="B98" s="51" t="s">
+        <v>941</v>
       </c>
       <c r="C98" s="47" t="s">
         <v>282</v>
@@ -65781,10 +66546,10 @@
       <c r="F98" s="43"/>
       <c r="G98" s="47"/>
     </row>
-    <row r="99" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="47"/>
       <c r="B99" s="151" t="s">
-        <v>991</v>
+        <v>942</v>
       </c>
       <c r="C99" s="47" t="s">
         <v>282</v>
@@ -65796,10 +66561,10 @@
       <c r="F99" s="43"/>
       <c r="G99" s="47"/>
     </row>
-    <row r="100" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="47"/>
-      <c r="B100" s="51" t="s">
-        <v>139</v>
+      <c r="B100" s="145" t="s">
+        <v>737</v>
       </c>
       <c r="C100" s="47" t="s">
         <v>282</v>
@@ -65811,10 +66576,10 @@
       <c r="F100" s="43"/>
       <c r="G100" s="47"/>
     </row>
-    <row r="101" spans="1:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="47"/>
-      <c r="B101" s="51" t="s">
-        <v>1002</v>
+      <c r="B101" s="151" t="s">
+        <v>957</v>
       </c>
       <c r="C101" s="47" t="s">
         <v>282</v>
@@ -65826,10 +66591,10 @@
       <c r="F101" s="43"/>
       <c r="G101" s="47"/>
     </row>
-    <row r="102" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="47"/>
-      <c r="B102" s="51" t="s">
-        <v>88</v>
+      <c r="B102" s="145" t="s">
+        <v>958</v>
       </c>
       <c r="C102" s="47" t="s">
         <v>282</v>
@@ -65841,10 +66606,10 @@
       <c r="F102" s="43"/>
       <c r="G102" s="47"/>
     </row>
-    <row r="103" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A103" s="47"/>
-      <c r="B103" s="148" t="s">
-        <v>1021</v>
+      <c r="B103" s="151" t="s">
+        <v>991</v>
       </c>
       <c r="C103" s="47" t="s">
         <v>282</v>
@@ -65856,10 +66621,10 @@
       <c r="F103" s="43"/>
       <c r="G103" s="47"/>
     </row>
-    <row r="104" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="47"/>
-      <c r="B104" s="145" t="s">
-        <v>58</v>
+      <c r="B104" s="51" t="s">
+        <v>139</v>
       </c>
       <c r="C104" s="47" t="s">
         <v>282</v>
@@ -65871,10 +66636,10 @@
       <c r="F104" s="43"/>
       <c r="G104" s="47"/>
     </row>
-    <row r="105" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="47"/>
-      <c r="B105" s="144" t="s">
-        <v>1053</v>
+      <c r="B105" s="51" t="s">
+        <v>1002</v>
       </c>
       <c r="C105" s="47" t="s">
         <v>282</v>
@@ -65886,10 +66651,10 @@
       <c r="F105" s="43"/>
       <c r="G105" s="47"/>
     </row>
-    <row r="106" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="47"/>
-      <c r="B106" s="145" t="s">
-        <v>69</v>
+      <c r="B106" s="51" t="s">
+        <v>88</v>
       </c>
       <c r="C106" s="47" t="s">
         <v>282</v>
@@ -65901,10 +66666,10 @@
       <c r="F106" s="43"/>
       <c r="G106" s="47"/>
     </row>
-    <row r="107" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="47"/>
-      <c r="B107" s="51" t="s">
-        <v>1054</v>
+      <c r="B107" s="148" t="s">
+        <v>1021</v>
       </c>
       <c r="C107" s="47" t="s">
         <v>282</v>
@@ -65916,10 +66681,10 @@
       <c r="F107" s="43"/>
       <c r="G107" s="47"/>
     </row>
-    <row r="108" spans="1:7" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="47"/>
-      <c r="B108" s="148" t="s">
-        <v>1066</v>
+      <c r="B108" s="145" t="s">
+        <v>58</v>
       </c>
       <c r="C108" s="47" t="s">
         <v>282</v>
@@ -65931,10 +66696,10 @@
       <c r="F108" s="43"/>
       <c r="G108" s="47"/>
     </row>
-    <row r="109" spans="1:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" ht="39" x14ac:dyDescent="0.25">
       <c r="A109" s="47"/>
-      <c r="B109" s="151" t="s">
-        <v>188</v>
+      <c r="B109" s="144" t="s">
+        <v>1053</v>
       </c>
       <c r="C109" s="47" t="s">
         <v>282</v>
@@ -65943,15 +66708,13 @@
       <c r="E109" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F109" s="47" t="s">
-        <v>848</v>
-      </c>
+      <c r="F109" s="43"/>
       <c r="G109" s="47"/>
     </row>
-    <row r="110" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="47"/>
       <c r="B110" s="145" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="C110" s="47" t="s">
         <v>282</v>
@@ -65963,13 +66726,13 @@
       <c r="F110" s="43"/>
       <c r="G110" s="47"/>
     </row>
-    <row r="111" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="47"/>
-      <c r="B111" s="145" t="s">
-        <v>794</v>
+      <c r="B111" s="51" t="s">
+        <v>1054</v>
       </c>
       <c r="C111" s="47" t="s">
-        <v>798</v>
+        <v>282</v>
       </c>
       <c r="D111" s="47"/>
       <c r="E111" s="47" t="s">
@@ -65978,13 +66741,13 @@
       <c r="F111" s="43"/>
       <c r="G111" s="47"/>
     </row>
-    <row r="112" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="47"/>
-      <c r="B112" s="151" t="s">
-        <v>769</v>
+      <c r="B112" s="148" t="s">
+        <v>1066</v>
       </c>
       <c r="C112" s="47" t="s">
-        <v>798</v>
+        <v>282</v>
       </c>
       <c r="D112" s="47"/>
       <c r="E112" s="47" t="s">
@@ -65993,28 +66756,30 @@
       <c r="F112" s="43"/>
       <c r="G112" s="47"/>
     </row>
-    <row r="113" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A113" s="47"/>
-      <c r="B113" s="143" t="s">
-        <v>775</v>
+      <c r="B113" s="151" t="s">
+        <v>188</v>
       </c>
       <c r="C113" s="47" t="s">
-        <v>798</v>
+        <v>282</v>
       </c>
       <c r="D113" s="47"/>
       <c r="E113" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F113" s="43"/>
+      <c r="F113" s="47" t="s">
+        <v>1270</v>
+      </c>
       <c r="G113" s="47"/>
     </row>
-    <row r="114" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="47"/>
       <c r="B114" s="145" t="s">
-        <v>783</v>
+        <v>80</v>
       </c>
       <c r="C114" s="47" t="s">
-        <v>798</v>
+        <v>282</v>
       </c>
       <c r="D114" s="47"/>
       <c r="E114" s="47" t="s">
@@ -66023,10 +66788,10 @@
       <c r="F114" s="43"/>
       <c r="G114" s="47"/>
     </row>
-    <row r="115" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="47"/>
-      <c r="B115" s="144" t="s">
-        <v>768</v>
+      <c r="B115" s="151" t="s">
+        <v>769</v>
       </c>
       <c r="C115" s="47" t="s">
         <v>798</v>
@@ -66035,18 +66800,16 @@
       <c r="E115" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F115" s="43" t="s">
-        <v>846</v>
-      </c>
+      <c r="F115" s="43"/>
       <c r="G115" s="47"/>
     </row>
-    <row r="116" spans="1:7" ht="39" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A116" s="47"/>
-      <c r="B116" s="144" t="s">
-        <v>865</v>
+      <c r="B116" s="143" t="s">
+        <v>775</v>
       </c>
       <c r="C116" s="47" t="s">
-        <v>554</v>
+        <v>798</v>
       </c>
       <c r="D116" s="47"/>
       <c r="E116" s="47" t="s">
@@ -66055,13 +66818,13 @@
       <c r="F116" s="43"/>
       <c r="G116" s="47"/>
     </row>
-    <row r="117" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="47"/>
-      <c r="B117" s="151" t="s">
-        <v>935</v>
+      <c r="B117" s="145" t="s">
+        <v>783</v>
       </c>
       <c r="C117" s="47" t="s">
-        <v>554</v>
+        <v>798</v>
       </c>
       <c r="D117" s="47"/>
       <c r="E117" s="47" t="s">
@@ -66070,25 +66833,27 @@
       <c r="F117" s="43"/>
       <c r="G117" s="47"/>
     </row>
-    <row r="118" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="47"/>
-      <c r="B118" s="151" t="s">
-        <v>936</v>
+      <c r="B118" s="144" t="s">
+        <v>768</v>
       </c>
       <c r="C118" s="47" t="s">
-        <v>554</v>
+        <v>798</v>
       </c>
       <c r="D118" s="47"/>
       <c r="E118" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F118" s="43"/>
+      <c r="F118" s="43" t="s">
+        <v>846</v>
+      </c>
       <c r="G118" s="47"/>
     </row>
     <row r="119" spans="1:7" ht="39" x14ac:dyDescent="0.25">
       <c r="A119" s="47"/>
       <c r="B119" s="144" t="s">
-        <v>937</v>
+        <v>865</v>
       </c>
       <c r="C119" s="47" t="s">
         <v>554</v>
@@ -66100,10 +66865,10 @@
       <c r="F119" s="43"/>
       <c r="G119" s="47"/>
     </row>
-    <row r="120" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="47"/>
-      <c r="B120" s="144" t="s">
-        <v>943</v>
+      <c r="B120" s="151" t="s">
+        <v>1252</v>
       </c>
       <c r="C120" s="47" t="s">
         <v>554</v>
@@ -66115,10 +66880,10 @@
       <c r="F120" s="43"/>
       <c r="G120" s="47"/>
     </row>
-    <row r="121" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="47"/>
-      <c r="B121" s="144" t="s">
-        <v>944</v>
+      <c r="B121" s="151" t="s">
+        <v>935</v>
       </c>
       <c r="C121" s="47" t="s">
         <v>554</v>
@@ -66130,10 +66895,10 @@
       <c r="F121" s="43"/>
       <c r="G121" s="47"/>
     </row>
-    <row r="122" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" ht="39" x14ac:dyDescent="0.25">
       <c r="A122" s="47"/>
       <c r="B122" s="144" t="s">
-        <v>960</v>
+        <v>937</v>
       </c>
       <c r="C122" s="47" t="s">
         <v>554</v>
@@ -66145,27 +66910,25 @@
       <c r="F122" s="43"/>
       <c r="G122" s="47"/>
     </row>
-    <row r="123" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A123" s="46"/>
-      <c r="B123" s="153" t="s">
-        <v>985</v>
-      </c>
-      <c r="C123" s="46" t="s">
+    <row r="123" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="47"/>
+      <c r="B123" s="144" t="s">
+        <v>943</v>
+      </c>
+      <c r="C123" s="47" t="s">
         <v>554</v>
       </c>
-      <c r="D123" s="46"/>
-      <c r="E123" s="46" t="s">
+      <c r="D123" s="47"/>
+      <c r="E123" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F123" s="46" t="s">
-        <v>1148</v>
-      </c>
-      <c r="G123" s="46"/>
+      <c r="F123" s="43"/>
+      <c r="G123" s="47"/>
     </row>
     <row r="124" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A124" s="47"/>
       <c r="B124" s="144" t="s">
-        <v>1081</v>
+        <v>944</v>
       </c>
       <c r="C124" s="47" t="s">
         <v>554</v>
@@ -66177,11 +66940,63 @@
       <c r="F124" s="43"/>
       <c r="G124" s="47"/>
     </row>
+    <row r="125" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A125" s="47"/>
+      <c r="B125" s="144" t="s">
+        <v>960</v>
+      </c>
+      <c r="C125" s="47" t="s">
+        <v>554</v>
+      </c>
+      <c r="D125" s="47"/>
+      <c r="E125" s="47" t="s">
+        <v>479</v>
+      </c>
+      <c r="F125" s="43"/>
+      <c r="G125" s="47"/>
+    </row>
+    <row r="126" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A126" s="46"/>
+      <c r="B126" s="153" t="s">
+        <v>985</v>
+      </c>
+      <c r="C126" s="46" t="s">
+        <v>554</v>
+      </c>
+      <c r="D126" s="46"/>
+      <c r="E126" s="46" t="s">
+        <v>479</v>
+      </c>
+      <c r="F126" s="46" t="s">
+        <v>1148</v>
+      </c>
+      <c r="G126" s="46"/>
+    </row>
+    <row r="127" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A127" s="47"/>
+      <c r="B127" s="144" t="s">
+        <v>1081</v>
+      </c>
+      <c r="C127" s="47" t="s">
+        <v>554</v>
+      </c>
+      <c r="D127" s="47"/>
+      <c r="E127" s="47" t="s">
+        <v>479</v>
+      </c>
+      <c r="F127" s="43"/>
+      <c r="G127" s="47"/>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B128" s="136" t="s">
+        <v>1289</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A3:G124">
-    <sortCondition ref="A3:A124"/>
-    <sortCondition ref="C3:C124"/>
-    <sortCondition ref="B3:B124"/>
+  <sortState ref="A3:G125">
+    <sortCondition ref="A3:A125"/>
+    <sortCondition ref="C3:C125"/>
+    <sortCondition ref="B3:B125"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>

</xml_diff>

<commit_message>
fixed bug + more data
</commit_message>
<xml_diff>
--- a/Literature_search/database.xlsx
+++ b/Literature_search/database.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin Vasilev\SkyDrive\R\reading_sounds\Literature_search\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7515" tabRatio="987" activeTab="8"/>
   </bookViews>
@@ -27,7 +22,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">' Step 2'!$A$2:$D$526</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">' Step 3'!$A$2:$C$344</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">' Step 4 (meta)'!$A$2:$C$125</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">' Step 4 (meta)'!$A$2:$C$128</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -39,7 +34,7 @@
     <author>Martin R. Vasilev</author>
   </authors>
   <commentList>
-    <comment ref="B19" authorId="0" shapeId="0">
+    <comment ref="B19" authorId="0">
       <text>
         <r>
           <rPr>
@@ -74,7 +69,7 @@
     <author>Martin R. Vasilev</author>
   </authors>
   <commentList>
-    <comment ref="B219" authorId="0" shapeId="0">
+    <comment ref="B219" authorId="0">
       <text>
         <r>
           <rPr>
@@ -110,7 +105,7 @@
     <author>Martin R. Vasilev</author>
   </authors>
   <commentList>
-    <comment ref="D2" authorId="0" shapeId="0">
+    <comment ref="D2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -134,7 +129,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D67" authorId="0" shapeId="0">
+    <comment ref="D67" authorId="0">
       <text>
         <r>
           <rPr>
@@ -159,7 +154,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B135" authorId="1" shapeId="0">
+    <comment ref="B135" authorId="1">
       <text>
         <r>
           <rPr>
@@ -194,7 +189,7 @@
     <author>Martin,Vasilev</author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0" shapeId="0">
+    <comment ref="B2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -218,7 +213,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F9" authorId="0" shapeId="0">
+    <comment ref="F9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -242,7 +237,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F12" authorId="0" shapeId="0">
+    <comment ref="F12" authorId="0">
       <text>
         <r>
           <rPr>
@@ -266,7 +261,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G21" authorId="0" shapeId="0">
+    <comment ref="G21" authorId="0">
       <text>
         <r>
           <rPr>
@@ -291,7 +286,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G22" authorId="0" shapeId="0">
+    <comment ref="G22" authorId="0">
       <text>
         <r>
           <rPr>
@@ -319,7 +314,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G41" authorId="0" shapeId="0">
+    <comment ref="G41" authorId="0">
       <text>
         <r>
           <rPr>
@@ -344,7 +339,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G60" authorId="0" shapeId="0">
+    <comment ref="G60" authorId="0">
       <text>
         <r>
           <rPr>
@@ -371,7 +366,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B62" authorId="0" shapeId="0">
+    <comment ref="B62" authorId="0">
       <text>
         <r>
           <rPr>
@@ -396,7 +391,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F63" authorId="0" shapeId="0">
+    <comment ref="F63" authorId="0">
       <text>
         <r>
           <rPr>
@@ -420,7 +415,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B67" authorId="0" shapeId="0">
+    <comment ref="B67" authorId="0">
       <text>
         <r>
           <rPr>
@@ -445,7 +440,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B68" authorId="0" shapeId="0">
+    <comment ref="B68" authorId="0">
       <text>
         <r>
           <rPr>
@@ -470,7 +465,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D69" authorId="0" shapeId="0">
+    <comment ref="D69" authorId="0">
       <text>
         <r>
           <rPr>
@@ -494,7 +489,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G69" authorId="0" shapeId="0">
+    <comment ref="G69" authorId="0">
       <text>
         <r>
           <rPr>
@@ -518,7 +513,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G70" authorId="0" shapeId="0">
+    <comment ref="G70" authorId="0">
       <text>
         <r>
           <rPr>
@@ -543,7 +538,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G71" authorId="0" shapeId="0">
+    <comment ref="G71" authorId="0">
       <text>
         <r>
           <rPr>
@@ -568,7 +563,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D72" authorId="0" shapeId="0">
+    <comment ref="D72" authorId="0">
       <text>
         <r>
           <rPr>
@@ -592,7 +587,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F73" authorId="0" shapeId="0">
+    <comment ref="F73" authorId="0">
       <text>
         <r>
           <rPr>
@@ -616,7 +611,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F77" authorId="0" shapeId="0">
+    <comment ref="F77" authorId="0">
       <text>
         <r>
           <rPr>
@@ -641,7 +636,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D79" authorId="0" shapeId="0">
+    <comment ref="D79" authorId="0">
       <text>
         <r>
           <rPr>
@@ -665,7 +660,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B84" authorId="0" shapeId="0">
+    <comment ref="B84" authorId="0">
       <text>
         <r>
           <rPr>
@@ -699,7 +694,7 @@
     <author>Martin,Vasilev</author>
   </authors>
   <commentList>
-    <comment ref="D175" authorId="0" shapeId="0">
+    <comment ref="D175" authorId="0">
       <text>
         <r>
           <rPr>
@@ -733,7 +728,7 @@
     <author>Martin R. Vasilev</author>
   </authors>
   <commentList>
-    <comment ref="B73" authorId="0" shapeId="0">
+    <comment ref="B73" authorId="0">
       <text>
         <r>
           <rPr>
@@ -763,7 +758,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5638" uniqueCount="1320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5063" uniqueCount="1332">
   <si>
     <t>ID</t>
   </si>
@@ -37932,11 +37927,227 @@
   <si>
     <t>for reading speed, I take average of 1st and second pass;  participants brought their own music for the preferred condition</t>
   </si>
+  <si>
+    <r>
+      <t>Hyönä, J., &amp; Ekholm, M. (2016). Background Speech Effects on Sentence Processing during Reading: An Eye Movement Study. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>PloS one</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(3), e0152133., </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Experiment 1</t>
+    </r>
+  </si>
+  <si>
+    <t>3 (background: silence, Finnish speech, Italian speech) x 2(sentence: complex, less complex)</t>
+  </si>
+  <si>
+    <t>syntactic complexity is averaged out; reading speed calculated as first-pass + lookback fixations</t>
+  </si>
+  <si>
+    <r>
+      <t>Hyönä, J., &amp; Ekholm, M. (2016). Background Speech Effects on Sentence Processing during Reading: An Eye Movement Study. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>PloS one</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(3), e0152133., </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Experiment 2</t>
+    </r>
+  </si>
+  <si>
+    <t>3 (background: silence, scrambled-same speech, scrambled-different speech) x 2(sentence: complex, less complex)</t>
+  </si>
+  <si>
+    <t>syntactic complexity and same-different scrambled speech are averaged out</t>
+  </si>
+  <si>
+    <r>
+      <t>Hyönä, J., &amp; Ekholm, M. (2016). Background Speech Effects on Sentence Processing during Reading: An Eye Movement Study. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>PloS one</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(3), e0152133., </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Experiment 3</t>
+    </r>
+  </si>
+  <si>
+    <t>3 (background: silence, Finnish speech, scrambled-different speech) x 2(sentence: complex, less complex)</t>
+  </si>
+  <si>
+    <t>syntactic complexity is averaged out</t>
+  </si>
+  <si>
+    <r>
+      <t>Hyönä, J., &amp; Ekholm, M. (2016). Background Speech Effects on Sentence Processing during Reading: An Eye Movement Study. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>PloS one</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(3), e0152133., </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Experiment 4</t>
+    </r>
+  </si>
+  <si>
+    <t>3 (background: silence,  scrambled-sem. an. Speech, scrambled-sem.+synt. an. speech) x 2(sentence: complex, less complex)</t>
+  </si>
+  <si>
+    <t>syntactic complexity and type of scrambled speech are averaged out</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="65" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -39014,14 +39225,14 @@
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="50" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -39368,7 +39579,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -50327,7 +50538,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:D20"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -50563,7 +50774,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C62"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView topLeftCell="A35" workbookViewId="0">
       <selection activeCell="C55" sqref="B13:C55"/>
     </sheetView>
   </sheetViews>
@@ -51143,7 +51354,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H71"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
+    <sheetView topLeftCell="A55" workbookViewId="0">
       <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
@@ -51154,14 +51365,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="164"/>
-      <c r="B1" s="164"/>
-      <c r="C1" s="164"/>
-      <c r="D1" s="164"/>
-      <c r="E1" s="164"/>
-      <c r="F1" s="164"/>
-      <c r="G1" s="164"/>
-      <c r="H1" s="164"/>
+      <c r="A1" s="166"/>
+      <c r="B1" s="166"/>
+      <c r="C1" s="166"/>
+      <c r="D1" s="166"/>
+      <c r="E1" s="166"/>
+      <c r="F1" s="166"/>
+      <c r="G1" s="166"/>
+      <c r="H1" s="166"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -64522,10 +64733,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G127"/>
+  <dimension ref="A1:G130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C52" workbookViewId="0">
-      <selection activeCell="F55" sqref="F55"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="G93" sqref="G93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -65249,7 +65460,7 @@
       <c r="A34" s="58">
         <v>32</v>
       </c>
-      <c r="B34" s="166" t="s">
+      <c r="B34" s="165" t="s">
         <v>703</v>
       </c>
       <c r="C34" s="47" t="s">
@@ -66430,7 +66641,7 @@
       <c r="A88" s="58">
         <v>86</v>
       </c>
-      <c r="B88" s="165" t="s">
+      <c r="B88" s="164" t="s">
         <v>90</v>
       </c>
       <c r="C88" s="47" t="s">
@@ -66449,70 +66660,102 @@
         <v>479</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="47"/>
-      <c r="B89" s="144" t="s">
-        <v>895</v>
+    <row r="89" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="58">
+        <v>87</v>
+      </c>
+      <c r="B89" s="150" t="s">
+        <v>1320</v>
       </c>
       <c r="C89" s="47" t="s">
-        <v>282</v>
-      </c>
-      <c r="D89" s="47"/>
-      <c r="E89" s="47" t="s">
+        <v>554</v>
+      </c>
+      <c r="D89" s="61" t="s">
+        <v>1321</v>
+      </c>
+      <c r="E89" s="58" t="s">
+        <v>1127</v>
+      </c>
+      <c r="F89" s="61" t="s">
+        <v>1322</v>
+      </c>
+      <c r="G89" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F89" s="43"/>
-      <c r="G89" s="47"/>
-    </row>
-    <row r="90" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="47"/>
+    </row>
+    <row r="90" spans="1:7" ht="78" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="58">
+        <v>88</v>
+      </c>
       <c r="B90" s="150" t="s">
-        <v>900</v>
+        <v>1323</v>
       </c>
       <c r="C90" s="47" t="s">
-        <v>282</v>
-      </c>
-      <c r="D90" s="47"/>
-      <c r="E90" s="47" t="s">
+        <v>554</v>
+      </c>
+      <c r="D90" s="61" t="s">
+        <v>1324</v>
+      </c>
+      <c r="E90" s="58" t="s">
+        <v>1127</v>
+      </c>
+      <c r="F90" s="61" t="s">
+        <v>1325</v>
+      </c>
+      <c r="G90" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F90" s="43"/>
-      <c r="G90" s="47"/>
-    </row>
-    <row r="91" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="47"/>
-      <c r="B91" s="144" t="s">
-        <v>901</v>
+    </row>
+    <row r="91" spans="1:7" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="58">
+        <v>89</v>
+      </c>
+      <c r="B91" s="150" t="s">
+        <v>1326</v>
       </c>
       <c r="C91" s="47" t="s">
-        <v>282</v>
-      </c>
-      <c r="D91" s="47"/>
-      <c r="E91" s="47" t="s">
+        <v>554</v>
+      </c>
+      <c r="D91" s="61" t="s">
+        <v>1327</v>
+      </c>
+      <c r="E91" s="58" t="s">
+        <v>1127</v>
+      </c>
+      <c r="F91" s="61" t="s">
+        <v>1328</v>
+      </c>
+      <c r="G91" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F91" s="43"/>
-      <c r="G91" s="47"/>
-    </row>
-    <row r="92" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="121"/>
-      <c r="B92" s="142" t="s">
-        <v>55</v>
-      </c>
-      <c r="C92" s="121" t="s">
-        <v>282</v>
-      </c>
-      <c r="D92" s="121"/>
-      <c r="E92" s="121"/>
-      <c r="F92" s="122" t="s">
-        <v>835</v>
-      </c>
-      <c r="G92" s="151"/>
-    </row>
-    <row r="93" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="92" spans="1:7" s="43" customFormat="1" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="47">
+        <v>90</v>
+      </c>
+      <c r="B92" s="150" t="s">
+        <v>1329</v>
+      </c>
+      <c r="C92" s="47" t="s">
+        <v>554</v>
+      </c>
+      <c r="D92" s="61" t="s">
+        <v>1330</v>
+      </c>
+      <c r="E92" s="58" t="s">
+        <v>1127</v>
+      </c>
+      <c r="F92" s="61" t="s">
+        <v>1331</v>
+      </c>
+      <c r="G92" s="47" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="47"/>
       <c r="B93" s="144" t="s">
-        <v>762</v>
+        <v>895</v>
       </c>
       <c r="C93" s="47" t="s">
         <v>282</v>
@@ -66524,10 +66767,10 @@
       <c r="F93" s="43"/>
       <c r="G93" s="47"/>
     </row>
-    <row r="94" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="47"/>
-      <c r="B94" s="51" t="s">
-        <v>82</v>
+      <c r="B94" s="150" t="s">
+        <v>900</v>
       </c>
       <c r="C94" s="47" t="s">
         <v>282</v>
@@ -66539,10 +66782,10 @@
       <c r="F94" s="43"/>
       <c r="G94" s="47"/>
     </row>
-    <row r="95" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="47"/>
-      <c r="B95" s="145" t="s">
-        <v>81</v>
+      <c r="B95" s="144" t="s">
+        <v>901</v>
       </c>
       <c r="C95" s="47" t="s">
         <v>282</v>
@@ -66554,25 +66797,25 @@
       <c r="F95" s="43"/>
       <c r="G95" s="47"/>
     </row>
-    <row r="96" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="47"/>
-      <c r="B96" s="150" t="s">
-        <v>933</v>
-      </c>
-      <c r="C96" s="47" t="s">
+    <row r="96" spans="1:7" ht="39" x14ac:dyDescent="0.25">
+      <c r="A96" s="121"/>
+      <c r="B96" s="142" t="s">
+        <v>55</v>
+      </c>
+      <c r="C96" s="121" t="s">
         <v>282</v>
       </c>
-      <c r="D96" s="47"/>
-      <c r="E96" s="47" t="s">
-        <v>479</v>
-      </c>
-      <c r="F96" s="43"/>
-      <c r="G96" s="47"/>
-    </row>
-    <row r="97" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D96" s="121"/>
+      <c r="E96" s="121"/>
+      <c r="F96" s="122" t="s">
+        <v>835</v>
+      </c>
+      <c r="G96" s="151"/>
+    </row>
+    <row r="97" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="47"/>
-      <c r="B97" s="51" t="s">
-        <v>938</v>
+      <c r="B97" s="144" t="s">
+        <v>762</v>
       </c>
       <c r="C97" s="47" t="s">
         <v>282</v>
@@ -66584,10 +66827,10 @@
       <c r="F97" s="43"/>
       <c r="G97" s="47"/>
     </row>
-    <row r="98" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="47"/>
-      <c r="B98" s="150" t="s">
-        <v>939</v>
+      <c r="B98" s="51" t="s">
+        <v>82</v>
       </c>
       <c r="C98" s="47" t="s">
         <v>282</v>
@@ -66599,10 +66842,10 @@
       <c r="F98" s="43"/>
       <c r="G98" s="47"/>
     </row>
-    <row r="99" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="47"/>
-      <c r="B99" s="51" t="s">
-        <v>940</v>
+      <c r="B99" s="145" t="s">
+        <v>81</v>
       </c>
       <c r="C99" s="47" t="s">
         <v>282</v>
@@ -66616,8 +66859,8 @@
     </row>
     <row r="100" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="47"/>
-      <c r="B100" s="51" t="s">
-        <v>941</v>
+      <c r="B100" s="150" t="s">
+        <v>933</v>
       </c>
       <c r="C100" s="47" t="s">
         <v>282</v>
@@ -66629,10 +66872,10 @@
       <c r="F100" s="43"/>
       <c r="G100" s="47"/>
     </row>
-    <row r="101" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="47"/>
-      <c r="B101" s="145" t="s">
-        <v>737</v>
+      <c r="B101" s="51" t="s">
+        <v>938</v>
       </c>
       <c r="C101" s="47" t="s">
         <v>282</v>
@@ -66644,10 +66887,10 @@
       <c r="F101" s="43"/>
       <c r="G101" s="47"/>
     </row>
-    <row r="102" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="47"/>
       <c r="B102" s="150" t="s">
-        <v>957</v>
+        <v>939</v>
       </c>
       <c r="C102" s="47" t="s">
         <v>282</v>
@@ -66659,10 +66902,10 @@
       <c r="F102" s="43"/>
       <c r="G102" s="47"/>
     </row>
-    <row r="103" spans="1:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="47"/>
-      <c r="B103" s="145" t="s">
-        <v>958</v>
+      <c r="B103" s="51" t="s">
+        <v>940</v>
       </c>
       <c r="C103" s="47" t="s">
         <v>282</v>
@@ -66674,10 +66917,10 @@
       <c r="F103" s="43"/>
       <c r="G103" s="47"/>
     </row>
-    <row r="104" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="47"/>
-      <c r="B104" s="150" t="s">
-        <v>991</v>
+      <c r="B104" s="51" t="s">
+        <v>941</v>
       </c>
       <c r="C104" s="47" t="s">
         <v>282</v>
@@ -66689,10 +66932,10 @@
       <c r="F104" s="43"/>
       <c r="G104" s="47"/>
     </row>
-    <row r="105" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A105" s="47"/>
-      <c r="B105" s="51" t="s">
-        <v>139</v>
+      <c r="B105" s="145" t="s">
+        <v>737</v>
       </c>
       <c r="C105" s="47" t="s">
         <v>282</v>
@@ -66704,10 +66947,10 @@
       <c r="F105" s="43"/>
       <c r="G105" s="47"/>
     </row>
-    <row r="106" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="47"/>
-      <c r="B106" s="51" t="s">
-        <v>1002</v>
+      <c r="B106" s="150" t="s">
+        <v>957</v>
       </c>
       <c r="C106" s="47" t="s">
         <v>282</v>
@@ -66719,10 +66962,10 @@
       <c r="F106" s="43"/>
       <c r="G106" s="47"/>
     </row>
-    <row r="107" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="47"/>
-      <c r="B107" s="51" t="s">
-        <v>88</v>
+      <c r="B107" s="145" t="s">
+        <v>958</v>
       </c>
       <c r="C107" s="47" t="s">
         <v>282</v>
@@ -66734,10 +66977,10 @@
       <c r="F107" s="43"/>
       <c r="G107" s="47"/>
     </row>
-    <row r="108" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="47"/>
-      <c r="B108" s="147" t="s">
-        <v>1021</v>
+      <c r="B108" s="150" t="s">
+        <v>991</v>
       </c>
       <c r="C108" s="47" t="s">
         <v>282</v>
@@ -66749,10 +66992,10 @@
       <c r="F108" s="43"/>
       <c r="G108" s="47"/>
     </row>
-    <row r="109" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="47"/>
-      <c r="B109" s="145" t="s">
-        <v>58</v>
+      <c r="B109" s="51" t="s">
+        <v>139</v>
       </c>
       <c r="C109" s="47" t="s">
         <v>282</v>
@@ -66764,10 +67007,10 @@
       <c r="F109" s="43"/>
       <c r="G109" s="47"/>
     </row>
-    <row r="110" spans="1:7" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="47"/>
-      <c r="B110" s="144" t="s">
-        <v>1053</v>
+      <c r="B110" s="51" t="s">
+        <v>1002</v>
       </c>
       <c r="C110" s="47" t="s">
         <v>282</v>
@@ -66779,10 +67022,10 @@
       <c r="F110" s="43"/>
       <c r="G110" s="47"/>
     </row>
-    <row r="111" spans="1:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" ht="39" x14ac:dyDescent="0.25">
       <c r="A111" s="47"/>
       <c r="B111" s="51" t="s">
-        <v>1054</v>
+        <v>88</v>
       </c>
       <c r="C111" s="47" t="s">
         <v>282</v>
@@ -66794,10 +67037,10 @@
       <c r="F111" s="43"/>
       <c r="G111" s="47"/>
     </row>
-    <row r="112" spans="1:7" ht="39" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="47"/>
       <c r="B112" s="147" t="s">
-        <v>1066</v>
+        <v>1021</v>
       </c>
       <c r="C112" s="47" t="s">
         <v>282</v>
@@ -66809,10 +67052,10 @@
       <c r="F112" s="43"/>
       <c r="G112" s="47"/>
     </row>
-    <row r="113" spans="1:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="47"/>
-      <c r="B113" s="150" t="s">
-        <v>188</v>
+      <c r="B113" s="145" t="s">
+        <v>58</v>
       </c>
       <c r="C113" s="47" t="s">
         <v>282</v>
@@ -66821,15 +67064,13 @@
       <c r="E113" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F113" s="47" t="s">
-        <v>1269</v>
-      </c>
+      <c r="F113" s="43"/>
       <c r="G113" s="47"/>
     </row>
-    <row r="114" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="47"/>
-      <c r="B114" s="145" t="s">
-        <v>80</v>
+      <c r="B114" s="144" t="s">
+        <v>1053</v>
       </c>
       <c r="C114" s="47" t="s">
         <v>282</v>
@@ -66841,13 +67082,13 @@
       <c r="F114" s="43"/>
       <c r="G114" s="47"/>
     </row>
-    <row r="115" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" ht="39" x14ac:dyDescent="0.25">
       <c r="A115" s="47"/>
-      <c r="B115" s="150" t="s">
-        <v>769</v>
+      <c r="B115" s="51" t="s">
+        <v>1054</v>
       </c>
       <c r="C115" s="47" t="s">
-        <v>798</v>
+        <v>282</v>
       </c>
       <c r="D115" s="47"/>
       <c r="E115" s="47" t="s">
@@ -66856,13 +67097,13 @@
       <c r="F115" s="43"/>
       <c r="G115" s="47"/>
     </row>
-    <row r="116" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="47"/>
-      <c r="B116" s="143" t="s">
-        <v>775</v>
+      <c r="B116" s="147" t="s">
+        <v>1066</v>
       </c>
       <c r="C116" s="47" t="s">
-        <v>798</v>
+        <v>282</v>
       </c>
       <c r="D116" s="47"/>
       <c r="E116" s="47" t="s">
@@ -66871,45 +67112,45 @@
       <c r="F116" s="43"/>
       <c r="G116" s="47"/>
     </row>
-    <row r="117" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="47"/>
-      <c r="B117" s="145" t="s">
-        <v>783</v>
+      <c r="B117" s="150" t="s">
+        <v>188</v>
       </c>
       <c r="C117" s="47" t="s">
-        <v>798</v>
+        <v>282</v>
       </c>
       <c r="D117" s="47"/>
       <c r="E117" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F117" s="43"/>
+      <c r="F117" s="47" t="s">
+        <v>1269</v>
+      </c>
       <c r="G117" s="47"/>
     </row>
-    <row r="118" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A118" s="47"/>
-      <c r="B118" s="144" t="s">
-        <v>768</v>
+      <c r="B118" s="145" t="s">
+        <v>80</v>
       </c>
       <c r="C118" s="47" t="s">
-        <v>798</v>
+        <v>282</v>
       </c>
       <c r="D118" s="47"/>
       <c r="E118" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F118" s="43" t="s">
-        <v>846</v>
-      </c>
+      <c r="F118" s="43"/>
       <c r="G118" s="47"/>
     </row>
-    <row r="119" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="47"/>
-      <c r="B119" s="144" t="s">
-        <v>865</v>
+      <c r="B119" s="150" t="s">
+        <v>769</v>
       </c>
       <c r="C119" s="47" t="s">
-        <v>554</v>
+        <v>798</v>
       </c>
       <c r="D119" s="47"/>
       <c r="E119" s="47" t="s">
@@ -66918,13 +67159,13 @@
       <c r="F119" s="43"/>
       <c r="G119" s="47"/>
     </row>
-    <row r="120" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="47"/>
-      <c r="B120" s="150" t="s">
-        <v>1251</v>
+      <c r="B120" s="143" t="s">
+        <v>775</v>
       </c>
       <c r="C120" s="47" t="s">
-        <v>554</v>
+        <v>798</v>
       </c>
       <c r="D120" s="47"/>
       <c r="E120" s="47" t="s">
@@ -66933,13 +67174,13 @@
       <c r="F120" s="43"/>
       <c r="G120" s="47"/>
     </row>
-    <row r="121" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A121" s="47"/>
-      <c r="B121" s="150" t="s">
-        <v>935</v>
+      <c r="B121" s="145" t="s">
+        <v>783</v>
       </c>
       <c r="C121" s="47" t="s">
-        <v>554</v>
+        <v>798</v>
       </c>
       <c r="D121" s="47"/>
       <c r="E121" s="47" t="s">
@@ -66948,25 +67189,27 @@
       <c r="F121" s="43"/>
       <c r="G121" s="47"/>
     </row>
-    <row r="122" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="47"/>
       <c r="B122" s="144" t="s">
-        <v>937</v>
+        <v>768</v>
       </c>
       <c r="C122" s="47" t="s">
-        <v>554</v>
+        <v>798</v>
       </c>
       <c r="D122" s="47"/>
       <c r="E122" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="F122" s="43"/>
+      <c r="F122" s="43" t="s">
+        <v>846</v>
+      </c>
       <c r="G122" s="47"/>
     </row>
-    <row r="123" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="47"/>
       <c r="B123" s="144" t="s">
-        <v>943</v>
+        <v>865</v>
       </c>
       <c r="C123" s="47" t="s">
         <v>554</v>
@@ -66978,10 +67221,10 @@
       <c r="F123" s="43"/>
       <c r="G123" s="47"/>
     </row>
-    <row r="124" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A124" s="47"/>
-      <c r="B124" s="144" t="s">
-        <v>944</v>
+      <c r="B124" s="150" t="s">
+        <v>1251</v>
       </c>
       <c r="C124" s="47" t="s">
         <v>554</v>
@@ -66993,10 +67236,10 @@
       <c r="F124" s="43"/>
       <c r="G124" s="47"/>
     </row>
-    <row r="125" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="47"/>
-      <c r="B125" s="144" t="s">
-        <v>960</v>
+      <c r="B125" s="150" t="s">
+        <v>935</v>
       </c>
       <c r="C125" s="47" t="s">
         <v>554</v>
@@ -67008,33 +67251,78 @@
       <c r="F125" s="43"/>
       <c r="G125" s="47"/>
     </row>
-    <row r="126" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A126" s="46"/>
-      <c r="B126" s="152" t="s">
+    <row r="126" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="47"/>
+      <c r="B126" s="144" t="s">
+        <v>937</v>
+      </c>
+      <c r="C126" s="47" t="s">
+        <v>554</v>
+      </c>
+      <c r="D126" s="47"/>
+      <c r="E126" s="47" t="s">
+        <v>479</v>
+      </c>
+      <c r="F126" s="43"/>
+      <c r="G126" s="47"/>
+    </row>
+    <row r="127" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A127" s="47"/>
+      <c r="B127" s="144" t="s">
+        <v>943</v>
+      </c>
+      <c r="C127" s="47" t="s">
+        <v>554</v>
+      </c>
+      <c r="D127" s="47"/>
+      <c r="E127" s="47" t="s">
+        <v>479</v>
+      </c>
+      <c r="F127" s="43"/>
+      <c r="G127" s="47"/>
+    </row>
+    <row r="128" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A128" s="47"/>
+      <c r="B128" s="144" t="s">
+        <v>944</v>
+      </c>
+      <c r="C128" s="47" t="s">
+        <v>554</v>
+      </c>
+      <c r="D128" s="47"/>
+      <c r="E128" s="47" t="s">
+        <v>479</v>
+      </c>
+      <c r="F128" s="43"/>
+      <c r="G128" s="47"/>
+    </row>
+    <row r="129" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A129" s="46"/>
+      <c r="B129" s="152" t="s">
         <v>985</v>
       </c>
-      <c r="C126" s="46" t="s">
+      <c r="C129" s="46" t="s">
         <v>554</v>
       </c>
-      <c r="D126" s="46"/>
-      <c r="E126" s="46" t="s">
+      <c r="D129" s="46"/>
+      <c r="E129" s="46" t="s">
         <v>479</v>
       </c>
-      <c r="F126" s="46" t="s">
+      <c r="F129" s="46" t="s">
         <v>1148</v>
       </c>
-      <c r="G126" s="46"/>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B127" s="136" t="s">
+      <c r="G129" s="46"/>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B130" s="136" t="s">
         <v>1288</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A3:G128">
-    <sortCondition ref="A3:A128"/>
-    <sortCondition ref="C3:C128"/>
-    <sortCondition ref="B3:B128"/>
+  <sortState ref="A3:G127">
+    <sortCondition ref="A3:A127"/>
+    <sortCondition ref="C3:C127"/>
+    <sortCondition ref="B3:B127"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>

</xml_diff>

<commit_message>
finished with experimental studies
</commit_message>
<xml_diff>
--- a/Literature_search/database.xlsx
+++ b/Literature_search/database.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin Vasilev\SkyDrive\R\reading_sounds\Literature_search\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="60" windowWidth="20490" windowHeight="7455" tabRatio="987" activeTab="8"/>
   </bookViews>
@@ -39,7 +34,7 @@
     <author>Martin R. Vasilev</author>
   </authors>
   <commentList>
-    <comment ref="B19" authorId="0" shapeId="0">
+    <comment ref="B19" authorId="0">
       <text>
         <r>
           <rPr>
@@ -74,7 +69,7 @@
     <author>Martin R. Vasilev</author>
   </authors>
   <commentList>
-    <comment ref="B219" authorId="0" shapeId="0">
+    <comment ref="B219" authorId="0">
       <text>
         <r>
           <rPr>
@@ -110,7 +105,7 @@
     <author>Martin R. Vasilev</author>
   </authors>
   <commentList>
-    <comment ref="D2" authorId="0" shapeId="0">
+    <comment ref="D2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -134,7 +129,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D67" authorId="0" shapeId="0">
+    <comment ref="D67" authorId="0">
       <text>
         <r>
           <rPr>
@@ -159,7 +154,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B135" authorId="1" shapeId="0">
+    <comment ref="B135" authorId="1">
       <text>
         <r>
           <rPr>
@@ -195,7 +190,7 @@
     <author>Martin R. Vasilev</author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0" shapeId="0">
+    <comment ref="B2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -219,7 +214,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F9" authorId="0" shapeId="0">
+    <comment ref="F9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -243,7 +238,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F12" authorId="0" shapeId="0">
+    <comment ref="F12" authorId="0">
       <text>
         <r>
           <rPr>
@@ -267,7 +262,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G21" authorId="0" shapeId="0">
+    <comment ref="G21" authorId="0">
       <text>
         <r>
           <rPr>
@@ -292,7 +287,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G22" authorId="0" shapeId="0">
+    <comment ref="G22" authorId="0">
       <text>
         <r>
           <rPr>
@@ -320,7 +315,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G41" authorId="0" shapeId="0">
+    <comment ref="G41" authorId="0">
       <text>
         <r>
           <rPr>
@@ -345,7 +340,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G60" authorId="0" shapeId="0">
+    <comment ref="G60" authorId="0">
       <text>
         <r>
           <rPr>
@@ -372,7 +367,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B62" authorId="0" shapeId="0">
+    <comment ref="B62" authorId="0">
       <text>
         <r>
           <rPr>
@@ -397,7 +392,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F63" authorId="0" shapeId="0">
+    <comment ref="F63" authorId="0">
       <text>
         <r>
           <rPr>
@@ -421,7 +416,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B67" authorId="0" shapeId="0">
+    <comment ref="B67" authorId="0">
       <text>
         <r>
           <rPr>
@@ -446,7 +441,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B68" authorId="0" shapeId="0">
+    <comment ref="B68" authorId="0">
       <text>
         <r>
           <rPr>
@@ -471,7 +466,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D69" authorId="0" shapeId="0">
+    <comment ref="D69" authorId="0">
       <text>
         <r>
           <rPr>
@@ -495,7 +490,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G69" authorId="0" shapeId="0">
+    <comment ref="G69" authorId="0">
       <text>
         <r>
           <rPr>
@@ -519,7 +514,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G70" authorId="0" shapeId="0">
+    <comment ref="G70" authorId="0">
       <text>
         <r>
           <rPr>
@@ -544,7 +539,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G71" authorId="0" shapeId="0">
+    <comment ref="G71" authorId="0">
       <text>
         <r>
           <rPr>
@@ -569,7 +564,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D72" authorId="0" shapeId="0">
+    <comment ref="D72" authorId="0">
       <text>
         <r>
           <rPr>
@@ -593,7 +588,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F73" authorId="0" shapeId="0">
+    <comment ref="F73" authorId="0">
       <text>
         <r>
           <rPr>
@@ -617,7 +612,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F77" authorId="0" shapeId="0">
+    <comment ref="F77" authorId="0">
       <text>
         <r>
           <rPr>
@@ -642,7 +637,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D79" authorId="0" shapeId="0">
+    <comment ref="D79" authorId="0">
       <text>
         <r>
           <rPr>
@@ -666,7 +661,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B84" authorId="0" shapeId="0">
+    <comment ref="B84" authorId="0">
       <text>
         <r>
           <rPr>
@@ -690,7 +685,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F93" authorId="0" shapeId="0">
+    <comment ref="F93" authorId="0">
       <text>
         <r>
           <rPr>
@@ -714,7 +709,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F94" authorId="0" shapeId="0">
+    <comment ref="F94" authorId="0">
       <text>
         <r>
           <rPr>
@@ -738,7 +733,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G110" authorId="1" shapeId="0">
+    <comment ref="G110" authorId="1">
       <text>
         <r>
           <rPr>
@@ -772,7 +767,7 @@
     <author>Martin,Vasilev</author>
   </authors>
   <commentList>
-    <comment ref="D175" authorId="0" shapeId="0">
+    <comment ref="D175" authorId="0">
       <text>
         <r>
           <rPr>
@@ -806,7 +801,7 @@
     <author>Martin R. Vasilev</author>
   </authors>
   <commentList>
-    <comment ref="B73" authorId="0" shapeId="0">
+    <comment ref="B73" authorId="0">
       <text>
         <r>
           <rPr>
@@ -836,7 +831,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5172" uniqueCount="1375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5175" uniqueCount="1377">
   <si>
     <t>ID</t>
   </si>
@@ -38830,11 +38825,17 @@
       <t>(5), 254</t>
     </r>
   </si>
+  <si>
+    <t>2 (background: silence vs speech) 2 (student ability: over- vs under-achievers)</t>
+  </si>
+  <si>
+    <t>student ability levels is averaged out</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="67" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -40300,7 +40301,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -65572,8 +65573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
-      <selection activeCell="A110" sqref="A110"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="G112" sqref="G112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -67998,7 +67999,7 @@
       </c>
     </row>
     <row r="111" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="12">
+      <c r="A111" s="58">
         <v>109</v>
       </c>
       <c r="B111" s="59" t="s">
@@ -68007,11 +68008,18 @@
       <c r="C111" s="47" t="s">
         <v>1353</v>
       </c>
-      <c r="D111" s="61"/>
-      <c r="E111" s="12" t="s">
+      <c r="D111" s="61" t="s">
+        <v>1375</v>
+      </c>
+      <c r="E111" s="58" t="s">
+        <v>1126</v>
+      </c>
+      <c r="F111" s="65" t="s">
+        <v>1376</v>
+      </c>
+      <c r="G111" s="12" t="s">
         <v>479</v>
       </c>
-      <c r="F111" s="65"/>
     </row>
     <row r="112" spans="1:7" ht="39" x14ac:dyDescent="0.25">
       <c r="A112" s="47"/>

</xml_diff>

<commit_message>
more code + data
</commit_message>
<xml_diff>
--- a/Literature_search/database.xlsx
+++ b/Literature_search/database.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin Vasilev\SkyDrive\R\reading_sounds\Literature_search\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="60" windowWidth="20490" windowHeight="7455" tabRatio="987" activeTab="8"/>
   </bookViews>
@@ -34,7 +39,7 @@
     <author>Martin,Vasilev</author>
   </authors>
   <commentList>
-    <comment ref="D2" authorId="0">
+    <comment ref="D2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -58,7 +63,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D67" authorId="0">
+    <comment ref="D67" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -94,7 +99,7 @@
     <author>Martin R. Vasilev</author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0">
+    <comment ref="B2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -118,7 +123,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F9" authorId="0">
+    <comment ref="F9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -142,7 +147,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F12" authorId="0">
+    <comment ref="F12" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -166,7 +171,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G21" authorId="0">
+    <comment ref="G21" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -191,7 +196,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G22" authorId="0">
+    <comment ref="G22" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -219,7 +224,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G41" authorId="0">
+    <comment ref="G41" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -244,7 +249,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G60" authorId="0">
+    <comment ref="G60" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -271,7 +276,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B62" authorId="0">
+    <comment ref="B62" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -296,7 +301,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F63" authorId="0">
+    <comment ref="F63" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -320,7 +325,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B67" authorId="0">
+    <comment ref="B67" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -345,7 +350,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B68" authorId="0">
+    <comment ref="B68" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -370,7 +375,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D69" authorId="0">
+    <comment ref="D69" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -394,7 +399,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G69" authorId="0">
+    <comment ref="G69" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -418,7 +423,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G70" authorId="0">
+    <comment ref="G70" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -443,7 +448,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G71" authorId="0">
+    <comment ref="G71" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -468,7 +473,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D72" authorId="0">
+    <comment ref="D72" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -492,7 +497,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F73" authorId="0">
+    <comment ref="F73" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -516,7 +521,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F77" authorId="0">
+    <comment ref="F77" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -541,7 +546,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D79" authorId="0">
+    <comment ref="D79" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -565,7 +570,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B84" authorId="0">
+    <comment ref="B84" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -589,7 +594,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F93" authorId="0">
+    <comment ref="F93" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -613,7 +618,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F94" authorId="0">
+    <comment ref="F94" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -637,7 +642,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G110" authorId="1">
+    <comment ref="G110" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -661,7 +666,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F113" authorId="1">
+    <comment ref="F113" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -685,7 +690,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F115" authorId="0">
+    <comment ref="F115" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -709,7 +714,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G116" authorId="0">
+    <comment ref="G116" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -734,7 +739,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G117" authorId="0">
+    <comment ref="G117" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -759,7 +764,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F119" authorId="0">
+    <comment ref="F119" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -783,7 +788,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G120" authorId="0">
+    <comment ref="G120" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -808,7 +813,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G121" authorId="0">
+    <comment ref="G121" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -836,7 +841,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F122" authorId="0">
+    <comment ref="F122" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -860,7 +865,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G123" authorId="0">
+    <comment ref="G123" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -962,7 +967,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G124" authorId="0">
+    <comment ref="G124" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -986,6 +991,31 @@
         </r>
       </text>
     </comment>
+    <comment ref="G125" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Martin R. Vasilev:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+There is a lot of averaging over across participants as only school-level scores are reported. No adequate information about socioeconomic variables is presented other than school-level poverty level. Due to these shortcomings, the study is added to the prior. 
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -996,7 +1026,7 @@
     <author>Martin,Vasilev</author>
   </authors>
   <commentList>
-    <comment ref="D175" authorId="0">
+    <comment ref="D175" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1030,7 +1060,7 @@
     <author>Martin R. Vasilev</author>
   </authors>
   <commentList>
-    <comment ref="B73" authorId="0">
+    <comment ref="B73" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1060,7 +1090,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5221" uniqueCount="1406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5224" uniqueCount="1408">
   <si>
     <t>ID</t>
   </si>
@@ -39151,11 +39181,17 @@
   <si>
     <t>Analysis of existing data on school tests and noise abatement</t>
   </si>
+  <si>
+    <t>correlations between (unoccupied) classroom noise and reading scores</t>
+  </si>
+  <si>
+    <t>N/A (added to prior)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="67" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -40643,7 +40679,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -65410,8 +65446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="B125" sqref="B125"/>
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="B126" sqref="B126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -68154,7 +68190,7 @@
       </c>
     </row>
     <row r="125" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="45">
+      <c r="A125" s="56">
         <v>123</v>
       </c>
       <c r="B125" s="133" t="s">
@@ -68163,12 +68199,18 @@
       <c r="C125" s="45" t="s">
         <v>282</v>
       </c>
-      <c r="D125" s="45"/>
-      <c r="E125" s="45" t="s">
-        <v>479</v>
-      </c>
-      <c r="F125" s="41"/>
-      <c r="G125" s="45"/>
+      <c r="D125" s="45" t="s">
+        <v>1236</v>
+      </c>
+      <c r="E125" s="56" t="s">
+        <v>1124</v>
+      </c>
+      <c r="F125" s="63" t="s">
+        <v>1406</v>
+      </c>
+      <c r="G125" s="45" t="s">
+        <v>1407</v>
+      </c>
     </row>
     <row r="126" spans="1:7" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="45">
@@ -68296,7 +68338,7 @@
       <c r="F133" s="41"/>
       <c r="G133" s="45"/>
     </row>
-    <row r="134" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A134" s="45"/>
       <c r="B134" s="49" t="s">
         <v>139</v>

</xml_diff>